<commit_message>
fix sync problems (bsp2nlg): use matching inter-TTL-intervals and fix jumps in clock
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$A$1:$Z$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$A$1:$AA$39</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="575">
   <si>
     <t>date</t>
   </si>
@@ -1746,6 +1746,15 @@
   </si>
   <si>
     <t>CalibTunnel</t>
+  </si>
+  <si>
+    <t>sync_jump_ts</t>
+  </si>
+  <si>
+    <t>[3018197071718]</t>
+  </si>
+  <si>
+    <t>[5586708860759]</t>
   </si>
 </sst>
 </file>
@@ -2497,13 +2506,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z174"/>
+  <dimension ref="A1:AA174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B138" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A163" sqref="A163"/>
+      <selection pane="bottomRight" activeCell="X84" sqref="X84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2530,13 +2539,13 @@
     <col min="20" max="20" width="3" customWidth="1"/>
     <col min="21" max="21" width="5.125" customWidth="1"/>
     <col min="22" max="22" width="8.125" customWidth="1"/>
-    <col min="23" max="23" width="5.375" customWidth="1"/>
-    <col min="24" max="24" width="59" customWidth="1"/>
-    <col min="25" max="25" width="107.625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="78.625" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="5.375" customWidth="1"/>
+    <col min="25" max="25" width="59" customWidth="1"/>
+    <col min="26" max="26" width="107.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="78.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -2607,16 +2616,19 @@
         <v>571</v>
       </c>
       <c r="X1" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>503</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>48</v>
       </c>
@@ -2656,8 +2668,11 @@
       <c r="U2">
         <v>3089</v>
       </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
@@ -2694,8 +2709,11 @@
       <c r="R3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>50</v>
       </c>
@@ -2732,8 +2750,11 @@
       <c r="R4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>51</v>
       </c>
@@ -2770,8 +2791,11 @@
       <c r="R5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -2808,8 +2832,11 @@
       <c r="R6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>53</v>
       </c>
@@ -2846,8 +2873,11 @@
       <c r="R7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>54</v>
       </c>
@@ -2884,8 +2914,11 @@
       <c r="R8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>55</v>
       </c>
@@ -2922,8 +2955,11 @@
       <c r="R9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>56</v>
       </c>
@@ -2960,8 +2996,11 @@
       <c r="R10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -2998,8 +3037,11 @@
       <c r="R11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -3036,8 +3078,11 @@
       <c r="R12" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>40</v>
       </c>
@@ -3074,8 +3119,11 @@
       <c r="R13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -3112,8 +3160,11 @@
       <c r="R14" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>42</v>
       </c>
@@ -3150,8 +3201,11 @@
       <c r="R15" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>43</v>
       </c>
@@ -3188,8 +3242,11 @@
       <c r="R16" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X16" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>44</v>
       </c>
@@ -3226,8 +3283,11 @@
       <c r="R17" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X17" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -3264,8 +3324,11 @@
       <c r="R18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>46</v>
       </c>
@@ -3302,8 +3365,11 @@
       <c r="R19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X19" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>47</v>
       </c>
@@ -3340,8 +3406,11 @@
       <c r="R20" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
@@ -3387,8 +3456,11 @@
       <c r="U21">
         <v>3089</v>
       </c>
-    </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -3434,8 +3506,11 @@
       <c r="U22">
         <v>3089</v>
       </c>
-    </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -3481,8 +3556,11 @@
       <c r="U23">
         <v>3089</v>
       </c>
-    </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>15</v>
       </c>
@@ -3528,8 +3606,11 @@
       <c r="U24">
         <v>3089</v>
       </c>
-    </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X24" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>16</v>
       </c>
@@ -3575,8 +3656,11 @@
       <c r="U25">
         <v>3089</v>
       </c>
-    </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X25" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>17</v>
       </c>
@@ -3622,8 +3706,11 @@
       <c r="U26">
         <v>3089</v>
       </c>
-    </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X26" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -3669,8 +3756,11 @@
       <c r="U27">
         <v>3089</v>
       </c>
-    </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -3716,8 +3806,11 @@
       <c r="U28">
         <v>3089</v>
       </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X28" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -3778,8 +3871,11 @@
       <c r="U29">
         <v>3089</v>
       </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X29" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -3825,8 +3921,11 @@
       <c r="U30">
         <v>3089</v>
       </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="X30" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -3873,10 +3972,13 @@
         <v>3089</v>
       </c>
       <c r="X31" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y31" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -3922,8 +4024,11 @@
       <c r="U32">
         <v>3089</v>
       </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
@@ -3969,8 +4074,11 @@
       <c r="U33">
         <v>3089</v>
       </c>
-    </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>25</v>
       </c>
@@ -4031,8 +4139,11 @@
       <c r="U34">
         <v>3089</v>
       </c>
-    </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>26</v>
       </c>
@@ -4078,11 +4189,14 @@
       <c r="U35">
         <v>3089</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="X35" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA35" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>27</v>
       </c>
@@ -4128,8 +4242,11 @@
       <c r="U36">
         <v>3089</v>
       </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X36" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>28</v>
       </c>
@@ -4175,8 +4292,11 @@
       <c r="U37">
         <v>3089</v>
       </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>29</v>
       </c>
@@ -4222,8 +4342,11 @@
       <c r="U38">
         <v>3089</v>
       </c>
-    </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X38" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>30</v>
       </c>
@@ -4269,8 +4392,11 @@
       <c r="U39">
         <v>3089</v>
       </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X39" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>31</v>
       </c>
@@ -4331,8 +4457,11 @@
       <c r="U40">
         <v>3089</v>
       </c>
-    </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>32</v>
       </c>
@@ -4378,8 +4507,11 @@
       <c r="U41">
         <v>3089</v>
       </c>
-    </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>6</v>
       </c>
@@ -4440,8 +4572,11 @@
       <c r="U42">
         <v>3089</v>
       </c>
-    </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X42" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>33</v>
       </c>
@@ -4502,8 +4637,11 @@
       <c r="U43">
         <v>3089</v>
       </c>
-    </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>34</v>
       </c>
@@ -4549,8 +4687,11 @@
       <c r="U44">
         <v>3089</v>
       </c>
-    </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>35</v>
       </c>
@@ -4596,8 +4737,11 @@
       <c r="U45">
         <v>3089</v>
       </c>
-    </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X45" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>36</v>
       </c>
@@ -4643,8 +4787,11 @@
       <c r="U46">
         <v>3089</v>
       </c>
-    </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>37</v>
       </c>
@@ -4690,8 +4837,11 @@
       <c r="U47">
         <v>3089</v>
       </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="X47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>57</v>
       </c>
@@ -4753,16 +4903,19 @@
         <v>3089</v>
       </c>
       <c r="X48" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y48" t="s">
         <v>61</v>
       </c>
-      <c r="Y48" t="s">
+      <c r="Z48" t="s">
         <v>60</v>
       </c>
-      <c r="Z48" t="s">
+      <c r="AA48" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="49" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>62</v>
       </c>
@@ -4824,13 +4977,16 @@
         <v>3089</v>
       </c>
       <c r="X49" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y49" t="s">
         <v>64</v>
       </c>
-      <c r="Y49" t="s">
+      <c r="Z49" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>65</v>
       </c>
@@ -4892,13 +5048,16 @@
         <v>3089</v>
       </c>
       <c r="X50" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y50" t="s">
         <v>69</v>
       </c>
-      <c r="Y50" t="s">
+      <c r="Z50" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>70</v>
       </c>
@@ -4960,13 +5119,16 @@
         <v>3089</v>
       </c>
       <c r="X51" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y51" t="s">
         <v>72</v>
       </c>
-      <c r="Y51" t="s">
+      <c r="Z51" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>73</v>
       </c>
@@ -5028,13 +5190,16 @@
         <v>3089</v>
       </c>
       <c r="X52" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y52" t="s">
         <v>75</v>
       </c>
-      <c r="Y52" t="s">
+      <c r="Z52" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>76</v>
       </c>
@@ -5096,13 +5261,16 @@
         <v>3089</v>
       </c>
       <c r="X53" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y53" t="s">
         <v>77</v>
       </c>
-      <c r="Y53" t="s">
+      <c r="Z53" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>79</v>
       </c>
@@ -5164,13 +5332,16 @@
         <v>2365</v>
       </c>
       <c r="X54" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y54" t="s">
         <v>81</v>
       </c>
-      <c r="Y54" t="s">
+      <c r="Z54" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>82</v>
       </c>
@@ -5232,13 +5403,16 @@
         <v>2365</v>
       </c>
       <c r="X55" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y55" t="s">
         <v>83</v>
       </c>
-      <c r="Y55" t="s">
+      <c r="Z55" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="56" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>88</v>
       </c>
@@ -5300,13 +5474,16 @@
         <v>2365</v>
       </c>
       <c r="X56" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y56" t="s">
         <v>83</v>
       </c>
-      <c r="Y56" t="s">
+      <c r="Z56" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>91</v>
       </c>
@@ -5368,13 +5545,16 @@
         <v>2365</v>
       </c>
       <c r="X57" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y57" t="s">
         <v>83</v>
       </c>
-      <c r="Y57" t="s">
+      <c r="Z57" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="58" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>93</v>
       </c>
@@ -5436,13 +5616,16 @@
         <v>2365</v>
       </c>
       <c r="X58" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y58" t="s">
         <v>94</v>
       </c>
-      <c r="Y58" t="s">
+      <c r="Z58" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="59" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>96</v>
       </c>
@@ -5504,13 +5687,16 @@
         <v>2365</v>
       </c>
       <c r="X59" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y59" t="s">
         <v>94</v>
       </c>
-      <c r="Y59" t="s">
+      <c r="Z59" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>98</v>
       </c>
@@ -5572,13 +5758,16 @@
         <v>2365</v>
       </c>
       <c r="X60" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y60" t="s">
         <v>99</v>
       </c>
-      <c r="Y60" t="s">
+      <c r="Z60" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>101</v>
       </c>
@@ -5640,13 +5829,16 @@
         <v>2365</v>
       </c>
       <c r="X61" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y61" t="s">
         <v>102</v>
       </c>
-      <c r="Y61" t="s">
+      <c r="Z61" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>106</v>
       </c>
@@ -5708,13 +5900,16 @@
         <v>2365</v>
       </c>
       <c r="X62" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y62" t="s">
         <v>94</v>
       </c>
-      <c r="Y62" t="s">
+      <c r="Z62" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="63" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>108</v>
       </c>
@@ -5776,13 +5971,16 @@
         <v>2365</v>
       </c>
       <c r="X63" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y63" t="s">
         <v>109</v>
       </c>
-      <c r="Y63" t="s">
+      <c r="Z63" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="64" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>111</v>
       </c>
@@ -5844,13 +6042,16 @@
         <v>2365</v>
       </c>
       <c r="X64" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y64" t="s">
         <v>112</v>
       </c>
-      <c r="Y64" t="s">
+      <c r="Z64" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>114</v>
       </c>
@@ -5912,13 +6113,16 @@
         <v>2365</v>
       </c>
       <c r="X65" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y65" t="s">
         <v>115</v>
       </c>
-      <c r="Y65" t="s">
+      <c r="Z65" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>116</v>
       </c>
@@ -5980,13 +6184,16 @@
         <v>2365</v>
       </c>
       <c r="X66" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y66" t="s">
         <v>117</v>
       </c>
-      <c r="Y66" t="s">
+      <c r="Z66" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>119</v>
       </c>
@@ -6048,13 +6255,16 @@
         <v>2365</v>
       </c>
       <c r="X67" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y67" t="s">
         <v>120</v>
       </c>
-      <c r="Y67" t="s">
+      <c r="Z67" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>122</v>
       </c>
@@ -6116,13 +6326,16 @@
         <v>2365</v>
       </c>
       <c r="X68" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y68" t="s">
         <v>123</v>
       </c>
-      <c r="Y68" t="s">
+      <c r="Z68" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>124</v>
       </c>
@@ -6172,13 +6385,16 @@
         <v>14</v>
       </c>
       <c r="X69" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y69" t="s">
         <v>125</v>
       </c>
-      <c r="Y69" t="s">
+      <c r="Z69" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>126</v>
       </c>
@@ -6240,13 +6456,16 @@
         <v>2365</v>
       </c>
       <c r="X70" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y70" t="s">
         <v>127</v>
       </c>
-      <c r="Y70" t="s">
+      <c r="Z70" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>130</v>
       </c>
@@ -6308,13 +6527,16 @@
         <v>2365</v>
       </c>
       <c r="X71" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y71" t="s">
         <v>131</v>
       </c>
-      <c r="Y71" t="s">
+      <c r="Z71" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>133</v>
       </c>
@@ -6376,16 +6598,19 @@
         <v>2365</v>
       </c>
       <c r="X72" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y72" t="s">
         <v>134</v>
       </c>
-      <c r="Y72" t="s">
+      <c r="Z72" t="s">
         <v>135</v>
       </c>
-      <c r="Z72" t="s">
+      <c r="AA72" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>136</v>
       </c>
@@ -6447,16 +6672,19 @@
         <v>2365</v>
       </c>
       <c r="X73" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y73" t="s">
         <v>137</v>
       </c>
-      <c r="Y73" t="s">
+      <c r="Z73" t="s">
         <v>138</v>
       </c>
-      <c r="Z73" t="s">
+      <c r="AA73" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>139</v>
       </c>
@@ -6518,13 +6746,16 @@
         <v>2365</v>
       </c>
       <c r="X74" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y74" t="s">
         <v>140</v>
       </c>
-      <c r="Y74" t="s">
+      <c r="Z74" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="75" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>142</v>
       </c>
@@ -6586,16 +6817,19 @@
         <v>2365</v>
       </c>
       <c r="X75" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y75" t="s">
         <v>143</v>
       </c>
-      <c r="Y75" t="s">
+      <c r="Z75" t="s">
         <v>144</v>
       </c>
-      <c r="Z75" t="s">
+      <c r="AA75" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="76" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>145</v>
       </c>
@@ -6657,13 +6891,16 @@
         <v>2365</v>
       </c>
       <c r="X76" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y76" t="s">
         <v>146</v>
       </c>
-      <c r="Y76" t="s">
+      <c r="Z76" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="77" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>148</v>
       </c>
@@ -6725,13 +6962,16 @@
         <v>2365</v>
       </c>
       <c r="X77" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y77" t="s">
         <v>150</v>
       </c>
-      <c r="Y77" t="s">
+      <c r="Z77" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>151</v>
       </c>
@@ -6793,13 +7033,16 @@
         <v>2365</v>
       </c>
       <c r="X78" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y78" t="s">
         <v>152</v>
       </c>
-      <c r="Y78" t="s">
+      <c r="Z78" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="79" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>154</v>
       </c>
@@ -6861,13 +7104,16 @@
         <v>2365</v>
       </c>
       <c r="X79" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y79" t="s">
         <v>155</v>
       </c>
-      <c r="Y79" t="s">
+      <c r="Z79" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>157</v>
       </c>
@@ -6929,13 +7175,16 @@
         <v>2365</v>
       </c>
       <c r="X80" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y80" t="s">
         <v>158</v>
       </c>
-      <c r="Y80" t="s">
+      <c r="Z80" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>160</v>
       </c>
@@ -6997,16 +7246,19 @@
         <v>2365</v>
       </c>
       <c r="X81" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y81" t="s">
         <v>164</v>
       </c>
-      <c r="Y81" t="s">
+      <c r="Z81" t="s">
         <v>159</v>
       </c>
-      <c r="Z81" t="s">
+      <c r="AA81" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>163</v>
       </c>
@@ -7068,13 +7320,16 @@
         <v>2365</v>
       </c>
       <c r="X82" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y82" t="s">
         <v>167</v>
       </c>
-      <c r="Y82" t="s">
+      <c r="Z82" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>165</v>
       </c>
@@ -7136,16 +7391,19 @@
         <v>2365</v>
       </c>
       <c r="X83" t="s">
+        <v>574</v>
+      </c>
+      <c r="Y83" t="s">
         <v>166</v>
       </c>
-      <c r="Y83" t="s">
+      <c r="Z83" t="s">
         <v>169</v>
       </c>
-      <c r="Z83" t="s">
+      <c r="AA83" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>171</v>
       </c>
@@ -7207,13 +7465,16 @@
         <v>2358</v>
       </c>
       <c r="X84" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y84" t="s">
         <v>173</v>
       </c>
-      <c r="Y84" t="s">
+      <c r="Z84" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="85" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>177</v>
       </c>
@@ -7275,16 +7536,19 @@
         <v>2358</v>
       </c>
       <c r="X85" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y85" t="s">
         <v>176</v>
       </c>
-      <c r="Y85" t="s">
+      <c r="Z85" t="s">
         <v>180</v>
       </c>
-      <c r="Z85" t="s">
+      <c r="AA85" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="86" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>178</v>
       </c>
@@ -7346,16 +7610,19 @@
         <v>2358</v>
       </c>
       <c r="X86" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y86" t="s">
         <v>179</v>
       </c>
-      <c r="Y86" t="s">
+      <c r="Z86" t="s">
         <v>180</v>
       </c>
-      <c r="Z86" t="s">
+      <c r="AA86" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>181</v>
       </c>
@@ -7417,16 +7684,19 @@
         <v>2365</v>
       </c>
       <c r="X87" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y87" t="s">
         <v>179</v>
       </c>
-      <c r="Y87" t="s">
+      <c r="Z87" t="s">
         <v>180</v>
       </c>
-      <c r="Z87" t="s">
+      <c r="AA87" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="88" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>183</v>
       </c>
@@ -7488,16 +7758,19 @@
         <v>2365</v>
       </c>
       <c r="X88" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y88" t="s">
         <v>184</v>
       </c>
-      <c r="Y88" t="s">
+      <c r="Z88" t="s">
         <v>180</v>
       </c>
-      <c r="Z88" t="s">
+      <c r="AA88" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>186</v>
       </c>
@@ -7559,16 +7832,19 @@
         <v>2365</v>
       </c>
       <c r="X89" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y89" t="s">
         <v>184</v>
       </c>
-      <c r="Y89" t="s">
+      <c r="Z89" t="s">
         <v>180</v>
       </c>
-      <c r="Z89" t="s">
+      <c r="AA89" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>194</v>
       </c>
@@ -7630,16 +7906,19 @@
         <v>2365</v>
       </c>
       <c r="X90" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y90" t="s">
         <v>184</v>
       </c>
-      <c r="Y90" t="s">
+      <c r="Z90" t="s">
         <v>189</v>
       </c>
-      <c r="Z90" t="s">
+      <c r="AA90" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>195</v>
       </c>
@@ -7701,16 +7980,19 @@
         <v>2365</v>
       </c>
       <c r="X91" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y91" t="s">
         <v>191</v>
       </c>
-      <c r="Y91" t="s">
+      <c r="Z91" t="s">
         <v>192</v>
       </c>
-      <c r="Z91" t="s">
+      <c r="AA91" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>196</v>
       </c>
@@ -7772,16 +8054,19 @@
         <v>2365</v>
       </c>
       <c r="X92" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y92" t="s">
         <v>191</v>
       </c>
-      <c r="Y92" t="s">
+      <c r="Z92" t="s">
         <v>192</v>
       </c>
-      <c r="Z92" t="s">
+      <c r="AA92" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>197</v>
       </c>
@@ -7843,16 +8128,19 @@
         <v>2365</v>
       </c>
       <c r="X93" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y93" t="s">
         <v>203</v>
       </c>
-      <c r="Y93" t="s">
+      <c r="Z93" t="s">
         <v>192</v>
       </c>
-      <c r="Z93" t="s">
+      <c r="AA93" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="94" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>201</v>
       </c>
@@ -7914,16 +8202,19 @@
         <v>2365</v>
       </c>
       <c r="X94" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y94" t="s">
         <v>204</v>
       </c>
-      <c r="Y94" t="s">
+      <c r="Z94" t="s">
         <v>192</v>
       </c>
-      <c r="Z94" t="s">
+      <c r="AA94" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="95" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>200</v>
       </c>
@@ -7985,16 +8276,19 @@
         <v>745</v>
       </c>
       <c r="X95" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y95" t="s">
         <v>203</v>
       </c>
-      <c r="Y95" t="s">
+      <c r="Z95" t="s">
         <v>192</v>
       </c>
-      <c r="Z95" t="s">
+      <c r="AA95" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="96" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>202</v>
       </c>
@@ -8056,16 +8350,19 @@
         <v>745</v>
       </c>
       <c r="X96" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y96" t="s">
         <v>203</v>
       </c>
-      <c r="Y96" t="s">
+      <c r="Z96" t="s">
         <v>205</v>
       </c>
-      <c r="Z96" t="s">
+      <c r="AA96" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="97" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>206</v>
       </c>
@@ -8127,16 +8424,19 @@
         <v>745</v>
       </c>
       <c r="X97" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y97" t="s">
         <v>207</v>
       </c>
-      <c r="Y97" t="s">
+      <c r="Z97" t="s">
         <v>208</v>
       </c>
-      <c r="Z97" t="s">
+      <c r="AA97" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="98" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>209</v>
       </c>
@@ -8198,16 +8498,19 @@
         <v>745</v>
       </c>
       <c r="X98" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y98" t="s">
         <v>210</v>
       </c>
-      <c r="Y98" t="s">
+      <c r="Z98" t="s">
         <v>211</v>
       </c>
-      <c r="Z98" t="s">
+      <c r="AA98" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="99" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>213</v>
       </c>
@@ -8269,13 +8572,16 @@
         <v>745</v>
       </c>
       <c r="X99" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y99" t="s">
         <v>214</v>
       </c>
-      <c r="Y99" t="s">
+      <c r="Z99" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="100" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>216</v>
       </c>
@@ -8337,16 +8643,19 @@
         <v>745</v>
       </c>
       <c r="X100" t="s">
+        <v>573</v>
+      </c>
+      <c r="Y100" t="s">
         <v>214</v>
       </c>
-      <c r="Y100" t="s">
+      <c r="Z100" t="s">
         <v>215</v>
       </c>
-      <c r="Z100" t="s">
+      <c r="AA100" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="101" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>218</v>
       </c>
@@ -8408,13 +8717,16 @@
         <v>745</v>
       </c>
       <c r="X101" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y101" t="s">
         <v>219</v>
       </c>
-      <c r="Y101" t="s">
+      <c r="Z101" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="102" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>220</v>
       </c>
@@ -8476,13 +8788,16 @@
         <v>745</v>
       </c>
       <c r="X102" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y102" t="s">
         <v>219</v>
       </c>
-      <c r="Y102" t="s">
+      <c r="Z102" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="103" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>222</v>
       </c>
@@ -8544,13 +8859,16 @@
         <v>745</v>
       </c>
       <c r="X103" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y103" t="s">
         <v>223</v>
       </c>
-      <c r="Y103" t="s">
+      <c r="Z103" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="104" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>225</v>
       </c>
@@ -8612,13 +8930,16 @@
         <v>745</v>
       </c>
       <c r="X104" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y104" t="s">
         <v>226</v>
       </c>
-      <c r="Y104" t="s">
+      <c r="Z104" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="105" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>228</v>
       </c>
@@ -8680,13 +9001,16 @@
         <v>745</v>
       </c>
       <c r="X105" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y105" t="s">
         <v>232</v>
       </c>
-      <c r="Y105" t="s">
+      <c r="Z105" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="106" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>230</v>
       </c>
@@ -8748,13 +9072,16 @@
         <v>745</v>
       </c>
       <c r="X106" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y106" t="s">
         <v>234</v>
       </c>
-      <c r="Y106" t="s">
+      <c r="Z106" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="107" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>235</v>
       </c>
@@ -8816,13 +9143,16 @@
         <v>2365</v>
       </c>
       <c r="X107" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y107" t="s">
         <v>231</v>
       </c>
-      <c r="Y107" t="s">
+      <c r="Z107" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="108" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>237</v>
       </c>
@@ -8884,13 +9214,16 @@
         <v>708</v>
       </c>
       <c r="X108" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y108" t="s">
         <v>239</v>
       </c>
-      <c r="Y108" t="s">
+      <c r="Z108" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="109" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>241</v>
       </c>
@@ -8952,16 +9285,19 @@
         <v>708</v>
       </c>
       <c r="X109" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y109" t="s">
         <v>243</v>
       </c>
-      <c r="Y109" t="s">
+      <c r="Z109" t="s">
         <v>240</v>
       </c>
-      <c r="Z109" t="s">
+      <c r="AA109" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="110" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>245</v>
       </c>
@@ -9023,16 +9359,19 @@
         <v>708</v>
       </c>
       <c r="X110" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y110" t="s">
         <v>246</v>
       </c>
-      <c r="Y110" t="s">
+      <c r="Z110" t="s">
         <v>247</v>
       </c>
-      <c r="Z110" t="s">
+      <c r="AA110" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="111" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>250</v>
       </c>
@@ -9094,13 +9433,16 @@
         <v>708</v>
       </c>
       <c r="X111" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y111" t="s">
         <v>252</v>
       </c>
-      <c r="Y111" t="s">
+      <c r="Z111" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="112" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>254</v>
       </c>
@@ -9162,10 +9504,13 @@
         <v>708</v>
       </c>
       <c r="X112" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y112" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="113" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>251</v>
       </c>
@@ -9227,13 +9572,16 @@
         <v>708</v>
       </c>
       <c r="X113" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y113" t="s">
         <v>252</v>
       </c>
-      <c r="Y113" t="s">
+      <c r="Z113" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="114" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>255</v>
       </c>
@@ -9295,13 +9643,16 @@
         <v>708</v>
       </c>
       <c r="X114" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y114" t="s">
         <v>257</v>
       </c>
-      <c r="Y114" t="s">
+      <c r="Z114" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="115" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>258</v>
       </c>
@@ -9363,13 +9714,16 @@
         <v>708</v>
       </c>
       <c r="X115" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y115" t="s">
         <v>259</v>
       </c>
-      <c r="Y115" t="s">
+      <c r="Z115" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="116" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>261</v>
       </c>
@@ -9431,13 +9785,16 @@
         <v>2358</v>
       </c>
       <c r="X116" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y116" t="s">
         <v>262</v>
       </c>
-      <c r="Y116" t="s">
+      <c r="Z116" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="117" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>264</v>
       </c>
@@ -9499,13 +9856,16 @@
         <v>708</v>
       </c>
       <c r="X117" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y117" t="s">
         <v>265</v>
       </c>
-      <c r="Y117" t="s">
+      <c r="Z117" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="118" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>266</v>
       </c>
@@ -9567,13 +9927,16 @@
         <v>2358</v>
       </c>
       <c r="X118" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y118" t="s">
         <v>262</v>
       </c>
-      <c r="Y118" t="s">
+      <c r="Z118" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="119" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>267</v>
       </c>
@@ -9635,13 +9998,16 @@
         <v>708</v>
       </c>
       <c r="X119" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y119" t="s">
         <v>265</v>
       </c>
-      <c r="Y119" t="s">
+      <c r="Z119" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="120" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>269</v>
       </c>
@@ -9703,13 +10069,16 @@
         <v>2358</v>
       </c>
       <c r="X120" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y120" t="s">
         <v>270</v>
       </c>
-      <c r="Y120" t="s">
+      <c r="Z120" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="121" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>271</v>
       </c>
@@ -9771,13 +10140,16 @@
         <v>708</v>
       </c>
       <c r="X121" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y121" t="s">
         <v>272</v>
       </c>
-      <c r="Y121" t="s">
+      <c r="Z121" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="122" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>274</v>
       </c>
@@ -9839,13 +10211,16 @@
         <v>2358</v>
       </c>
       <c r="X122" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y122" t="s">
         <v>276</v>
       </c>
-      <c r="Y122" t="s">
+      <c r="Z122" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="123" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>277</v>
       </c>
@@ -9907,13 +10282,16 @@
         <v>2358</v>
       </c>
       <c r="X123" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y123" t="s">
         <v>278</v>
       </c>
-      <c r="Y123" t="s">
+      <c r="Z123" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="124" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>280</v>
       </c>
@@ -9975,10 +10353,13 @@
         <v>2358</v>
       </c>
       <c r="X124" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y124" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="125" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>281</v>
       </c>
@@ -10040,10 +10421,13 @@
         <v>708</v>
       </c>
       <c r="X125" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y125" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="126" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>282</v>
       </c>
@@ -10105,10 +10489,13 @@
         <v>2358</v>
       </c>
       <c r="X126" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y126" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="127" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>283</v>
       </c>
@@ -10170,10 +10557,13 @@
         <v>2358</v>
       </c>
       <c r="X127" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y127" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="128" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>286</v>
       </c>
@@ -10235,10 +10625,13 @@
         <v>708</v>
       </c>
       <c r="X128" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y128" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="129" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>287</v>
       </c>
@@ -10300,13 +10693,16 @@
         <v>2358</v>
       </c>
       <c r="X129" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y129" t="s">
         <v>291</v>
       </c>
-      <c r="Y129" t="s">
+      <c r="Z129" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="130" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>289</v>
       </c>
@@ -10368,13 +10764,16 @@
         <v>708</v>
       </c>
       <c r="X130" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y130" t="s">
         <v>290</v>
       </c>
-      <c r="Y130" t="s">
+      <c r="Z130" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="131" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>293</v>
       </c>
@@ -10436,13 +10835,16 @@
         <v>708</v>
       </c>
       <c r="X131" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y131" t="s">
         <v>294</v>
       </c>
-      <c r="Y131" t="s">
+      <c r="Z131" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="132" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>296</v>
       </c>
@@ -10504,13 +10906,16 @@
         <v>2358</v>
       </c>
       <c r="X132" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y132" t="s">
         <v>290</v>
       </c>
-      <c r="Y132" t="s">
+      <c r="Z132" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="133" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>297</v>
       </c>
@@ -10572,16 +10977,19 @@
         <v>708</v>
       </c>
       <c r="X133" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y133" t="s">
         <v>294</v>
       </c>
-      <c r="Y133" t="s">
+      <c r="Z133" t="s">
         <v>298</v>
       </c>
-      <c r="Z133" t="s">
+      <c r="AA133" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="134" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>299</v>
       </c>
@@ -10643,16 +11051,19 @@
         <v>2358</v>
       </c>
       <c r="X134" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y134" t="s">
         <v>300</v>
       </c>
-      <c r="Y134" t="s">
+      <c r="Z134" t="s">
         <v>298</v>
       </c>
-      <c r="Z134" t="s">
+      <c r="AA134" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="135" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>302</v>
       </c>
@@ -10714,16 +11125,19 @@
         <v>2358</v>
       </c>
       <c r="X135" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y135" t="s">
         <v>303</v>
       </c>
-      <c r="Y135" t="s">
+      <c r="Z135" t="s">
         <v>304</v>
       </c>
-      <c r="Z135" t="s">
+      <c r="AA135" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="136" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>305</v>
       </c>
@@ -10785,16 +11199,19 @@
         <v>2358</v>
       </c>
       <c r="X136" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y136" t="s">
         <v>306</v>
       </c>
-      <c r="Y136" t="s">
+      <c r="Z136" t="s">
         <v>307</v>
       </c>
-      <c r="Z136" t="s">
+      <c r="AA136" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="137" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>310</v>
       </c>
@@ -10856,16 +11273,19 @@
         <v>2358</v>
       </c>
       <c r="X137" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y137" t="s">
         <v>311</v>
       </c>
-      <c r="Y137" t="s">
+      <c r="Z137" t="s">
         <v>312</v>
       </c>
-      <c r="Z137" t="s">
+      <c r="AA137" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="138" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>314</v>
       </c>
@@ -10927,16 +11347,19 @@
         <v>708</v>
       </c>
       <c r="X138" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y138" t="s">
         <v>285</v>
       </c>
-      <c r="Y138" t="s">
+      <c r="Z138" t="s">
         <v>315</v>
       </c>
-      <c r="Z138" t="s">
+      <c r="AA138" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="139" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>316</v>
       </c>
@@ -10998,13 +11421,16 @@
         <v>2358</v>
       </c>
       <c r="X139" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y139" t="s">
         <v>317</v>
       </c>
-      <c r="Y139" t="s">
+      <c r="Z139" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="140" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>318</v>
       </c>
@@ -11066,13 +11492,16 @@
         <v>2358</v>
       </c>
       <c r="X140" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y140" t="s">
         <v>322</v>
       </c>
-      <c r="Y140" t="s">
+      <c r="Z140" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="141" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>321</v>
       </c>
@@ -11134,13 +11563,16 @@
         <v>2358</v>
       </c>
       <c r="X141" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y141" t="s">
         <v>326</v>
       </c>
-      <c r="Y141" t="s">
+      <c r="Z141" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="142" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>324</v>
       </c>
@@ -11202,13 +11634,16 @@
         <v>2358</v>
       </c>
       <c r="X142" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y142" t="s">
         <v>325</v>
       </c>
-      <c r="Y142" t="s">
+      <c r="Z142" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="143" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>328</v>
       </c>
@@ -11270,16 +11705,19 @@
         <v>2358</v>
       </c>
       <c r="X143" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y143" t="s">
         <v>325</v>
       </c>
-      <c r="Y143" t="s">
+      <c r="Z143" t="s">
         <v>329</v>
       </c>
-      <c r="Z143" t="s">
+      <c r="AA143" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="144" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>331</v>
       </c>
@@ -11337,11 +11775,14 @@
       <c r="T144">
         <v>9</v>
       </c>
-      <c r="Z144" t="s">
+      <c r="X144" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA144" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="145" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>334</v>
       </c>
@@ -11403,16 +11844,19 @@
         <v>2358</v>
       </c>
       <c r="X145" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y145" t="s">
         <v>325</v>
       </c>
-      <c r="Y145" t="s">
+      <c r="Z145" t="s">
         <v>329</v>
       </c>
-      <c r="Z145" t="s">
+      <c r="AA145" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="146" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>336</v>
       </c>
@@ -11474,16 +11918,19 @@
         <v>2358</v>
       </c>
       <c r="X146" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y146" t="s">
         <v>337</v>
       </c>
-      <c r="Y146" t="s">
+      <c r="Z146" t="s">
         <v>338</v>
       </c>
-      <c r="Z146" t="s">
+      <c r="AA146" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="147" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
         <v>339</v>
       </c>
@@ -11545,10 +11992,13 @@
         <v>708</v>
       </c>
       <c r="X147" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y147" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="148" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>342</v>
       </c>
@@ -11610,13 +12060,16 @@
         <v>2358</v>
       </c>
       <c r="X148" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y148" t="s">
         <v>344</v>
       </c>
-      <c r="Y148" t="s">
+      <c r="Z148" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="149" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>345</v>
       </c>
@@ -11678,13 +12131,16 @@
         <v>2358</v>
       </c>
       <c r="X149" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y149" t="s">
         <v>346</v>
       </c>
-      <c r="Y149" t="s">
+      <c r="Z149" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="150" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>348</v>
       </c>
@@ -11746,16 +12202,19 @@
         <v>2358</v>
       </c>
       <c r="X150" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y150" t="s">
         <v>350</v>
       </c>
-      <c r="Y150" t="s">
+      <c r="Z150" t="s">
         <v>349</v>
       </c>
-      <c r="Z150" t="s">
+      <c r="AA150" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="151" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>352</v>
       </c>
@@ -11817,13 +12276,16 @@
         <v>2358</v>
       </c>
       <c r="X151" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y151" t="s">
         <v>353</v>
       </c>
-      <c r="Y151" t="s">
+      <c r="Z151" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="152" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>354</v>
       </c>
@@ -11885,16 +12347,19 @@
         <v>2358</v>
       </c>
       <c r="X152" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y152" t="s">
         <v>355</v>
       </c>
-      <c r="Y152" t="s">
+      <c r="Z152" t="s">
         <v>356</v>
       </c>
-      <c r="Z152" t="s">
+      <c r="AA152" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="153" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>358</v>
       </c>
@@ -11956,16 +12421,19 @@
         <v>2358</v>
       </c>
       <c r="X153" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y153" t="s">
         <v>353</v>
       </c>
-      <c r="Y153" t="s">
+      <c r="Z153" t="s">
         <v>343</v>
       </c>
-      <c r="Z153" t="s">
+      <c r="AA153" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="154" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>360</v>
       </c>
@@ -12027,13 +12495,16 @@
         <v>2358</v>
       </c>
       <c r="X154" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y154" t="s">
         <v>361</v>
       </c>
-      <c r="Y154" t="s">
+      <c r="Z154" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="155" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>362</v>
       </c>
@@ -12095,13 +12566,16 @@
         <v>2358</v>
       </c>
       <c r="X155" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y155" t="s">
         <v>350</v>
       </c>
-      <c r="Y155" t="s">
+      <c r="Z155" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="156" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>363</v>
       </c>
@@ -12163,13 +12637,16 @@
         <v>2358</v>
       </c>
       <c r="X156" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y156" t="s">
         <v>374</v>
       </c>
-      <c r="Y156" t="s">
+      <c r="Z156" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="157" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>364</v>
       </c>
@@ -12231,13 +12708,16 @@
         <v>2358</v>
       </c>
       <c r="X157" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y157" t="s">
         <v>353</v>
       </c>
-      <c r="Y157" t="s">
+      <c r="Z157" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="158" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>365</v>
       </c>
@@ -12299,13 +12779,16 @@
         <v>2358</v>
       </c>
       <c r="X158" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y158" t="s">
         <v>366</v>
       </c>
-      <c r="Y158" t="s">
+      <c r="Z158" t="s">
         <v>347</v>
       </c>
     </row>
-    <row r="159" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>367</v>
       </c>
@@ -12367,13 +12850,16 @@
         <v>2358</v>
       </c>
       <c r="X159" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y159" t="s">
         <v>374</v>
       </c>
-      <c r="Y159" t="s">
+      <c r="Z159" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="160" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>369</v>
       </c>
@@ -12435,13 +12921,16 @@
         <v>2358</v>
       </c>
       <c r="X160" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y160" t="s">
         <v>366</v>
       </c>
-      <c r="Y160" t="s">
+      <c r="Z160" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="161" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>371</v>
       </c>
@@ -12503,13 +12992,16 @@
         <v>2358</v>
       </c>
       <c r="X161" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y161" t="s">
         <v>366</v>
       </c>
-      <c r="Y161" t="s">
+      <c r="Z161" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="162" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>373</v>
       </c>
@@ -12571,13 +13063,16 @@
         <v>2358</v>
       </c>
       <c r="X162" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y162" t="s">
         <v>374</v>
       </c>
-      <c r="Y162" t="s">
+      <c r="Z162" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="163" spans="1:26" ht="15" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:27" ht="15" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>376</v>
       </c>
@@ -12639,16 +13134,19 @@
         <v>2358</v>
       </c>
       <c r="X163" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y163" t="s">
         <v>374</v>
       </c>
-      <c r="Y163" t="s">
+      <c r="Z163" t="s">
         <v>380</v>
       </c>
-      <c r="Z163" t="s">
+      <c r="AA163" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="164" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>378</v>
       </c>
@@ -12710,13 +13208,16 @@
         <v>2358</v>
       </c>
       <c r="X164" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y164" t="s">
         <v>366</v>
       </c>
-      <c r="Y164" t="s">
+      <c r="Z164" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="165" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>379</v>
       </c>
@@ -12778,13 +13279,16 @@
         <v>2358</v>
       </c>
       <c r="X165" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y165" t="s">
         <v>366</v>
       </c>
-      <c r="Y165" t="s">
+      <c r="Z165" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="166" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>381</v>
       </c>
@@ -12846,13 +13350,16 @@
         <v>2358</v>
       </c>
       <c r="X166" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y166" t="s">
         <v>382</v>
       </c>
-      <c r="Y166" t="s">
+      <c r="Z166" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="167" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>383</v>
       </c>
@@ -12914,16 +13421,19 @@
         <v>2358</v>
       </c>
       <c r="X167" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y167" t="s">
         <v>353</v>
       </c>
-      <c r="Y167" t="s">
+      <c r="Z167" t="s">
         <v>385</v>
       </c>
-      <c r="Z167" t="s">
+      <c r="AA167" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="168" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>386</v>
       </c>
@@ -12985,13 +13495,16 @@
         <v>2358</v>
       </c>
       <c r="X168" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y168" t="s">
         <v>387</v>
       </c>
-      <c r="Y168" t="s">
+      <c r="Z168" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="169" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>388</v>
       </c>
@@ -13053,13 +13566,16 @@
         <v>2358</v>
       </c>
       <c r="X169" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y169" t="s">
         <v>387</v>
       </c>
-      <c r="Y169" t="s">
+      <c r="Z169" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="170" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>389</v>
       </c>
@@ -13121,16 +13637,19 @@
         <v>2358</v>
       </c>
       <c r="X170" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y170" t="s">
         <v>390</v>
       </c>
-      <c r="Y170" t="s">
+      <c r="Z170" t="s">
         <v>385</v>
       </c>
-      <c r="Z170" t="s">
+      <c r="AA170" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="171" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>392</v>
       </c>
@@ -13192,13 +13711,16 @@
         <v>2358</v>
       </c>
       <c r="X171" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y171" t="s">
         <v>390</v>
       </c>
-      <c r="Y171" t="s">
+      <c r="Z171" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="172" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>393</v>
       </c>
@@ -13260,13 +13782,16 @@
         <v>2358</v>
       </c>
       <c r="X172" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y172" t="s">
         <v>394</v>
       </c>
-      <c r="Y172" t="s">
+      <c r="Z172" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="173" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>395</v>
       </c>
@@ -13328,13 +13853,16 @@
         <v>2358</v>
       </c>
       <c r="X173" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y173" t="s">
         <v>396</v>
       </c>
-      <c r="Y173" t="s">
+      <c r="Z173" t="s">
         <v>385</v>
       </c>
     </row>
-    <row r="174" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>397</v>
       </c>
@@ -13396,17 +13924,20 @@
         <v>2358</v>
       </c>
       <c r="X174" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y174" t="s">
         <v>398</v>
       </c>
-      <c r="Y174" t="s">
+      <c r="Z174" t="s">
         <v>385</v>
       </c>
-      <c r="Z174" t="s">
+      <c r="AA174" t="s">
         <v>399</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Z47">
+  <autoFilter ref="A1:AA47">
     <sortState ref="A2:Y47">
       <sortCondition ref="D1:D39"/>
     </sortState>

</xml_diff>

<commit_message>
update bat 79 brain regions of each TT for all days
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2086" uniqueCount="585">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="589">
   <si>
     <t>date</t>
   </si>
@@ -1785,6 +1785,18 @@
   </si>
   <si>
     <t>[1 1 1 1;1 1 1 1;1 1 1 1; 1 1 1 1]</t>
+  </si>
+  <si>
+    <t>{'WM','WM','WM','N/A'}</t>
+  </si>
+  <si>
+    <t>{'WM','WM','CA1','N/A'}</t>
+  </si>
+  <si>
+    <t>{'WM','CA1','CA1','N/A'}</t>
+  </si>
+  <si>
+    <t>{'CA1','CA1','CA1','N/A'}</t>
   </si>
 </sst>
 </file>
@@ -2539,10 +2551,10 @@
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I45" sqref="I45"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4544,11 +4556,20 @@
       <c r="J31" t="s">
         <v>8</v>
       </c>
+      <c r="K31" t="s">
+        <v>585</v>
+      </c>
       <c r="L31" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>562</v>
+      </c>
+      <c r="N31">
+        <v>1</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
       </c>
       <c r="P31">
         <v>0</v>
@@ -4594,11 +4615,20 @@
       <c r="J32" t="s">
         <v>8</v>
       </c>
+      <c r="K32" t="s">
+        <v>585</v>
+      </c>
       <c r="L32" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M32" s="9" t="s">
         <v>561</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
       </c>
       <c r="P32">
         <v>0</v>
@@ -4644,11 +4674,20 @@
       <c r="J33" t="s">
         <v>8</v>
       </c>
+      <c r="K33" t="s">
+        <v>586</v>
+      </c>
       <c r="L33" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M33" s="9" t="s">
         <v>560</v>
+      </c>
+      <c r="N33">
+        <v>1</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -4694,11 +4733,20 @@
       <c r="J34" t="s">
         <v>8</v>
       </c>
+      <c r="K34" t="s">
+        <v>586</v>
+      </c>
       <c r="L34" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>559</v>
+      </c>
+      <c r="N34">
+        <v>1</v>
+      </c>
+      <c r="O34">
+        <v>1</v>
       </c>
       <c r="P34">
         <v>0</v>
@@ -4744,11 +4792,20 @@
       <c r="J35" t="s">
         <v>8</v>
       </c>
+      <c r="K35" t="s">
+        <v>586</v>
+      </c>
       <c r="L35" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M35" s="9" t="s">
         <v>558</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
       </c>
       <c r="P35">
         <v>0</v>
@@ -4794,11 +4851,20 @@
       <c r="J36" t="s">
         <v>8</v>
       </c>
+      <c r="K36" t="s">
+        <v>586</v>
+      </c>
       <c r="L36" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>557</v>
+      </c>
+      <c r="N36">
+        <v>1</v>
+      </c>
+      <c r="O36">
+        <v>1</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -4844,6 +4910,9 @@
       <c r="J37" t="s">
         <v>8</v>
       </c>
+      <c r="K37" t="s">
+        <v>587</v>
+      </c>
       <c r="L37" s="10" t="s">
         <v>500</v>
       </c>
@@ -4909,11 +4978,20 @@
       <c r="J38" t="s">
         <v>8</v>
       </c>
+      <c r="K38" t="s">
+        <v>587</v>
+      </c>
       <c r="L38" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>556</v>
+      </c>
+      <c r="N38">
+        <v>1</v>
+      </c>
+      <c r="O38">
+        <v>1</v>
       </c>
       <c r="P38">
         <v>0</v>
@@ -4959,11 +5037,20 @@
       <c r="J39" t="s">
         <v>8</v>
       </c>
+      <c r="K39" t="s">
+        <v>587</v>
+      </c>
       <c r="L39" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M39" s="9" t="s">
         <v>554</v>
+      </c>
+      <c r="N39">
+        <v>1</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
       </c>
       <c r="P39">
         <v>0</v>
@@ -5012,11 +5099,20 @@
       <c r="J40" t="s">
         <v>8</v>
       </c>
+      <c r="K40" t="s">
+        <v>587</v>
+      </c>
       <c r="L40" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M40" s="9" t="s">
         <v>553</v>
+      </c>
+      <c r="N40">
+        <v>1</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
       </c>
       <c r="P40">
         <v>0</v>
@@ -5062,11 +5158,20 @@
       <c r="J41" t="s">
         <v>8</v>
       </c>
+      <c r="K41" t="s">
+        <v>587</v>
+      </c>
       <c r="L41" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>552</v>
+      </c>
+      <c r="N41">
+        <v>1</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
       </c>
       <c r="P41">
         <v>0</v>
@@ -5112,6 +5217,9 @@
       <c r="J42" t="s">
         <v>8</v>
       </c>
+      <c r="K42" t="s">
+        <v>587</v>
+      </c>
       <c r="L42" s="10" t="s">
         <v>500</v>
       </c>
@@ -5177,11 +5285,20 @@
       <c r="J43" t="s">
         <v>8</v>
       </c>
+      <c r="K43" t="s">
+        <v>587</v>
+      </c>
       <c r="L43" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>550</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>1</v>
       </c>
       <c r="P43">
         <v>0</v>
@@ -5230,11 +5347,20 @@
       <c r="J44" t="s">
         <v>8</v>
       </c>
+      <c r="K44" t="s">
+        <v>587</v>
+      </c>
       <c r="L44" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>549</v>
+      </c>
+      <c r="N44">
+        <v>1</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
       </c>
       <c r="P44">
         <v>0</v>
@@ -5280,11 +5406,20 @@
       <c r="J45" t="s">
         <v>8</v>
       </c>
+      <c r="K45" t="s">
+        <v>587</v>
+      </c>
       <c r="L45" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M45" s="9" t="s">
         <v>548</v>
+      </c>
+      <c r="N45">
+        <v>1</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
       </c>
       <c r="P45">
         <v>0</v>
@@ -5330,11 +5465,20 @@
       <c r="J46" t="s">
         <v>8</v>
       </c>
+      <c r="K46" t="s">
+        <v>587</v>
+      </c>
       <c r="L46" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>547</v>
+      </c>
+      <c r="N46">
+        <v>1</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
       </c>
       <c r="P46">
         <v>0</v>
@@ -5380,11 +5524,20 @@
       <c r="J47" t="s">
         <v>8</v>
       </c>
+      <c r="K47" t="s">
+        <v>587</v>
+      </c>
       <c r="L47" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M47" s="9" t="s">
         <v>546</v>
+      </c>
+      <c r="N47">
+        <v>1</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
       </c>
       <c r="P47">
         <v>0</v>
@@ -5430,6 +5583,9 @@
       <c r="J48" t="s">
         <v>8</v>
       </c>
+      <c r="K48" t="s">
+        <v>588</v>
+      </c>
       <c r="L48" s="10" t="s">
         <v>500</v>
       </c>
@@ -5495,11 +5651,20 @@
       <c r="J49" t="s">
         <v>8</v>
       </c>
+      <c r="K49" t="s">
+        <v>588</v>
+      </c>
       <c r="L49" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M49" s="9" t="s">
         <v>545</v>
+      </c>
+      <c r="N49">
+        <v>1</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
       </c>
       <c r="P49">
         <v>0</v>
@@ -5545,6 +5710,9 @@
       <c r="J50" t="s">
         <v>8</v>
       </c>
+      <c r="K50" t="s">
+        <v>588</v>
+      </c>
       <c r="L50" s="10" t="s">
         <v>500</v>
       </c>
@@ -5610,6 +5778,9 @@
       <c r="J51" t="s">
         <v>8</v>
       </c>
+      <c r="K51" t="s">
+        <v>588</v>
+      </c>
       <c r="L51" s="10" t="s">
         <v>500</v>
       </c>
@@ -5675,11 +5846,20 @@
       <c r="J52" t="s">
         <v>8</v>
       </c>
+      <c r="K52" t="s">
+        <v>588</v>
+      </c>
       <c r="L52" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M52" s="9" t="s">
         <v>544</v>
+      </c>
+      <c r="N52">
+        <v>1</v>
+      </c>
+      <c r="O52">
+        <v>1</v>
       </c>
       <c r="P52">
         <v>0</v>
@@ -5725,11 +5905,20 @@
       <c r="J53" t="s">
         <v>8</v>
       </c>
+      <c r="K53" t="s">
+        <v>588</v>
+      </c>
       <c r="L53" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M53" s="9" t="s">
         <v>543</v>
+      </c>
+      <c r="N53">
+        <v>1</v>
+      </c>
+      <c r="O53">
+        <v>1</v>
       </c>
       <c r="P53">
         <v>0</v>
@@ -5775,11 +5964,20 @@
       <c r="J54" t="s">
         <v>8</v>
       </c>
+      <c r="K54" t="s">
+        <v>588</v>
+      </c>
       <c r="L54" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M54" s="9" t="s">
         <v>542</v>
+      </c>
+      <c r="N54">
+        <v>1</v>
+      </c>
+      <c r="O54">
+        <v>1</v>
       </c>
       <c r="P54">
         <v>0</v>
@@ -5825,11 +6023,20 @@
       <c r="J55" t="s">
         <v>8</v>
       </c>
+      <c r="K55" t="s">
+        <v>588</v>
+      </c>
       <c r="L55" s="10" t="s">
         <v>500</v>
       </c>
       <c r="M55" s="9" t="s">
         <v>541</v>
+      </c>
+      <c r="N55">
+        <v>1</v>
+      </c>
+      <c r="O55">
+        <v>1</v>
       </c>
       <c r="P55">
         <v>0</v>

</xml_diff>

<commit_message>
update bat 9861 brain regions of each TT for all days
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Experiments" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$A$1:$AC$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Experiments!$A$1:$AC$174</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2111" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="596">
   <si>
     <t>date</t>
   </si>
@@ -1754,30 +1754,15 @@
     <t>TT_loc</t>
   </si>
   <si>
-    <t>{'dCA1','WM','dCA1','dCA1'}</t>
-  </si>
-  <si>
     <t>{'CTX','CTX','CTX','CTX'}</t>
   </si>
   <si>
     <t>probably still in cortex; maybe TT3,4 in CA1</t>
   </si>
   <si>
-    <t>{'dCA1','N/A','N/A','dCA1'}</t>
-  </si>
-  <si>
     <t>{'N/A','N/A','N/A','N/A'}</t>
   </si>
   <si>
-    <t>{'WM','N/A','N/A','dCA1'}</t>
-  </si>
-  <si>
-    <t>{'dCA1','dCA1','dCA1','dCA1'}</t>
-  </si>
-  <si>
-    <t>{'dCA1','WM',WM','dCA1'}</t>
-  </si>
-  <si>
     <t>UseNegThr</t>
   </si>
   <si>
@@ -1797,6 +1782,42 @@
   </si>
   <si>
     <t>{'CA1','CA1','CA1','N/A'}</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','WM2','DG'}</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','DG/CA3','DG'}</t>
+  </si>
+  <si>
+    <t>{'CA1','WM','CA1','CA1'}</t>
+  </si>
+  <si>
+    <t>{'WM','N/A','N/A','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','N/A','N/A','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','WM',WM','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','CA1','CA1','CA1'}</t>
+  </si>
+  <si>
+    <t>{'WM2','WM2','CA1','CA1'}</t>
+  </si>
+  <si>
+    <t>{'WM2','WM2','CA1','WM2'}</t>
+  </si>
+  <si>
+    <t>{'DG','WM2','CA1','WM2'}</t>
+  </si>
+  <si>
+    <t>{'DG','WM2','CA1','DG'}</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','CA1','DG'}</t>
   </si>
 </sst>
 </file>
@@ -2551,10 +2572,10 @@
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
+      <selection pane="bottomRight" activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2606,7 +2627,7 @@
         <v>489</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>395</v>
@@ -2705,7 +2726,7 @@
         <v>8</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>563</v>
@@ -2783,7 +2804,7 @@
         <v>8</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>500</v>
@@ -2861,7 +2882,7 @@
         <v>8</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>500</v>
@@ -2939,7 +2960,7 @@
         <v>8</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>500</v>
@@ -3016,7 +3037,9 @@
       <c r="J6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K6" s="1"/>
+      <c r="K6" s="1" t="s">
+        <v>586</v>
+      </c>
       <c r="L6" s="10" t="s">
         <v>500</v>
       </c>
@@ -3060,7 +3083,7 @@
         <v>199</v>
       </c>
       <c r="AB6" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AC6" t="s">
         <v>189</v>
@@ -3092,6 +3115,9 @@
       <c r="J7" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K7" s="1" t="s">
+        <v>586</v>
+      </c>
       <c r="L7" s="10" t="s">
         <v>500</v>
       </c>
@@ -3135,7 +3161,7 @@
         <v>198</v>
       </c>
       <c r="AB7" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="AC7" t="s">
         <v>189</v>
@@ -3168,7 +3194,7 @@
         <v>8</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>500</v>
@@ -3246,7 +3272,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>500</v>
@@ -3324,7 +3350,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>500</v>
@@ -3402,7 +3428,7 @@
         <v>8</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>500</v>
@@ -3477,7 +3503,7 @@
         <v>8</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>500</v>
@@ -3555,7 +3581,7 @@
         <v>8</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>500</v>
@@ -3630,7 +3656,7 @@
         <v>8</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>574</v>
+        <v>586</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>500</v>
@@ -3705,7 +3731,7 @@
         <v>8</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>500</v>
@@ -3780,7 +3806,7 @@
         <v>8</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>500</v>
@@ -3855,7 +3881,7 @@
         <v>8</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>500</v>
@@ -3930,7 +3956,7 @@
         <v>8</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>500</v>
@@ -4005,7 +4031,7 @@
         <v>8</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>500</v>
@@ -4445,13 +4471,13 @@
         <v>42614</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G29">
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J29" t="s">
         <v>8</v>
@@ -4495,13 +4521,13 @@
         <v>42615</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G30">
         <v>4</v>
       </c>
       <c r="I30" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J30" t="s">
         <v>8</v>
@@ -4545,19 +4571,19 @@
         <v>42617</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G31">
         <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J31" t="s">
         <v>8</v>
       </c>
       <c r="K31" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="L31" s="10" t="s">
         <v>500</v>
@@ -4604,19 +4630,19 @@
         <v>42620</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G32">
         <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J32" t="s">
         <v>8</v>
       </c>
       <c r="K32" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="L32" s="10" t="s">
         <v>500</v>
@@ -4663,19 +4689,19 @@
         <v>42621</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G33">
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J33" t="s">
         <v>8</v>
       </c>
       <c r="K33" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L33" s="10" t="s">
         <v>500</v>
@@ -4722,19 +4748,19 @@
         <v>42622</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G34">
         <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J34" t="s">
         <v>8</v>
       </c>
       <c r="K34" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L34" s="10" t="s">
         <v>500</v>
@@ -4781,19 +4807,19 @@
         <v>42624</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G35">
         <v>4</v>
       </c>
       <c r="I35" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J35" t="s">
         <v>8</v>
       </c>
       <c r="K35" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L35" s="10" t="s">
         <v>500</v>
@@ -4840,19 +4866,19 @@
         <v>42625</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G36">
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J36" t="s">
         <v>8</v>
       </c>
       <c r="K36" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="L36" s="10" t="s">
         <v>500</v>
@@ -4899,19 +4925,19 @@
         <v>42626</v>
       </c>
       <c r="E37" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G37">
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J37" t="s">
         <v>8</v>
       </c>
       <c r="K37" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L37" s="10" t="s">
         <v>500</v>
@@ -4967,19 +4993,19 @@
         <v>42627</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G38">
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J38" t="s">
         <v>8</v>
       </c>
       <c r="K38" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L38" s="10" t="s">
         <v>500</v>
@@ -5026,19 +5052,19 @@
         <v>42628</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G39">
         <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J39" t="s">
         <v>8</v>
       </c>
       <c r="K39" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L39" s="10" t="s">
         <v>500</v>
@@ -5088,19 +5114,19 @@
         <v>42629</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G40">
         <v>4</v>
       </c>
       <c r="I40" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J40" t="s">
         <v>8</v>
       </c>
       <c r="K40" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L40" s="10" t="s">
         <v>500</v>
@@ -5147,19 +5173,19 @@
         <v>42631</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G41">
         <v>4</v>
       </c>
       <c r="I41" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J41" t="s">
         <v>8</v>
       </c>
       <c r="K41" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L41" s="10" t="s">
         <v>500</v>
@@ -5206,19 +5232,19 @@
         <v>42632</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G42">
         <v>4</v>
       </c>
       <c r="I42" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J42" t="s">
         <v>8</v>
       </c>
       <c r="K42" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L42" s="10" t="s">
         <v>500</v>
@@ -5274,19 +5300,19 @@
         <v>42633</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G43">
         <v>4</v>
       </c>
       <c r="I43" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J43" t="s">
         <v>8</v>
       </c>
       <c r="K43" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L43" s="10" t="s">
         <v>500</v>
@@ -5336,19 +5362,19 @@
         <v>42634</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G44">
         <v>4</v>
       </c>
       <c r="I44" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J44" t="s">
         <v>8</v>
       </c>
       <c r="K44" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L44" s="10" t="s">
         <v>500</v>
@@ -5395,19 +5421,19 @@
         <v>42636</v>
       </c>
       <c r="E45" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G45">
         <v>4</v>
       </c>
       <c r="I45" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J45" t="s">
         <v>8</v>
       </c>
       <c r="K45" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L45" s="10" t="s">
         <v>500</v>
@@ -5454,19 +5480,19 @@
         <v>42637</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G46">
         <v>4</v>
       </c>
       <c r="I46" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J46" t="s">
         <v>8</v>
       </c>
       <c r="K46" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L46" s="10" t="s">
         <v>500</v>
@@ -5513,19 +5539,19 @@
         <v>42638</v>
       </c>
       <c r="E47" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G47">
         <v>4</v>
       </c>
       <c r="I47" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J47" t="s">
         <v>8</v>
       </c>
       <c r="K47" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="L47" s="10" t="s">
         <v>500</v>
@@ -5572,19 +5598,19 @@
         <v>42639</v>
       </c>
       <c r="E48" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G48">
         <v>4</v>
       </c>
       <c r="I48" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J48" t="s">
         <v>8</v>
       </c>
       <c r="K48" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L48" s="10" t="s">
         <v>500</v>
@@ -5640,19 +5666,19 @@
         <v>42640</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G49">
         <v>4</v>
       </c>
       <c r="I49" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J49" t="s">
         <v>8</v>
       </c>
       <c r="K49" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L49" s="10" t="s">
         <v>500</v>
@@ -5699,19 +5725,19 @@
         <v>42641</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G50">
         <v>4</v>
       </c>
       <c r="I50" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J50" t="s">
         <v>8</v>
       </c>
       <c r="K50" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L50" s="10" t="s">
         <v>500</v>
@@ -5767,19 +5793,19 @@
         <v>42642</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G51">
         <v>4</v>
       </c>
       <c r="I51" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J51" t="s">
         <v>8</v>
       </c>
       <c r="K51" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L51" s="10" t="s">
         <v>500</v>
@@ -5835,19 +5861,19 @@
         <v>42643</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G52">
         <v>4</v>
       </c>
       <c r="I52" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J52" t="s">
         <v>8</v>
       </c>
       <c r="K52" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L52" s="10" t="s">
         <v>500</v>
@@ -5894,19 +5920,19 @@
         <v>42646</v>
       </c>
       <c r="E53" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G53">
         <v>4</v>
       </c>
       <c r="I53" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J53" t="s">
         <v>8</v>
       </c>
       <c r="K53" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L53" s="10" t="s">
         <v>500</v>
@@ -5953,19 +5979,19 @@
         <v>42647</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G54">
         <v>4</v>
       </c>
       <c r="I54" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J54" t="s">
         <v>8</v>
       </c>
       <c r="K54" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L54" s="10" t="s">
         <v>500</v>
@@ -6012,19 +6038,19 @@
         <v>42648</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
       <c r="G55">
         <v>4</v>
       </c>
       <c r="I55" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J55" t="s">
         <v>8</v>
       </c>
       <c r="K55" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="L55" s="10" t="s">
         <v>500</v>
@@ -6083,7 +6109,7 @@
         <v>88</v>
       </c>
       <c r="K56" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>563</v>
@@ -6160,7 +6186,7 @@
         <v>88</v>
       </c>
       <c r="K57" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>500</v>
@@ -6234,7 +6260,7 @@
         <v>88</v>
       </c>
       <c r="K58" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>500</v>
@@ -6308,7 +6334,7 @@
         <v>88</v>
       </c>
       <c r="K59" t="s">
-        <v>579</v>
+        <v>587</v>
       </c>
       <c r="L59" s="10" t="s">
         <v>500</v>
@@ -6382,7 +6408,7 @@
         <v>88</v>
       </c>
       <c r="K60" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>500</v>
@@ -6456,7 +6482,7 @@
         <v>88</v>
       </c>
       <c r="K61" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>500</v>
@@ -6530,7 +6556,7 @@
         <v>88</v>
       </c>
       <c r="K62" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>500</v>
@@ -6604,7 +6630,7 @@
         <v>88</v>
       </c>
       <c r="K63" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>500</v>
@@ -6678,7 +6704,7 @@
         <v>88</v>
       </c>
       <c r="K64" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>500</v>
@@ -6752,7 +6778,7 @@
         <v>88</v>
       </c>
       <c r="K65" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>500</v>
@@ -6826,7 +6852,7 @@
         <v>88</v>
       </c>
       <c r="K66" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>500</v>
@@ -6900,7 +6926,7 @@
         <v>88</v>
       </c>
       <c r="K67" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>500</v>
@@ -6974,7 +7000,7 @@
         <v>88</v>
       </c>
       <c r="K68" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>500</v>
@@ -7048,7 +7074,7 @@
         <v>88</v>
       </c>
       <c r="K69" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L69" s="10" t="s">
         <v>500</v>
@@ -7122,7 +7148,7 @@
         <v>88</v>
       </c>
       <c r="K70" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>500</v>
@@ -7196,7 +7222,7 @@
         <v>88</v>
       </c>
       <c r="K71" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>500</v>
@@ -7270,7 +7296,7 @@
         <v>88</v>
       </c>
       <c r="K72" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>500</v>
@@ -7344,7 +7370,7 @@
         <v>88</v>
       </c>
       <c r="K73" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>500</v>
@@ -7418,7 +7444,7 @@
         <v>88</v>
       </c>
       <c r="K74" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>500</v>
@@ -7492,7 +7518,7 @@
         <v>88</v>
       </c>
       <c r="K75" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L75" s="10" t="s">
         <v>500</v>
@@ -7566,7 +7592,7 @@
         <v>88</v>
       </c>
       <c r="K76" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L76" s="10" t="s">
         <v>505</v>
@@ -7640,7 +7666,7 @@
         <v>88</v>
       </c>
       <c r="K77" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L77" s="10" t="s">
         <v>563</v>
@@ -7702,7 +7728,7 @@
         <v>88</v>
       </c>
       <c r="K78" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L78" s="10" t="s">
         <v>500</v>
@@ -7776,7 +7802,7 @@
         <v>88</v>
       </c>
       <c r="K79" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L79" s="10" t="s">
         <v>500</v>
@@ -7850,7 +7876,7 @@
         <v>88</v>
       </c>
       <c r="K80" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L80" s="10" t="s">
         <v>500</v>
@@ -7927,7 +7953,7 @@
         <v>88</v>
       </c>
       <c r="K81" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>500</v>
@@ -8004,7 +8030,7 @@
         <v>88</v>
       </c>
       <c r="K82" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L82" s="10" t="s">
         <v>500</v>
@@ -8078,7 +8104,7 @@
         <v>88</v>
       </c>
       <c r="K83" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L83" s="10" t="s">
         <v>500</v>
@@ -8155,7 +8181,7 @@
         <v>88</v>
       </c>
       <c r="K84" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L84" s="10" t="s">
         <v>500</v>
@@ -8229,7 +8255,7 @@
         <v>88</v>
       </c>
       <c r="K85" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L85" s="10" t="s">
         <v>500</v>
@@ -8303,7 +8329,7 @@
         <v>88</v>
       </c>
       <c r="K86" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L86" s="10" t="s">
         <v>500</v>
@@ -8377,7 +8403,7 @@
         <v>88</v>
       </c>
       <c r="K87" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L87" s="10" t="s">
         <v>500</v>
@@ -8451,7 +8477,7 @@
         <v>88</v>
       </c>
       <c r="K88" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L88" s="10" t="s">
         <v>500</v>
@@ -8525,7 +8551,7 @@
         <v>88</v>
       </c>
       <c r="K89" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L89" s="10" t="s">
         <v>500</v>
@@ -8602,7 +8628,7 @@
         <v>88</v>
       </c>
       <c r="K90" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L90" s="10" t="s">
         <v>500</v>
@@ -8676,7 +8702,7 @@
         <v>88</v>
       </c>
       <c r="K91" t="s">
-        <v>577</v>
+        <v>588</v>
       </c>
       <c r="L91" s="10" t="s">
         <v>500</v>
@@ -9989,7 +10015,7 @@
         <v>8</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>500</v>
@@ -10064,7 +10090,7 @@
         <v>8</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>500</v>
@@ -10139,7 +10165,7 @@
         <v>8</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>581</v>
+        <v>589</v>
       </c>
       <c r="L111" s="10" t="s">
         <v>500</v>
@@ -10214,7 +10240,7 @@
         <v>8</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L112" s="10" t="s">
         <v>500</v>
@@ -10289,7 +10315,7 @@
         <v>8</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L113" s="10" t="s">
         <v>500</v>
@@ -10364,7 +10390,7 @@
         <v>8</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L114" s="10" t="s">
         <v>500</v>
@@ -10439,7 +10465,7 @@
         <v>8</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L115" s="10" t="s">
         <v>500</v>
@@ -10514,7 +10540,7 @@
         <v>8</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L116" s="10" t="s">
         <v>500</v>
@@ -10589,7 +10615,7 @@
         <v>8</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>580</v>
+        <v>590</v>
       </c>
       <c r="L117" s="10" t="s">
         <v>500</v>
@@ -10660,7 +10686,9 @@
       <c r="J118" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K118" s="1"/>
+      <c r="K118" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="L118" s="10" t="s">
         <v>500</v>
       </c>
@@ -10730,7 +10758,9 @@
       <c r="J119" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K119" s="1"/>
+      <c r="K119" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="L119" s="10" t="s">
         <v>500</v>
       </c>
@@ -10800,7 +10830,9 @@
       <c r="J120" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K120" s="1"/>
+      <c r="K120" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="L120" s="10" t="s">
         <v>500</v>
       </c>
@@ -10873,7 +10905,9 @@
       <c r="J121" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K121" s="1"/>
+      <c r="K121" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="L121" s="10" t="s">
         <v>500</v>
       </c>
@@ -10946,7 +10980,9 @@
       <c r="J122" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K122" s="1"/>
+      <c r="K122" s="1" t="s">
+        <v>590</v>
+      </c>
       <c r="L122" s="10" t="s">
         <v>500</v>
       </c>
@@ -11022,7 +11058,9 @@
       <c r="J123" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K123" s="1"/>
+      <c r="K123" s="1" t="s">
+        <v>591</v>
+      </c>
       <c r="L123" s="10" t="s">
         <v>500</v>
       </c>
@@ -11098,7 +11136,9 @@
       <c r="J124" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K124" s="1"/>
+      <c r="K124" s="1" t="s">
+        <v>592</v>
+      </c>
       <c r="L124" s="10" t="s">
         <v>500</v>
       </c>
@@ -11174,7 +11214,9 @@
       <c r="J125" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K125" s="1"/>
+      <c r="K125" s="1" t="s">
+        <v>593</v>
+      </c>
       <c r="L125" s="10" t="s">
         <v>500</v>
       </c>
@@ -11250,7 +11292,9 @@
       <c r="J126" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K126" s="1"/>
+      <c r="K126" s="1" t="s">
+        <v>593</v>
+      </c>
       <c r="L126" s="10" t="s">
         <v>500</v>
       </c>
@@ -11326,7 +11370,9 @@
       <c r="J127" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K127" s="1"/>
+      <c r="K127" s="1" t="s">
+        <v>594</v>
+      </c>
       <c r="L127" s="10" t="s">
         <v>500</v>
       </c>
@@ -11399,7 +11445,9 @@
       <c r="J128" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K128" s="1"/>
+      <c r="K128" s="1" t="s">
+        <v>594</v>
+      </c>
       <c r="L128" s="10" t="s">
         <v>500</v>
       </c>
@@ -11472,7 +11520,9 @@
       <c r="J129" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K129" s="1"/>
+      <c r="K129" s="1" t="s">
+        <v>594</v>
+      </c>
       <c r="L129" s="10" t="s">
         <v>500</v>
       </c>
@@ -11545,7 +11595,9 @@
       <c r="J130" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K130" s="1"/>
+      <c r="K130" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L130" s="10" t="s">
         <v>500</v>
       </c>
@@ -11618,7 +11670,9 @@
       <c r="J131" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K131" s="1"/>
+      <c r="K131" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L131" s="10" t="s">
         <v>500</v>
       </c>
@@ -11694,7 +11748,9 @@
       <c r="J132" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K132" s="1"/>
+      <c r="K132" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L132" s="10" t="s">
         <v>500</v>
       </c>
@@ -11770,7 +11826,9 @@
       <c r="J133" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K133" s="1"/>
+      <c r="K133" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L133" s="10" t="s">
         <v>505</v>
       </c>
@@ -11846,7 +11904,9 @@
       <c r="J134" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K134" s="1"/>
+      <c r="K134" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L134" s="10" t="s">
         <v>500</v>
       </c>
@@ -11919,7 +11979,9 @@
       <c r="J135" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K135" s="1"/>
+      <c r="K135" s="1" t="s">
+        <v>595</v>
+      </c>
       <c r="L135" s="10" t="s">
         <v>500</v>
       </c>
@@ -11992,7 +12054,9 @@
       <c r="J136" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K136" s="1"/>
+      <c r="K136" s="1" t="s">
+        <v>584</v>
+      </c>
       <c r="L136" s="10" t="s">
         <v>500</v>
       </c>
@@ -12068,7 +12132,9 @@
       <c r="J137" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K137" s="1"/>
+      <c r="K137" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L137" s="10" t="s">
         <v>500</v>
       </c>
@@ -12141,7 +12207,9 @@
       <c r="J138" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K138" s="1"/>
+      <c r="K138" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L138" s="10" t="s">
         <v>500</v>
       </c>
@@ -12217,7 +12285,9 @@
       <c r="J139" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K139" s="1"/>
+      <c r="K139" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L139" s="10" t="s">
         <v>500</v>
       </c>
@@ -12290,7 +12360,9 @@
       <c r="J140" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K140" s="1"/>
+      <c r="K140" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L140" s="10" t="s">
         <v>500</v>
       </c>
@@ -12363,7 +12435,9 @@
       <c r="J141" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K141" s="1"/>
+      <c r="K141" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L141" s="10" t="s">
         <v>500</v>
       </c>
@@ -12436,7 +12510,9 @@
       <c r="J142" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K142" s="1"/>
+      <c r="K142" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L142" s="10" t="s">
         <v>500</v>
       </c>
@@ -12509,7 +12585,9 @@
       <c r="J143" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K143" s="1"/>
+      <c r="K143" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L143" s="10" t="s">
         <v>500</v>
       </c>
@@ -12582,7 +12660,9 @@
       <c r="J144" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K144" s="1"/>
+      <c r="K144" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L144" s="10" t="s">
         <v>500</v>
       </c>
@@ -12655,7 +12735,9 @@
       <c r="J145" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K145" s="1"/>
+      <c r="K145" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L145" s="10" t="s">
         <v>500</v>
       </c>
@@ -12728,7 +12810,9 @@
       <c r="J146" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K146" s="1"/>
+      <c r="K146" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L146" s="10" t="s">
         <v>500</v>
       </c>
@@ -12801,7 +12885,9 @@
       <c r="J147" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K147" s="1"/>
+      <c r="K147" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L147" s="10" t="s">
         <v>500</v>
       </c>
@@ -12877,7 +12963,9 @@
       <c r="J148" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K148" s="1"/>
+      <c r="K148" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L148" s="10" t="s">
         <v>500</v>
       </c>
@@ -12950,7 +13038,9 @@
       <c r="J149" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K149" s="1"/>
+      <c r="K149" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L149" s="10" t="s">
         <v>500</v>
       </c>
@@ -13023,7 +13113,9 @@
       <c r="J150" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K150" s="1"/>
+      <c r="K150" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L150" s="10" t="s">
         <v>500</v>
       </c>
@@ -13096,7 +13188,9 @@
       <c r="J151" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K151" s="1"/>
+      <c r="K151" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L151" s="10" t="s">
         <v>500</v>
       </c>
@@ -13172,7 +13266,9 @@
       <c r="J152" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K152" s="1"/>
+      <c r="K152" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L152" s="10" t="s">
         <v>500</v>
       </c>
@@ -13245,7 +13341,9 @@
       <c r="J153" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K153" s="1"/>
+      <c r="K153" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L153" s="10" t="s">
         <v>500</v>
       </c>
@@ -13318,7 +13416,9 @@
       <c r="J154" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K154" s="1"/>
+      <c r="K154" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L154" s="10" t="s">
         <v>500</v>
       </c>
@@ -13394,7 +13494,9 @@
       <c r="J155" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K155" s="1"/>
+      <c r="K155" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L155" s="10" t="s">
         <v>500</v>
       </c>
@@ -13467,7 +13569,9 @@
       <c r="J156" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K156" s="1"/>
+      <c r="K156" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L156" s="10" t="s">
         <v>500</v>
       </c>
@@ -13540,7 +13644,9 @@
       <c r="J157" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K157" s="1"/>
+      <c r="K157" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L157" s="10" t="s">
         <v>500</v>
       </c>
@@ -13613,7 +13719,9 @@
       <c r="J158" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K158" s="1"/>
+      <c r="K158" s="1" t="s">
+        <v>585</v>
+      </c>
       <c r="L158" s="10" t="s">
         <v>500</v>
       </c>
@@ -14539,7 +14647,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AC47">
+  <autoFilter ref="A1:AC174">
     <sortState ref="A2:Y47">
       <sortCondition ref="D1:D39"/>
     </sortState>

</xml_diff>

<commit_message>
start a new cell summary (for the new sorting)
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="596">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2154" uniqueCount="597">
   <si>
     <t>date</t>
   </si>
@@ -1818,6 +1818,9 @@
   </si>
   <si>
     <t>{'DG','CA3','CA1','DG'}</t>
+  </si>
+  <si>
+    <t>{'???','WM','???','???'}</t>
   </si>
 </sst>
 </file>
@@ -2569,13 +2572,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B110" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K135" sqref="K135"/>
+      <selection pane="bottomRight" activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2713,7 +2717,7 @@
         <v>43158</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2">
@@ -2791,7 +2795,7 @@
         <v>43159</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3">
@@ -2869,7 +2873,7 @@
         <v>43160</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4">
@@ -2947,7 +2951,7 @@
         <v>43163</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>86</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5">
@@ -3038,7 +3042,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>500</v>
@@ -3116,7 +3120,7 @@
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>586</v>
+        <v>596</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>500</v>
@@ -4079,7 +4083,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -4121,7 +4125,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -4163,7 +4167,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -4205,7 +4209,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -4247,7 +4251,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -4289,7 +4293,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -4331,7 +4335,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -4373,7 +4377,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4415,7 +4419,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4457,7 +4461,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -4507,7 +4511,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -4557,7 +4561,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -4616,7 +4620,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -4675,7 +4679,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -4734,7 +4738,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -4793,7 +4797,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -4852,7 +4856,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -4911,7 +4915,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -4979,7 +4983,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -5038,7 +5042,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5100,7 +5104,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -5159,7 +5163,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -5218,7 +5222,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -5286,7 +5290,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -5348,7 +5352,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -5407,7 +5411,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -5466,7 +5470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -5525,7 +5529,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -5584,7 +5588,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -5652,7 +5656,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
@@ -5711,7 +5715,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>6</v>
       </c>
@@ -5779,7 +5783,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
@@ -5847,7 +5851,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -5906,7 +5910,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
@@ -5965,7 +5969,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
@@ -6024,7 +6028,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -6083,7 +6087,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -6160,7 +6164,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -6234,7 +6238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -6308,7 +6312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
@@ -6382,7 +6386,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
@@ -6456,7 +6460,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -6530,7 +6534,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
@@ -6604,7 +6608,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
@@ -6678,7 +6682,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
@@ -6752,7 +6756,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
@@ -6826,7 +6830,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
@@ -6900,7 +6904,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
@@ -6974,7 +6978,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -7048,7 +7052,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>99</v>
       </c>
@@ -7122,7 +7126,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>102</v>
       </c>
@@ -7196,7 +7200,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -7270,7 +7274,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>107</v>
       </c>
@@ -7344,7 +7348,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>110</v>
       </c>
@@ -7418,7 +7422,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>112</v>
       </c>
@@ -7492,7 +7496,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>115</v>
       </c>
@@ -7566,7 +7570,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>118</v>
       </c>
@@ -7640,7 +7644,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
@@ -7702,7 +7706,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>122</v>
       </c>
@@ -7776,7 +7780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>126</v>
       </c>
@@ -7850,7 +7854,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>129</v>
       </c>
@@ -7927,7 +7931,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>132</v>
       </c>
@@ -8004,7 +8008,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>135</v>
       </c>
@@ -8078,7 +8082,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>138</v>
       </c>
@@ -8155,7 +8159,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>141</v>
       </c>
@@ -8229,7 +8233,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>144</v>
       </c>
@@ -8303,7 +8307,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>147</v>
       </c>
@@ -8377,7 +8381,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>150</v>
       </c>
@@ -8451,7 +8455,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>153</v>
       </c>
@@ -8525,7 +8529,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>156</v>
       </c>
@@ -8602,7 +8606,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>159</v>
       </c>
@@ -8676,7 +8680,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -8753,7 +8757,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>232</v>
       </c>
@@ -8826,7 +8830,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>236</v>
       </c>
@@ -8902,7 +8906,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>240</v>
       </c>
@@ -8978,7 +8982,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>249</v>
       </c>
@@ -9048,7 +9052,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>256</v>
       </c>
@@ -9121,7 +9125,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
         <v>261</v>
       </c>
@@ -9194,7 +9198,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
         <v>264</v>
       </c>
@@ -9267,7 +9271,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
         <v>272</v>
       </c>
@@ -9340,7 +9344,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
         <v>276</v>
       </c>
@@ -9410,7 +9414,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
         <v>281</v>
       </c>
@@ -9480,7 +9484,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
         <v>284</v>
       </c>
@@ -9553,7 +9557,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
         <v>291</v>
       </c>
@@ -9626,7 +9630,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
         <v>309</v>
       </c>
@@ -9702,7 +9706,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
         <v>326</v>
       </c>
@@ -9769,7 +9773,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
         <v>334</v>
       </c>
@@ -9839,7 +9843,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
         <v>349</v>
       </c>
@@ -9915,7 +9919,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
         <v>355</v>
       </c>
@@ -9988,7 +9992,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>245</v>
       </c>
@@ -10063,7 +10067,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>246</v>
       </c>
@@ -10138,7 +10142,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>250</v>
       </c>
@@ -10213,7 +10217,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>253</v>
       </c>
@@ -10288,7 +10292,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>259</v>
       </c>
@@ -10363,7 +10367,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>262</v>
       </c>
@@ -10438,7 +10442,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>266</v>
       </c>
@@ -10513,7 +10517,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>269</v>
       </c>
@@ -10588,7 +10592,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>275</v>
       </c>
@@ -10660,7 +10664,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>277</v>
       </c>
@@ -10732,7 +10736,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>278</v>
       </c>
@@ -10804,7 +10808,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>282</v>
       </c>
@@ -10879,7 +10883,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>288</v>
       </c>
@@ -10954,7 +10958,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>292</v>
       </c>
@@ -11032,7 +11036,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>294</v>
       </c>
@@ -11110,7 +11114,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>297</v>
       </c>
@@ -11188,7 +11192,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>300</v>
       </c>
@@ -11266,7 +11270,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>305</v>
       </c>
@@ -11344,7 +11348,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>311</v>
       </c>
@@ -11419,7 +11423,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>313</v>
       </c>
@@ -11494,7 +11498,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>316</v>
       </c>
@@ -11569,7 +11573,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>319</v>
       </c>
@@ -11644,7 +11648,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>323</v>
       </c>
@@ -11722,7 +11726,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>329</v>
       </c>
@@ -11800,7 +11804,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>331</v>
       </c>
@@ -11878,7 +11882,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>337</v>
       </c>
@@ -11953,7 +11957,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>340</v>
       </c>
@@ -12028,7 +12032,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>343</v>
       </c>
@@ -12106,7 +12110,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>347</v>
       </c>
@@ -12181,7 +12185,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>353</v>
       </c>
@@ -12259,7 +12263,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>357</v>
       </c>
@@ -12334,7 +12338,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>358</v>
       </c>
@@ -12409,7 +12413,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>359</v>
       </c>
@@ -12484,7 +12488,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>360</v>
       </c>
@@ -12559,7 +12563,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>362</v>
       </c>
@@ -12634,7 +12638,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>364</v>
       </c>
@@ -12709,7 +12713,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>366</v>
       </c>
@@ -12784,7 +12788,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>368</v>
       </c>
@@ -12859,7 +12863,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="147" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>371</v>
       </c>
@@ -12937,7 +12941,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>373</v>
       </c>
@@ -13012,7 +13016,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>374</v>
       </c>
@@ -13087,7 +13091,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>376</v>
       </c>
@@ -13162,7 +13166,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>378</v>
       </c>
@@ -13240,7 +13244,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>381</v>
       </c>
@@ -13315,7 +13319,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>383</v>
       </c>
@@ -13390,7 +13394,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>384</v>
       </c>
@@ -13468,7 +13472,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>387</v>
       </c>
@@ -13543,7 +13547,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>388</v>
       </c>
@@ -13618,7 +13622,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>390</v>
       </c>
@@ -13693,7 +13697,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>392</v>
       </c>
@@ -13771,7 +13775,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>167</v>
       </c>
@@ -13844,7 +13848,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>173</v>
       </c>
@@ -13920,7 +13924,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>174</v>
       </c>
@@ -13996,7 +14000,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>177</v>
       </c>
@@ -14072,7 +14076,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>179</v>
       </c>
@@ -14148,7 +14152,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>182</v>
       </c>
@@ -14224,7 +14228,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>48</v>
       </c>
@@ -14268,7 +14272,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>49</v>
       </c>
@@ -14310,7 +14314,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>50</v>
       </c>
@@ -14352,7 +14356,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>51</v>
       </c>
@@ -14394,7 +14398,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>52</v>
       </c>
@@ -14436,7 +14440,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>53</v>
       </c>
@@ -14478,7 +14482,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>54</v>
       </c>
@@ -14520,7 +14524,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>55</v>
       </c>
@@ -14562,7 +14566,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>56</v>
       </c>
@@ -14604,7 +14608,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
@@ -14648,6 +14652,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AC174">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="34"/>
+      </filters>
+    </filterColumn>
     <sortState ref="A2:Y47">
       <sortCondition ref="D1:D39"/>
     </sortState>

</xml_diff>

<commit_message>
update summaries for sorting/cells/exp
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="597">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="598">
   <si>
     <t>date</t>
   </si>
@@ -1814,13 +1814,16 @@
     <t>{'DG','CA3','CA1','DG'}</t>
   </si>
   <si>
-    <t>{'???','WM','???','???'}</t>
-  </si>
-  <si>
     <t>problem with nlg clock diff (huge values)</t>
   </si>
   <si>
     <t>very small cells; probably omnetics got disconnected in the middle (abrupt noise from the middle)</t>
+  </si>
+  <si>
+    <t>{'WM','WM','CA1','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','CA1','CA1','WM'}</t>
   </si>
 </sst>
 </file>
@@ -2572,14 +2575,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AB100" sqref="AB100"/>
+      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2703,7 +2705,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>190</v>
       </c>
@@ -2781,7 +2783,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>191</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>192</v>
       </c>
@@ -2937,7 +2939,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -3015,7 +3017,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>196</v>
       </c>
@@ -3042,7 +3044,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>498</v>
@@ -3093,7 +3095,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -3120,7 +3122,7 @@
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>498</v>
@@ -3171,7 +3173,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>197</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>201</v>
       </c>
@@ -3327,7 +3329,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>204</v>
       </c>
@@ -3405,7 +3407,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>208</v>
       </c>
@@ -3480,7 +3482,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>211</v>
       </c>
@@ -3558,7 +3560,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>213</v>
       </c>
@@ -3633,7 +3635,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -3708,7 +3710,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>220</v>
       </c>
@@ -3858,7 +3860,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>223</v>
       </c>
@@ -3933,7 +3935,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>225</v>
       </c>
@@ -4008,7 +4010,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>230</v>
       </c>
@@ -4083,7 +4085,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -4125,7 +4127,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -4167,7 +4169,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -4251,7 +4253,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -4293,7 +4295,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -4335,7 +4337,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -4377,7 +4379,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4419,7 +4421,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4461,7 +4463,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -4511,7 +4513,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -4561,7 +4563,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -4620,7 +4622,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:28" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -4679,7 +4681,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -4738,7 +4740,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -4797,7 +4799,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -4856,7 +4858,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -4915,7 +4917,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -4983,7 +4985,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -5042,7 +5044,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5104,7 +5106,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="40" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -5163,7 +5165,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -5222,7 +5224,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -5290,7 +5292,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -5352,7 +5354,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -5411,7 +5413,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -5470,7 +5472,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -5529,7 +5531,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -5588,7 +5590,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -5656,7 +5658,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
@@ -5715,7 +5717,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>6</v>
       </c>
@@ -5783,7 +5785,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
@@ -5851,7 +5853,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -5910,7 +5912,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
@@ -5969,7 +5971,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
@@ -6028,7 +6030,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -6087,7 +6089,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -6164,7 +6166,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -6238,7 +6240,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -6312,7 +6314,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
@@ -6386,7 +6388,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
@@ -6460,7 +6462,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -6534,7 +6536,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
@@ -6608,7 +6610,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
@@ -6682,7 +6684,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
@@ -6756,7 +6758,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
@@ -6830,7 +6832,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
@@ -6904,7 +6906,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
@@ -6978,7 +6980,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -7052,7 +7054,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>99</v>
       </c>
@@ -7126,7 +7128,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>102</v>
       </c>
@@ -7200,7 +7202,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -7274,7 +7276,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>107</v>
       </c>
@@ -7348,7 +7350,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>110</v>
       </c>
@@ -7422,7 +7424,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>112</v>
       </c>
@@ -7496,7 +7498,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
         <v>115</v>
       </c>
@@ -7570,7 +7572,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>118</v>
       </c>
@@ -7644,7 +7646,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
@@ -7706,7 +7708,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>122</v>
       </c>
@@ -7780,7 +7782,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
         <v>126</v>
       </c>
@@ -7854,7 +7856,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>129</v>
       </c>
@@ -7931,7 +7933,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>132</v>
       </c>
@@ -8008,7 +8010,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>135</v>
       </c>
@@ -8082,7 +8084,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>138</v>
       </c>
@@ -8159,7 +8161,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>141</v>
       </c>
@@ -8233,7 +8235,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>144</v>
       </c>
@@ -8307,7 +8309,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>147</v>
       </c>
@@ -8381,7 +8383,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>150</v>
       </c>
@@ -8455,7 +8457,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>153</v>
       </c>
@@ -8529,7 +8531,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>156</v>
       </c>
@@ -8606,7 +8608,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>159</v>
       </c>
@@ -8680,7 +8682,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -8932,7 +8934,9 @@
       <c r="J94" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K94" s="1"/>
+      <c r="K94" t="s">
+        <v>588</v>
+      </c>
       <c r="L94" s="10" t="s">
         <v>498</v>
       </c>
@@ -9008,7 +9012,9 @@
       <c r="J95" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K95" s="1"/>
+      <c r="K95" t="s">
+        <v>588</v>
+      </c>
       <c r="L95" s="10" t="s">
         <v>498</v>
       </c>
@@ -9078,7 +9084,9 @@
       <c r="J96" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K96" s="1"/>
+      <c r="K96" t="s">
+        <v>597</v>
+      </c>
       <c r="L96" s="10" t="s">
         <v>498</v>
       </c>
@@ -9151,7 +9159,9 @@
       <c r="J97" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K97" s="1"/>
+      <c r="K97" t="s">
+        <v>597</v>
+      </c>
       <c r="L97" s="10" t="s">
         <v>498</v>
       </c>
@@ -9224,7 +9234,9 @@
       <c r="J98" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K98" s="1"/>
+      <c r="K98" t="s">
+        <v>597</v>
+      </c>
       <c r="L98" s="10" t="s">
         <v>498</v>
       </c>
@@ -9297,7 +9309,9 @@
       <c r="J99" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K99" s="1"/>
+      <c r="K99" t="s">
+        <v>597</v>
+      </c>
       <c r="L99" s="10" t="s">
         <v>498</v>
       </c>
@@ -9341,7 +9355,7 @@
         <v>272</v>
       </c>
       <c r="AB99" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.2">
@@ -9370,7 +9384,9 @@
       <c r="J100" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K100" s="1"/>
+      <c r="K100" t="s">
+        <v>597</v>
+      </c>
       <c r="L100" s="10" t="s">
         <v>498</v>
       </c>
@@ -9440,7 +9456,9 @@
       <c r="J101" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K101" s="1"/>
+      <c r="K101" t="s">
+        <v>597</v>
+      </c>
       <c r="L101" s="10" t="s">
         <v>498</v>
       </c>
@@ -9992,7 +10010,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="109" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
         <v>244</v>
       </c>
@@ -10067,7 +10085,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="110" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
         <v>245</v>
       </c>
@@ -10142,7 +10160,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
         <v>249</v>
       </c>
@@ -10217,7 +10235,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="112" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
         <v>252</v>
       </c>
@@ -10292,7 +10310,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="113" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>258</v>
       </c>
@@ -10367,7 +10385,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="114" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>261</v>
       </c>
@@ -10442,7 +10460,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="115" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>265</v>
       </c>
@@ -10517,7 +10535,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>268</v>
       </c>
@@ -10592,7 +10610,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="117" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>273</v>
       </c>
@@ -10664,7 +10682,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="118" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>275</v>
       </c>
@@ -10736,7 +10754,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="119" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>276</v>
       </c>
@@ -10808,7 +10826,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="120" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>280</v>
       </c>
@@ -10883,10 +10901,10 @@
         <v>281</v>
       </c>
       <c r="AC120" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="121" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>286</v>
       </c>
@@ -10961,7 +10979,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="122" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>290</v>
       </c>
@@ -11039,7 +11057,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="123" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>292</v>
       </c>
@@ -11117,7 +11135,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="124" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>295</v>
       </c>
@@ -11195,7 +11213,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="125" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
         <v>298</v>
       </c>
@@ -11273,7 +11291,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="126" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
         <v>303</v>
       </c>
@@ -11351,7 +11369,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="127" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
         <v>309</v>
       </c>
@@ -11426,7 +11444,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="128" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
         <v>311</v>
       </c>
@@ -11501,7 +11519,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
         <v>314</v>
       </c>
@@ -11576,7 +11594,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="130" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -11651,7 +11669,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
         <v>321</v>
       </c>
@@ -11729,7 +11747,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="132" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
         <v>327</v>
       </c>
@@ -11807,7 +11825,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
         <v>329</v>
       </c>
@@ -11885,7 +11903,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
         <v>335</v>
       </c>
@@ -11960,7 +11978,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
         <v>338</v>
       </c>
@@ -12035,7 +12053,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
         <v>341</v>
       </c>
@@ -12113,7 +12131,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="137" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
         <v>345</v>
       </c>
@@ -12188,7 +12206,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="138" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
         <v>351</v>
       </c>
@@ -12266,7 +12284,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="139" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
         <v>355</v>
       </c>
@@ -12341,7 +12359,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="140" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
         <v>356</v>
       </c>
@@ -12416,7 +12434,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="141" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
         <v>357</v>
       </c>
@@ -12491,7 +12509,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="142" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
         <v>358</v>
       </c>
@@ -12566,7 +12584,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
         <v>360</v>
       </c>
@@ -12641,7 +12659,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="144" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
         <v>362</v>
       </c>
@@ -12716,7 +12734,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="145" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
         <v>364</v>
       </c>
@@ -12791,7 +12809,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="146" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>366</v>
       </c>
@@ -12866,7 +12884,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="147" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" ht="15" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>369</v>
       </c>
@@ -12944,7 +12962,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="148" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
         <v>371</v>
       </c>
@@ -13019,7 +13037,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="149" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
         <v>372</v>
       </c>
@@ -13094,7 +13112,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="150" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
         <v>374</v>
       </c>
@@ -13169,7 +13187,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="151" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
         <v>376</v>
       </c>
@@ -13247,7 +13265,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="152" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
         <v>379</v>
       </c>
@@ -13322,7 +13340,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="153" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
         <v>381</v>
       </c>
@@ -13397,7 +13415,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="154" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
         <v>382</v>
       </c>
@@ -13475,7 +13493,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="155" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
         <v>385</v>
       </c>
@@ -13550,7 +13568,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="156" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
         <v>386</v>
       </c>
@@ -13625,7 +13643,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="157" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
         <v>388</v>
       </c>
@@ -13700,7 +13718,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="158" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
         <v>390</v>
       </c>
@@ -13778,7 +13796,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="159" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
         <v>167</v>
       </c>
@@ -13851,7 +13869,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
         <v>173</v>
       </c>
@@ -13927,7 +13945,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>174</v>
       </c>
@@ -14003,7 +14021,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>177</v>
       </c>
@@ -14079,7 +14097,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="163" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>179</v>
       </c>
@@ -14155,7 +14173,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="164" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>182</v>
       </c>
@@ -14231,7 +14249,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="165" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>48</v>
       </c>
@@ -14275,7 +14293,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>49</v>
       </c>
@@ -14317,7 +14335,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>50</v>
       </c>
@@ -14359,7 +14377,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>51</v>
       </c>
@@ -14401,7 +14419,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="169" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>52</v>
       </c>
@@ -14443,7 +14461,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>53</v>
       </c>
@@ -14485,7 +14503,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>54</v>
       </c>
@@ -14527,7 +14545,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>55</v>
       </c>
@@ -14569,7 +14587,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>56</v>
       </c>
@@ -14611,7 +14629,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
@@ -14655,11 +14673,6 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:AC174">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="2289"/>
-      </filters>
-    </filterColumn>
     <sortState ref="A2:Y47">
       <sortCondition ref="D1:D39"/>
     </sortState>

</xml_diff>

<commit_message>
update sorting - mostly bat 79 resorting by Tamir
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2163" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2199" uniqueCount="599">
   <si>
     <t>date</t>
   </si>
@@ -1793,9 +1793,6 @@
     <t>{'CA1','N/A','N/A','CA1'}</t>
   </si>
   <si>
-    <t>{'CA1','WM',WM','CA1'}</t>
-  </si>
-  <si>
     <t>{'CA1','CA1','CA1','CA1'}</t>
   </si>
   <si>
@@ -1824,6 +1821,12 @@
   </si>
   <si>
     <t>{'CA1','CA1','CA1','WM'}</t>
+  </si>
+  <si>
+    <t>{'TBD','TBD','TBD','TBD'}</t>
+  </si>
+  <si>
+    <t>{'CA1','WM','WM','CA1'}</t>
   </si>
 </sst>
 </file>
@@ -2578,10 +2581,10 @@
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C74" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B94" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K102" sqref="K102"/>
+      <selection pane="bottomRight" activeCell="K112" sqref="K112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3044,7 +3047,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>498</v>
@@ -3122,7 +3125,7 @@
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>498</v>
@@ -4110,7 +4113,9 @@
       <c r="J20" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K20" s="7"/>
+      <c r="K20" t="s">
+        <v>597</v>
+      </c>
       <c r="L20" s="10" t="s">
         <v>498</v>
       </c>
@@ -4152,7 +4157,9 @@
       <c r="J21" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K21" s="7"/>
+      <c r="K21" t="s">
+        <v>597</v>
+      </c>
       <c r="L21" s="10" t="s">
         <v>498</v>
       </c>
@@ -4194,7 +4201,9 @@
       <c r="J22" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K22" s="7"/>
+      <c r="K22" t="s">
+        <v>597</v>
+      </c>
       <c r="L22" s="10" t="s">
         <v>498</v>
       </c>
@@ -4236,7 +4245,9 @@
       <c r="J23" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K23" s="7"/>
+      <c r="K23" t="s">
+        <v>597</v>
+      </c>
       <c r="L23" s="10" t="s">
         <v>498</v>
       </c>
@@ -4278,7 +4289,9 @@
       <c r="J24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K24" s="7"/>
+      <c r="K24" t="s">
+        <v>597</v>
+      </c>
       <c r="L24" s="10" t="s">
         <v>498</v>
       </c>
@@ -4320,7 +4333,9 @@
       <c r="J25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K25" s="7"/>
+      <c r="K25" t="s">
+        <v>597</v>
+      </c>
       <c r="L25" s="10" t="s">
         <v>498</v>
       </c>
@@ -4362,7 +4377,9 @@
       <c r="J26" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K26" s="7"/>
+      <c r="K26" t="s">
+        <v>597</v>
+      </c>
       <c r="L26" s="10" t="s">
         <v>498</v>
       </c>
@@ -4404,7 +4421,9 @@
       <c r="J27" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K27" s="7"/>
+      <c r="K27" t="s">
+        <v>597</v>
+      </c>
       <c r="L27" s="10" t="s">
         <v>498</v>
       </c>
@@ -4446,7 +4465,9 @@
       <c r="J28" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K28" s="7"/>
+      <c r="K28" t="s">
+        <v>597</v>
+      </c>
       <c r="L28" s="10" t="s">
         <v>498</v>
       </c>
@@ -4487,6 +4508,9 @@
       </c>
       <c r="J29" t="s">
         <v>8</v>
+      </c>
+      <c r="K29" t="s">
+        <v>597</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>561</v>
@@ -4538,6 +4562,9 @@
       <c r="J30" t="s">
         <v>8</v>
       </c>
+      <c r="K30" t="s">
+        <v>597</v>
+      </c>
       <c r="L30" s="10" t="s">
         <v>561</v>
       </c>
@@ -8785,7 +8812,9 @@
       <c r="J92" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K92" s="1"/>
+      <c r="K92" t="s">
+        <v>597</v>
+      </c>
       <c r="L92" s="10" t="s">
         <v>498</v>
       </c>
@@ -8858,7 +8887,9 @@
       <c r="J93" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K93" s="1"/>
+      <c r="K93" t="s">
+        <v>597</v>
+      </c>
       <c r="L93" s="10" t="s">
         <v>498</v>
       </c>
@@ -8935,7 +8966,7 @@
         <v>8</v>
       </c>
       <c r="K94" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L94" s="10" t="s">
         <v>498</v>
@@ -9013,7 +9044,7 @@
         <v>8</v>
       </c>
       <c r="K95" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L95" s="10" t="s">
         <v>498</v>
@@ -9085,7 +9116,7 @@
         <v>8</v>
       </c>
       <c r="K96" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L96" s="10" t="s">
         <v>498</v>
@@ -9160,7 +9191,7 @@
         <v>8</v>
       </c>
       <c r="K97" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>498</v>
@@ -9235,7 +9266,7 @@
         <v>8</v>
       </c>
       <c r="K98" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>498</v>
@@ -9310,7 +9341,7 @@
         <v>8</v>
       </c>
       <c r="K99" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L99" s="10" t="s">
         <v>498</v>
@@ -9355,7 +9386,7 @@
         <v>272</v>
       </c>
       <c r="AB99" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="100" spans="1:29" x14ac:dyDescent="0.2">
@@ -9385,7 +9416,7 @@
         <v>8</v>
       </c>
       <c r="K100" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>498</v>
@@ -9457,7 +9488,7 @@
         <v>8</v>
       </c>
       <c r="K101" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>498</v>
@@ -9528,7 +9559,9 @@
       <c r="J102" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K102" s="1"/>
+      <c r="K102" t="s">
+        <v>597</v>
+      </c>
       <c r="L102" s="10" t="s">
         <v>498</v>
       </c>
@@ -9601,7 +9634,9 @@
       <c r="J103" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K103" s="1"/>
+      <c r="K103" t="s">
+        <v>597</v>
+      </c>
       <c r="L103" s="10" t="s">
         <v>498</v>
       </c>
@@ -9674,7 +9709,9 @@
       <c r="J104" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K104" s="1"/>
+      <c r="K104" t="s">
+        <v>597</v>
+      </c>
       <c r="L104" s="10" t="s">
         <v>498</v>
       </c>
@@ -9750,7 +9787,9 @@
       <c r="J105" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K105" s="1"/>
+      <c r="K105" t="s">
+        <v>597</v>
+      </c>
       <c r="L105" s="10" t="s">
         <v>561</v>
       </c>
@@ -9817,7 +9856,9 @@
       <c r="J106" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K106" s="1"/>
+      <c r="K106" t="s">
+        <v>597</v>
+      </c>
       <c r="L106" s="10" t="s">
         <v>498</v>
       </c>
@@ -9887,7 +9928,9 @@
       <c r="J107" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K107" s="1"/>
+      <c r="K107" t="s">
+        <v>597</v>
+      </c>
       <c r="L107" s="10" t="s">
         <v>498</v>
       </c>
@@ -9963,7 +10006,9 @@
       <c r="J108" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K108" s="1"/>
+      <c r="K108" t="s">
+        <v>597</v>
+      </c>
       <c r="L108" s="10" t="s">
         <v>498</v>
       </c>
@@ -10037,7 +10082,7 @@
         <v>8</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>498</v>
@@ -10112,7 +10157,7 @@
         <v>8</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>498</v>
@@ -10187,7 +10232,7 @@
         <v>8</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>587</v>
+        <v>598</v>
       </c>
       <c r="L111" s="10" t="s">
         <v>498</v>
@@ -10262,7 +10307,7 @@
         <v>8</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L112" s="10" t="s">
         <v>498</v>
@@ -10337,7 +10382,7 @@
         <v>8</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L113" s="10" t="s">
         <v>498</v>
@@ -10412,7 +10457,7 @@
         <v>8</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L114" s="10" t="s">
         <v>498</v>
@@ -10487,7 +10532,7 @@
         <v>8</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L115" s="10" t="s">
         <v>498</v>
@@ -10562,7 +10607,7 @@
         <v>8</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L116" s="10" t="s">
         <v>498</v>
@@ -10637,7 +10682,7 @@
         <v>8</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L117" s="10" t="s">
         <v>498</v>
@@ -10709,7 +10754,7 @@
         <v>8</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L118" s="10" t="s">
         <v>498</v>
@@ -10781,7 +10826,7 @@
         <v>8</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L119" s="10" t="s">
         <v>498</v>
@@ -10853,7 +10898,7 @@
         <v>8</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L120" s="10" t="s">
         <v>498</v>
@@ -10901,7 +10946,7 @@
         <v>281</v>
       </c>
       <c r="AC120" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="121" spans="1:29" x14ac:dyDescent="0.2">
@@ -10931,7 +10976,7 @@
         <v>8</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L121" s="10" t="s">
         <v>498</v>
@@ -11006,7 +11051,7 @@
         <v>8</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L122" s="10" t="s">
         <v>498</v>
@@ -11084,7 +11129,7 @@
         <v>8</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L123" s="10" t="s">
         <v>498</v>
@@ -11162,7 +11207,7 @@
         <v>8</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L124" s="10" t="s">
         <v>498</v>
@@ -11240,7 +11285,7 @@
         <v>8</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L125" s="10" t="s">
         <v>498</v>
@@ -11318,7 +11363,7 @@
         <v>8</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L126" s="10" t="s">
         <v>498</v>
@@ -11396,7 +11441,7 @@
         <v>8</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L127" s="10" t="s">
         <v>498</v>
@@ -11471,7 +11516,7 @@
         <v>8</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L128" s="10" t="s">
         <v>498</v>
@@ -11546,7 +11591,7 @@
         <v>8</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L129" s="10" t="s">
         <v>498</v>
@@ -11621,7 +11666,7 @@
         <v>8</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L130" s="10" t="s">
         <v>498</v>
@@ -11696,7 +11741,7 @@
         <v>8</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L131" s="10" t="s">
         <v>498</v>
@@ -11774,7 +11819,7 @@
         <v>8</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L132" s="10" t="s">
         <v>498</v>
@@ -11852,7 +11897,7 @@
         <v>8</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L133" s="10" t="s">
         <v>503</v>
@@ -11930,7 +11975,7 @@
         <v>8</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L134" s="10" t="s">
         <v>498</v>
@@ -12005,7 +12050,7 @@
         <v>8</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="L135" s="10" t="s">
         <v>498</v>
@@ -13822,7 +13867,9 @@
       <c r="J159" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K159" s="1"/>
+      <c r="K159" t="s">
+        <v>597</v>
+      </c>
       <c r="L159" s="10" t="s">
         <v>498</v>
       </c>
@@ -13895,7 +13942,9 @@
       <c r="J160" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K160" s="1"/>
+      <c r="K160" t="s">
+        <v>597</v>
+      </c>
       <c r="L160" s="10" t="s">
         <v>498</v>
       </c>
@@ -13971,7 +14020,9 @@
       <c r="J161" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K161" s="1"/>
+      <c r="K161" t="s">
+        <v>597</v>
+      </c>
       <c r="L161" s="10" t="s">
         <v>498</v>
       </c>
@@ -14047,7 +14098,9 @@
       <c r="J162" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K162" s="1"/>
+      <c r="K162" t="s">
+        <v>597</v>
+      </c>
       <c r="L162" s="10" t="s">
         <v>498</v>
       </c>
@@ -14123,7 +14176,9 @@
       <c r="J163" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K163" s="1"/>
+      <c r="K163" t="s">
+        <v>597</v>
+      </c>
       <c r="L163" s="10" t="s">
         <v>498</v>
       </c>
@@ -14199,7 +14254,9 @@
       <c r="J164" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K164" s="1"/>
+      <c r="K164" t="s">
+        <v>597</v>
+      </c>
       <c r="L164" s="10" t="s">
         <v>498</v>
       </c>
@@ -14274,6 +14331,9 @@
       <c r="J165" t="s">
         <v>8</v>
       </c>
+      <c r="K165" t="s">
+        <v>597</v>
+      </c>
       <c r="L165" s="10" t="s">
         <v>498</v>
       </c>
@@ -14318,7 +14378,9 @@
       <c r="J166" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K166" s="7"/>
+      <c r="K166" t="s">
+        <v>597</v>
+      </c>
       <c r="L166" s="10" t="s">
         <v>498</v>
       </c>
@@ -14360,7 +14422,9 @@
       <c r="J167" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K167" s="7"/>
+      <c r="K167" t="s">
+        <v>597</v>
+      </c>
       <c r="L167" s="10" t="s">
         <v>498</v>
       </c>
@@ -14402,7 +14466,9 @@
       <c r="J168" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K168" s="7"/>
+      <c r="K168" t="s">
+        <v>597</v>
+      </c>
       <c r="L168" s="10" t="s">
         <v>498</v>
       </c>
@@ -14444,7 +14510,9 @@
       <c r="J169" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K169" s="7"/>
+      <c r="K169" t="s">
+        <v>597</v>
+      </c>
       <c r="L169" s="10" t="s">
         <v>498</v>
       </c>
@@ -14486,7 +14554,9 @@
       <c r="J170" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K170" s="7"/>
+      <c r="K170" t="s">
+        <v>597</v>
+      </c>
       <c r="L170" s="10" t="s">
         <v>498</v>
       </c>
@@ -14528,7 +14598,9 @@
       <c r="J171" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K171" s="7"/>
+      <c r="K171" t="s">
+        <v>597</v>
+      </c>
       <c r="L171" s="10" t="s">
         <v>498</v>
       </c>
@@ -14570,7 +14642,9 @@
       <c r="J172" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K172" s="7"/>
+      <c r="K172" t="s">
+        <v>597</v>
+      </c>
       <c r="L172" s="10" t="s">
         <v>498</v>
       </c>
@@ -14612,7 +14686,9 @@
       <c r="J173" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K173" s="7"/>
+      <c r="K173" t="s">
+        <v>597</v>
+      </c>
       <c r="L173" s="10" t="s">
         <v>498</v>
       </c>
@@ -14654,7 +14730,9 @@
       <c r="J174" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="K174" s="7"/>
+      <c r="K174" t="s">
+        <v>597</v>
+      </c>
       <c r="L174" s="10" t="s">
         <v>498</v>
       </c>

</xml_diff>

<commit_message>
update CA3/DG histology identification for bats 9681 and 2289
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="742">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="745">
   <si>
     <t>date</t>
   </si>
@@ -1137,7 +1137,7 @@
         <b/>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Arial"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -1781,9 +1781,6 @@
     <t>{'DG','CA3','WM2','DG'}</t>
   </si>
   <si>
-    <t>{'DG','CA3','DG/CA3','DG'}</t>
-  </si>
-  <si>
     <t>{'CA1','WM','CA1','CA1'}</t>
   </si>
   <si>
@@ -2256,6 +2253,18 @@
   </si>
   <si>
     <t>[1820;2780;2440;1900]</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','DG','DG'}</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','WM3','DG'}</t>
+  </si>
+  <si>
+    <t>{'DG','CA3','CA3','DG'}</t>
+  </si>
+  <si>
+    <t>{'TBD','TBD','TBD','CA3'}</t>
   </si>
 </sst>
 </file>
@@ -2266,7 +2275,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -2274,14 +2283,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -3010,45 +3019,45 @@
   <dimension ref="A1:AC174"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q48" sqref="Q48"/>
+      <selection pane="bottomRight" activeCell="K108" sqref="K108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15" style="1" customWidth="1"/>
-    <col min="2" max="2" width="4.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="4.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="2" customWidth="1"/>
-    <col min="8" max="8" width="26.5" customWidth="1"/>
-    <col min="9" max="9" width="27.5" customWidth="1"/>
-    <col min="10" max="10" width="8.625" customWidth="1"/>
-    <col min="11" max="11" width="25.625" customWidth="1"/>
-    <col min="12" max="12" width="2.75" customWidth="1"/>
-    <col min="13" max="13" width="12.5" style="9" customWidth="1"/>
-    <col min="14" max="14" width="2.75" customWidth="1"/>
-    <col min="15" max="15" width="2.5" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" customWidth="1"/>
+    <col min="9" max="9" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="11" max="11" width="25.5703125" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="2.7109375" customWidth="1"/>
+    <col min="15" max="15" width="2.42578125" customWidth="1"/>
     <col min="16" max="16" width="3" customWidth="1"/>
-    <col min="17" max="17" width="5.5" customWidth="1"/>
-    <col min="18" max="18" width="6.5" customWidth="1"/>
-    <col min="19" max="19" width="3.125" customWidth="1"/>
-    <col min="20" max="20" width="5.375" customWidth="1"/>
-    <col min="21" max="21" width="19.5" customWidth="1"/>
+    <col min="17" max="17" width="5.42578125" customWidth="1"/>
+    <col min="18" max="18" width="6.42578125" customWidth="1"/>
+    <col min="19" max="19" width="3.140625" customWidth="1"/>
+    <col min="20" max="20" width="5.42578125" customWidth="1"/>
+    <col min="21" max="21" width="19.42578125" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
-    <col min="23" max="23" width="3.75" customWidth="1"/>
-    <col min="24" max="24" width="2.5" customWidth="1"/>
-    <col min="25" max="25" width="3.75" customWidth="1"/>
-    <col min="26" max="26" width="4.875" customWidth="1"/>
+    <col min="23" max="23" width="3.7109375" customWidth="1"/>
+    <col min="24" max="24" width="2.42578125" customWidth="1"/>
+    <col min="25" max="25" width="3.7109375" customWidth="1"/>
+    <col min="26" max="26" width="4.85546875" customWidth="1"/>
     <col min="27" max="27" width="20" customWidth="1"/>
-    <col min="28" max="28" width="107.625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="78.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="107.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="2" customFormat="1" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3137,7 +3146,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>190</v>
       </c>
@@ -3158,7 +3167,7 @@
         <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>7</v>
@@ -3218,7 +3227,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>191</v>
       </c>
@@ -3239,7 +3248,7 @@
         <v>4</v>
       </c>
       <c r="H3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>7</v>
@@ -3299,7 +3308,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>192</v>
       </c>
@@ -3320,7 +3329,7 @@
         <v>4</v>
       </c>
       <c r="H4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>7</v>
@@ -3380,7 +3389,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>193</v>
       </c>
@@ -3401,7 +3410,7 @@
         <v>4</v>
       </c>
       <c r="H5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>7</v>
@@ -3461,7 +3470,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>196</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>7</v>
@@ -3491,7 +3500,7 @@
         <v>8</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>498</v>
@@ -3542,7 +3551,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>195</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>7</v>
@@ -3572,7 +3581,7 @@
         <v>8</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>498</v>
@@ -3623,7 +3632,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>197</v>
       </c>
@@ -3644,7 +3653,7 @@
         <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>7</v>
@@ -3653,7 +3662,7 @@
         <v>8</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>498</v>
@@ -3704,7 +3713,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>201</v>
       </c>
@@ -3725,7 +3734,7 @@
         <v>4</v>
       </c>
       <c r="H9" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>7</v>
@@ -3734,7 +3743,7 @@
         <v>8</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>498</v>
@@ -3785,7 +3794,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>204</v>
       </c>
@@ -3806,7 +3815,7 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>7</v>
@@ -3815,7 +3824,7 @@
         <v>8</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>498</v>
@@ -3866,7 +3875,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>208</v>
       </c>
@@ -3887,7 +3896,7 @@
         <v>4</v>
       </c>
       <c r="H11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>7</v>
@@ -3896,7 +3905,7 @@
         <v>8</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>498</v>
@@ -3944,7 +3953,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>211</v>
       </c>
@@ -3965,7 +3974,7 @@
         <v>4</v>
       </c>
       <c r="H12" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>7</v>
@@ -3974,7 +3983,7 @@
         <v>8</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>498</v>
@@ -4025,7 +4034,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>213</v>
       </c>
@@ -4046,7 +4055,7 @@
         <v>4</v>
       </c>
       <c r="H13" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>7</v>
@@ -4055,7 +4064,7 @@
         <v>8</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>498</v>
@@ -4103,7 +4112,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>215</v>
       </c>
@@ -4124,7 +4133,7 @@
         <v>4</v>
       </c>
       <c r="H14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>7</v>
@@ -4133,7 +4142,7 @@
         <v>8</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>498</v>
@@ -4181,7 +4190,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>217</v>
       </c>
@@ -4202,7 +4211,7 @@
         <v>4</v>
       </c>
       <c r="H15" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>7</v>
@@ -4259,7 +4268,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>220</v>
       </c>
@@ -4280,7 +4289,7 @@
         <v>4</v>
       </c>
       <c r="H16" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>7</v>
@@ -4337,7 +4346,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>223</v>
       </c>
@@ -4358,7 +4367,7 @@
         <v>4</v>
       </c>
       <c r="H17" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>7</v>
@@ -4415,7 +4424,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>225</v>
       </c>
@@ -4436,7 +4445,7 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>7</v>
@@ -4493,7 +4502,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>230</v>
       </c>
@@ -4514,7 +4523,7 @@
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>7</v>
@@ -4571,7 +4580,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -4591,7 +4600,7 @@
         <v>4</v>
       </c>
       <c r="H20" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I20" s="7" t="s">
         <v>86</v>
@@ -4600,7 +4609,7 @@
         <v>86</v>
       </c>
       <c r="K20" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>498</v>
@@ -4618,7 +4627,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
@@ -4638,7 +4647,7 @@
         <v>4</v>
       </c>
       <c r="H21" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I21" s="7" t="s">
         <v>86</v>
@@ -4647,7 +4656,7 @@
         <v>86</v>
       </c>
       <c r="K21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L21" s="10" t="s">
         <v>498</v>
@@ -4665,7 +4674,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -4685,7 +4694,7 @@
         <v>4</v>
       </c>
       <c r="H22" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I22" s="7" t="s">
         <v>86</v>
@@ -4694,7 +4703,7 @@
         <v>86</v>
       </c>
       <c r="K22" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L22" s="10" t="s">
         <v>498</v>
@@ -4712,7 +4721,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>42</v>
       </c>
@@ -4732,7 +4741,7 @@
         <v>4</v>
       </c>
       <c r="H23" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I23" s="7" t="s">
         <v>86</v>
@@ -4741,7 +4750,7 @@
         <v>86</v>
       </c>
       <c r="K23" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L23" s="10" t="s">
         <v>498</v>
@@ -4759,7 +4768,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>43</v>
       </c>
@@ -4779,7 +4788,7 @@
         <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I24" s="7" t="s">
         <v>86</v>
@@ -4788,7 +4797,7 @@
         <v>86</v>
       </c>
       <c r="K24" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L24" s="10" t="s">
         <v>498</v>
@@ -4806,7 +4815,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -4826,7 +4835,7 @@
         <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I25" s="7" t="s">
         <v>86</v>
@@ -4835,7 +4844,7 @@
         <v>86</v>
       </c>
       <c r="K25" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L25" s="10" t="s">
         <v>498</v>
@@ -4853,7 +4862,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
@@ -4873,7 +4882,7 @@
         <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I26" s="7" t="s">
         <v>86</v>
@@ -4882,7 +4891,7 @@
         <v>86</v>
       </c>
       <c r="K26" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L26" s="10" t="s">
         <v>498</v>
@@ -4900,7 +4909,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
@@ -4920,7 +4929,7 @@
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I27" s="7" t="s">
         <v>86</v>
@@ -4929,7 +4938,7 @@
         <v>86</v>
       </c>
       <c r="K27" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L27" s="10" t="s">
         <v>498</v>
@@ -4947,7 +4956,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>47</v>
       </c>
@@ -4967,7 +4976,7 @@
         <v>4</v>
       </c>
       <c r="H28" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I28" s="7" t="s">
         <v>86</v>
@@ -4976,7 +4985,7 @@
         <v>86</v>
       </c>
       <c r="K28" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L28" s="10" t="s">
         <v>498</v>
@@ -4994,7 +5003,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>1</v>
       </c>
@@ -5014,7 +5023,7 @@
         <v>4</v>
       </c>
       <c r="H29" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I29" t="s">
         <v>577</v>
@@ -5023,7 +5032,7 @@
         <v>8</v>
       </c>
       <c r="K29" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L29" s="10" t="s">
         <v>561</v>
@@ -5050,7 +5059,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>13</v>
       </c>
@@ -5070,7 +5079,7 @@
         <v>4</v>
       </c>
       <c r="H30" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I30" t="s">
         <v>577</v>
@@ -5079,7 +5088,7 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L30" s="10" t="s">
         <v>561</v>
@@ -5106,7 +5115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>14</v>
       </c>
@@ -5126,7 +5135,7 @@
         <v>4</v>
       </c>
       <c r="H31" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I31" t="s">
         <v>577</v>
@@ -5177,7 +5186,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -5197,7 +5206,7 @@
         <v>4</v>
       </c>
       <c r="H32" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="I32" t="s">
         <v>577</v>
@@ -5248,7 +5257,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>16</v>
       </c>
@@ -5268,7 +5277,7 @@
         <v>4</v>
       </c>
       <c r="H33" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="I33" t="s">
         <v>577</v>
@@ -5319,7 +5328,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>17</v>
       </c>
@@ -5339,7 +5348,7 @@
         <v>4</v>
       </c>
       <c r="H34" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="I34" t="s">
         <v>577</v>
@@ -5390,7 +5399,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>18</v>
       </c>
@@ -5410,7 +5419,7 @@
         <v>4</v>
       </c>
       <c r="H35" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="I35" t="s">
         <v>577</v>
@@ -5461,7 +5470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>20</v>
       </c>
@@ -5481,7 +5490,7 @@
         <v>4</v>
       </c>
       <c r="H36" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="I36" t="s">
         <v>577</v>
@@ -5532,7 +5541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -5552,7 +5561,7 @@
         <v>4</v>
       </c>
       <c r="H37" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="I37" t="s">
         <v>577</v>
@@ -5603,7 +5612,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>22</v>
       </c>
@@ -5623,7 +5632,7 @@
         <v>4</v>
       </c>
       <c r="H38" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="I38" t="s">
         <v>577</v>
@@ -5674,7 +5683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>23</v>
       </c>
@@ -5694,7 +5703,7 @@
         <v>4</v>
       </c>
       <c r="H39" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="I39" t="s">
         <v>577</v>
@@ -5748,7 +5757,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -5768,7 +5777,7 @@
         <v>4</v>
       </c>
       <c r="H40" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="I40" t="s">
         <v>577</v>
@@ -5819,7 +5828,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
@@ -5839,7 +5848,7 @@
         <v>4</v>
       </c>
       <c r="H41" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="I41" t="s">
         <v>577</v>
@@ -5890,7 +5899,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>25</v>
       </c>
@@ -5910,7 +5919,7 @@
         <v>4</v>
       </c>
       <c r="H42" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="I42" t="s">
         <v>577</v>
@@ -5961,7 +5970,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>26</v>
       </c>
@@ -5981,7 +5990,7 @@
         <v>4</v>
       </c>
       <c r="H43" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="I43" t="s">
         <v>577</v>
@@ -6035,7 +6044,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>27</v>
       </c>
@@ -6055,7 +6064,7 @@
         <v>4</v>
       </c>
       <c r="H44" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="I44" t="s">
         <v>577</v>
@@ -6106,7 +6115,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>28</v>
       </c>
@@ -6126,7 +6135,7 @@
         <v>4</v>
       </c>
       <c r="H45" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="I45" t="s">
         <v>577</v>
@@ -6177,7 +6186,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>29</v>
       </c>
@@ -6197,7 +6206,7 @@
         <v>4</v>
       </c>
       <c r="H46" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="I46" t="s">
         <v>577</v>
@@ -6248,7 +6257,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>30</v>
       </c>
@@ -6268,7 +6277,7 @@
         <v>4</v>
       </c>
       <c r="H47" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="I47" t="s">
         <v>577</v>
@@ -6319,7 +6328,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>31</v>
       </c>
@@ -6339,7 +6348,7 @@
         <v>4</v>
       </c>
       <c r="H48" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I48" t="s">
         <v>577</v>
@@ -6390,7 +6399,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>32</v>
       </c>
@@ -6410,7 +6419,7 @@
         <v>4</v>
       </c>
       <c r="H49" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="I49" t="s">
         <v>577</v>
@@ -6461,7 +6470,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>6</v>
       </c>
@@ -6481,7 +6490,7 @@
         <v>4</v>
       </c>
       <c r="H50" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="I50" t="s">
         <v>577</v>
@@ -6532,7 +6541,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>33</v>
       </c>
@@ -6552,7 +6561,7 @@
         <v>4</v>
       </c>
       <c r="H51" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="I51" t="s">
         <v>577</v>
@@ -6603,7 +6612,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>34</v>
       </c>
@@ -6623,7 +6632,7 @@
         <v>4</v>
       </c>
       <c r="H52" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="I52" t="s">
         <v>577</v>
@@ -6674,7 +6683,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>35</v>
       </c>
@@ -6694,7 +6703,7 @@
         <v>4</v>
       </c>
       <c r="H53" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="I53" t="s">
         <v>577</v>
@@ -6745,7 +6754,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>36</v>
       </c>
@@ -6765,7 +6774,7 @@
         <v>4</v>
       </c>
       <c r="H54" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="I54" t="s">
         <v>577</v>
@@ -6816,7 +6825,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>37</v>
       </c>
@@ -6836,7 +6845,7 @@
         <v>4</v>
       </c>
       <c r="H55" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="I55" t="s">
         <v>577</v>
@@ -6887,7 +6896,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
@@ -6907,7 +6916,7 @@
         <v>4</v>
       </c>
       <c r="H56" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="I56" t="s">
         <v>63</v>
@@ -6916,7 +6925,7 @@
         <v>88</v>
       </c>
       <c r="K56" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L56" s="10" t="s">
         <v>561</v>
@@ -6967,7 +6976,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>62</v>
       </c>
@@ -6987,7 +6996,7 @@
         <v>4</v>
       </c>
       <c r="H57" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="I57" t="s">
         <v>63</v>
@@ -6996,7 +7005,7 @@
         <v>88</v>
       </c>
       <c r="K57" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L57" s="10" t="s">
         <v>498</v>
@@ -7044,7 +7053,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -7064,7 +7073,7 @@
         <v>4</v>
       </c>
       <c r="H58" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="I58" t="s">
         <v>63</v>
@@ -7073,7 +7082,7 @@
         <v>88</v>
       </c>
       <c r="K58" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L58" s="10" t="s">
         <v>498</v>
@@ -7121,7 +7130,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>70</v>
       </c>
@@ -7141,7 +7150,7 @@
         <v>4</v>
       </c>
       <c r="H59" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="I59" t="s">
         <v>63</v>
@@ -7150,7 +7159,7 @@
         <v>88</v>
       </c>
       <c r="K59" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="L59" s="10" t="s">
         <v>498</v>
@@ -7198,7 +7207,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>73</v>
       </c>
@@ -7218,7 +7227,7 @@
         <v>4</v>
       </c>
       <c r="H60" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="I60" t="s">
         <v>63</v>
@@ -7227,7 +7236,7 @@
         <v>88</v>
       </c>
       <c r="K60" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L60" s="10" t="s">
         <v>498</v>
@@ -7275,7 +7284,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>76</v>
       </c>
@@ -7295,7 +7304,7 @@
         <v>4</v>
       </c>
       <c r="H61" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="I61" t="s">
         <v>63</v>
@@ -7304,7 +7313,7 @@
         <v>88</v>
       </c>
       <c r="K61" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L61" s="10" t="s">
         <v>498</v>
@@ -7352,7 +7361,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>79</v>
       </c>
@@ -7372,7 +7381,7 @@
         <v>4</v>
       </c>
       <c r="H62" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="I62" t="s">
         <v>63</v>
@@ -7381,7 +7390,7 @@
         <v>88</v>
       </c>
       <c r="K62" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L62" s="10" t="s">
         <v>498</v>
@@ -7429,7 +7438,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>82</v>
       </c>
@@ -7449,7 +7458,7 @@
         <v>4</v>
       </c>
       <c r="H63" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="I63" t="s">
         <v>63</v>
@@ -7458,7 +7467,7 @@
         <v>88</v>
       </c>
       <c r="K63" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L63" s="10" t="s">
         <v>498</v>
@@ -7506,7 +7515,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>87</v>
       </c>
@@ -7526,7 +7535,7 @@
         <v>4</v>
       </c>
       <c r="H64" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="I64" t="s">
         <v>63</v>
@@ -7535,7 +7544,7 @@
         <v>88</v>
       </c>
       <c r="K64" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L64" s="10" t="s">
         <v>498</v>
@@ -7583,7 +7592,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>89</v>
       </c>
@@ -7603,7 +7612,7 @@
         <v>4</v>
       </c>
       <c r="H65" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="I65" t="s">
         <v>63</v>
@@ -7612,7 +7621,7 @@
         <v>88</v>
       </c>
       <c r="K65" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L65" s="10" t="s">
         <v>498</v>
@@ -7660,7 +7669,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>91</v>
       </c>
@@ -7680,7 +7689,7 @@
         <v>4</v>
       </c>
       <c r="H66" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="I66" t="s">
         <v>63</v>
@@ -7689,7 +7698,7 @@
         <v>88</v>
       </c>
       <c r="K66" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L66" s="10" t="s">
         <v>498</v>
@@ -7737,7 +7746,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>94</v>
       </c>
@@ -7757,7 +7766,7 @@
         <v>4</v>
       </c>
       <c r="H67" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="I67" t="s">
         <v>63</v>
@@ -7766,7 +7775,7 @@
         <v>88</v>
       </c>
       <c r="K67" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L67" s="10" t="s">
         <v>498</v>
@@ -7814,7 +7823,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>96</v>
       </c>
@@ -7834,7 +7843,7 @@
         <v>4</v>
       </c>
       <c r="H68" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I68" t="s">
         <v>63</v>
@@ -7843,7 +7852,7 @@
         <v>88</v>
       </c>
       <c r="K68" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L68" s="10" t="s">
         <v>498</v>
@@ -7891,7 +7900,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>99</v>
       </c>
@@ -7911,7 +7920,7 @@
         <v>4</v>
       </c>
       <c r="H69" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I69" t="s">
         <v>63</v>
@@ -7920,7 +7929,7 @@
         <v>88</v>
       </c>
       <c r="K69" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L69" s="10" t="s">
         <v>498</v>
@@ -7968,7 +7977,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>102</v>
       </c>
@@ -7988,7 +7997,7 @@
         <v>4</v>
       </c>
       <c r="H70" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I70" t="s">
         <v>63</v>
@@ -7997,7 +8006,7 @@
         <v>88</v>
       </c>
       <c r="K70" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L70" s="10" t="s">
         <v>498</v>
@@ -8045,7 +8054,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>104</v>
       </c>
@@ -8065,7 +8074,7 @@
         <v>4</v>
       </c>
       <c r="H71" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I71" t="s">
         <v>63</v>
@@ -8074,7 +8083,7 @@
         <v>88</v>
       </c>
       <c r="K71" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L71" s="10" t="s">
         <v>498</v>
@@ -8122,7 +8131,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>107</v>
       </c>
@@ -8142,7 +8151,7 @@
         <v>4</v>
       </c>
       <c r="H72" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I72" t="s">
         <v>63</v>
@@ -8151,7 +8160,7 @@
         <v>88</v>
       </c>
       <c r="K72" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L72" s="10" t="s">
         <v>498</v>
@@ -8199,7 +8208,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>110</v>
       </c>
@@ -8219,7 +8228,7 @@
         <v>4</v>
       </c>
       <c r="H73" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I73" t="s">
         <v>63</v>
@@ -8228,7 +8237,7 @@
         <v>88</v>
       </c>
       <c r="K73" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L73" s="10" t="s">
         <v>498</v>
@@ -8276,7 +8285,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>112</v>
       </c>
@@ -8296,7 +8305,7 @@
         <v>4</v>
       </c>
       <c r="H74" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I74" t="s">
         <v>63</v>
@@ -8305,7 +8314,7 @@
         <v>88</v>
       </c>
       <c r="K74" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L74" s="10" t="s">
         <v>498</v>
@@ -8353,7 +8362,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
         <v>115</v>
       </c>
@@ -8373,7 +8382,7 @@
         <v>4</v>
       </c>
       <c r="H75" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I75" t="s">
         <v>63</v>
@@ -8382,7 +8391,7 @@
         <v>88</v>
       </c>
       <c r="K75" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L75" s="10" t="s">
         <v>498</v>
@@ -8430,7 +8439,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
         <v>118</v>
       </c>
@@ -8450,7 +8459,7 @@
         <v>4</v>
       </c>
       <c r="H76" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I76" t="s">
         <v>63</v>
@@ -8459,7 +8468,7 @@
         <v>88</v>
       </c>
       <c r="K76" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L76" s="10" t="s">
         <v>503</v>
@@ -8507,7 +8516,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
         <v>120</v>
       </c>
@@ -8527,7 +8536,7 @@
         <v>4</v>
       </c>
       <c r="H77" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I77" t="s">
         <v>63</v>
@@ -8536,7 +8545,7 @@
         <v>88</v>
       </c>
       <c r="K77" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L77" s="10" t="s">
         <v>561</v>
@@ -8572,7 +8581,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
         <v>122</v>
       </c>
@@ -8592,7 +8601,7 @@
         <v>4</v>
       </c>
       <c r="H78" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I78" t="s">
         <v>63</v>
@@ -8601,7 +8610,7 @@
         <v>88</v>
       </c>
       <c r="K78" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L78" s="10" t="s">
         <v>498</v>
@@ -8649,7 +8658,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
         <v>126</v>
       </c>
@@ -8669,7 +8678,7 @@
         <v>4</v>
       </c>
       <c r="H79" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="I79" t="s">
         <v>63</v>
@@ -8678,7 +8687,7 @@
         <v>88</v>
       </c>
       <c r="K79" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L79" s="10" t="s">
         <v>498</v>
@@ -8726,7 +8735,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
         <v>129</v>
       </c>
@@ -8746,7 +8755,7 @@
         <v>4</v>
       </c>
       <c r="H80" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="I80" t="s">
         <v>63</v>
@@ -8755,7 +8764,7 @@
         <v>88</v>
       </c>
       <c r="K80" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L80" s="10" t="s">
         <v>498</v>
@@ -8806,7 +8815,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>132</v>
       </c>
@@ -8826,7 +8835,7 @@
         <v>4</v>
       </c>
       <c r="H81" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I81" t="s">
         <v>63</v>
@@ -8835,7 +8844,7 @@
         <v>88</v>
       </c>
       <c r="K81" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L81" s="10" t="s">
         <v>498</v>
@@ -8886,7 +8895,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
         <v>135</v>
       </c>
@@ -8906,7 +8915,7 @@
         <v>4</v>
       </c>
       <c r="H82" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I82" t="s">
         <v>63</v>
@@ -8915,7 +8924,7 @@
         <v>88</v>
       </c>
       <c r="K82" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L82" s="10" t="s">
         <v>498</v>
@@ -8963,7 +8972,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
         <v>138</v>
       </c>
@@ -8983,7 +8992,7 @@
         <v>4</v>
       </c>
       <c r="H83" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I83" t="s">
         <v>63</v>
@@ -8992,7 +9001,7 @@
         <v>88</v>
       </c>
       <c r="K83" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L83" s="10" t="s">
         <v>498</v>
@@ -9043,7 +9052,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>141</v>
       </c>
@@ -9063,7 +9072,7 @@
         <v>4</v>
       </c>
       <c r="H84" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I84" t="s">
         <v>63</v>
@@ -9072,7 +9081,7 @@
         <v>88</v>
       </c>
       <c r="K84" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L84" s="10" t="s">
         <v>498</v>
@@ -9120,7 +9129,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
         <v>144</v>
       </c>
@@ -9140,7 +9149,7 @@
         <v>4</v>
       </c>
       <c r="H85" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I85" t="s">
         <v>63</v>
@@ -9149,7 +9158,7 @@
         <v>88</v>
       </c>
       <c r="K85" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L85" s="10" t="s">
         <v>498</v>
@@ -9197,7 +9206,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>147</v>
       </c>
@@ -9217,7 +9226,7 @@
         <v>4</v>
       </c>
       <c r="H86" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I86" t="s">
         <v>63</v>
@@ -9226,7 +9235,7 @@
         <v>88</v>
       </c>
       <c r="K86" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L86" s="10" t="s">
         <v>498</v>
@@ -9274,7 +9283,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>150</v>
       </c>
@@ -9294,7 +9303,7 @@
         <v>4</v>
       </c>
       <c r="H87" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I87" t="s">
         <v>63</v>
@@ -9303,7 +9312,7 @@
         <v>88</v>
       </c>
       <c r="K87" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L87" s="10" t="s">
         <v>498</v>
@@ -9351,7 +9360,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>153</v>
       </c>
@@ -9371,7 +9380,7 @@
         <v>4</v>
       </c>
       <c r="H88" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I88" t="s">
         <v>63</v>
@@ -9380,7 +9389,7 @@
         <v>88</v>
       </c>
       <c r="K88" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L88" s="10" t="s">
         <v>498</v>
@@ -9428,7 +9437,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
         <v>156</v>
       </c>
@@ -9448,7 +9457,7 @@
         <v>4</v>
       </c>
       <c r="H89" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I89" t="s">
         <v>63</v>
@@ -9457,7 +9466,7 @@
         <v>88</v>
       </c>
       <c r="K89" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L89" s="10" t="s">
         <v>498</v>
@@ -9508,7 +9517,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
         <v>159</v>
       </c>
@@ -9528,7 +9537,7 @@
         <v>4</v>
       </c>
       <c r="H90" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I90" t="s">
         <v>63</v>
@@ -9537,7 +9546,7 @@
         <v>88</v>
       </c>
       <c r="K90" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L90" s="10" t="s">
         <v>498</v>
@@ -9585,7 +9594,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
         <v>161</v>
       </c>
@@ -9605,7 +9614,7 @@
         <v>4</v>
       </c>
       <c r="H91" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="I91" t="s">
         <v>63</v>
@@ -9614,7 +9623,7 @@
         <v>88</v>
       </c>
       <c r="K91" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="L91" s="10" t="s">
         <v>498</v>
@@ -9665,7 +9674,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="92" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
         <v>232</v>
       </c>
@@ -9686,7 +9695,7 @@
         <v>4</v>
       </c>
       <c r="H92" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="I92" s="1" t="s">
         <v>7</v>
@@ -9695,7 +9704,7 @@
         <v>8</v>
       </c>
       <c r="K92" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L92" s="10" t="s">
         <v>498</v>
@@ -9743,7 +9752,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="93" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
         <v>236</v>
       </c>
@@ -9764,7 +9773,7 @@
         <v>4</v>
       </c>
       <c r="H93" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>7</v>
@@ -9773,7 +9782,7 @@
         <v>8</v>
       </c>
       <c r="K93" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L93" s="10" t="s">
         <v>498</v>
@@ -9824,7 +9833,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="94" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>240</v>
       </c>
@@ -9845,7 +9854,7 @@
         <v>4</v>
       </c>
       <c r="H94" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="I94" s="1" t="s">
         <v>7</v>
@@ -9854,7 +9863,7 @@
         <v>8</v>
       </c>
       <c r="K94" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L94" s="10" t="s">
         <v>498</v>
@@ -9905,7 +9914,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="95" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
         <v>248</v>
       </c>
@@ -9926,7 +9935,7 @@
         <v>4</v>
       </c>
       <c r="H95" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="I95" s="1" t="s">
         <v>7</v>
@@ -9935,7 +9944,7 @@
         <v>8</v>
       </c>
       <c r="K95" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L95" s="10" t="s">
         <v>498</v>
@@ -9980,7 +9989,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
         <v>255</v>
       </c>
@@ -10001,7 +10010,7 @@
         <v>4</v>
       </c>
       <c r="H96" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>7</v>
@@ -10010,7 +10019,7 @@
         <v>8</v>
       </c>
       <c r="K96" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L96" s="10" t="s">
         <v>498</v>
@@ -10058,7 +10067,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="97" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
         <v>260</v>
       </c>
@@ -10079,7 +10088,7 @@
         <v>4</v>
       </c>
       <c r="H97" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>7</v>
@@ -10088,7 +10097,7 @@
         <v>8</v>
       </c>
       <c r="K97" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L97" s="10" t="s">
         <v>498</v>
@@ -10136,7 +10145,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="98" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>263</v>
       </c>
@@ -10157,7 +10166,7 @@
         <v>4</v>
       </c>
       <c r="H98" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="I98" s="1" t="s">
         <v>7</v>
@@ -10166,7 +10175,7 @@
         <v>8</v>
       </c>
       <c r="K98" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L98" s="10" t="s">
         <v>498</v>
@@ -10214,7 +10223,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="99" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>271</v>
       </c>
@@ -10235,7 +10244,7 @@
         <v>4</v>
       </c>
       <c r="H99" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="I99" s="1" t="s">
         <v>7</v>
@@ -10244,7 +10253,7 @@
         <v>8</v>
       </c>
       <c r="K99" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L99" s="10" t="s">
         <v>498</v>
@@ -10289,10 +10298,10 @@
         <v>272</v>
       </c>
       <c r="AB99" t="s">
-        <v>594</v>
-      </c>
-    </row>
-    <row r="100" spans="1:29" x14ac:dyDescent="0.2">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="100" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>274</v>
       </c>
@@ -10313,7 +10322,7 @@
         <v>4</v>
       </c>
       <c r="H100" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="I100" s="1" t="s">
         <v>7</v>
@@ -10322,7 +10331,7 @@
         <v>8</v>
       </c>
       <c r="K100" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L100" s="10" t="s">
         <v>498</v>
@@ -10367,7 +10376,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="101" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>279</v>
       </c>
@@ -10388,7 +10397,7 @@
         <v>4</v>
       </c>
       <c r="H101" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I101" s="1" t="s">
         <v>7</v>
@@ -10397,7 +10406,7 @@
         <v>8</v>
       </c>
       <c r="K101" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="L101" s="10" t="s">
         <v>498</v>
@@ -10442,7 +10451,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="102" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>282</v>
       </c>
@@ -10463,7 +10472,7 @@
         <v>4</v>
       </c>
       <c r="H102" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>7</v>
@@ -10472,7 +10481,7 @@
         <v>8</v>
       </c>
       <c r="K102" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L102" s="10" t="s">
         <v>498</v>
@@ -10520,7 +10529,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="103" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
         <v>289</v>
       </c>
@@ -10541,7 +10550,7 @@
         <v>4</v>
       </c>
       <c r="H103" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I103" s="1" t="s">
         <v>7</v>
@@ -10550,7 +10559,7 @@
         <v>8</v>
       </c>
       <c r="K103" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L103" s="10" t="s">
         <v>498</v>
@@ -10598,7 +10607,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="104" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
         <v>307</v>
       </c>
@@ -10619,7 +10628,7 @@
         <v>4</v>
       </c>
       <c r="H104" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I104" s="1" t="s">
         <v>7</v>
@@ -10628,7 +10637,7 @@
         <v>8</v>
       </c>
       <c r="K104" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L104" s="10" t="s">
         <v>498</v>
@@ -10679,7 +10688,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="105" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>324</v>
       </c>
@@ -10700,7 +10709,7 @@
         <v>4</v>
       </c>
       <c r="H105" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I105" s="1" t="s">
         <v>7</v>
@@ -10709,7 +10718,7 @@
         <v>8</v>
       </c>
       <c r="K105" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L105" s="10" t="s">
         <v>561</v>
@@ -10751,7 +10760,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="106" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>332</v>
       </c>
@@ -10772,7 +10781,7 @@
         <v>4</v>
       </c>
       <c r="H106" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>7</v>
@@ -10781,7 +10790,7 @@
         <v>8</v>
       </c>
       <c r="K106" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L106" s="10" t="s">
         <v>498</v>
@@ -10826,7 +10835,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="107" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>347</v>
       </c>
@@ -10847,7 +10856,7 @@
         <v>4</v>
       </c>
       <c r="H107" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="I107" s="1" t="s">
         <v>7</v>
@@ -10856,7 +10865,7 @@
         <v>8</v>
       </c>
       <c r="K107" t="s">
-        <v>597</v>
+        <v>744</v>
       </c>
       <c r="L107" s="10" t="s">
         <v>498</v>
@@ -10907,7 +10916,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="108" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
         <v>353</v>
       </c>
@@ -10928,7 +10937,7 @@
         <v>4</v>
       </c>
       <c r="H108" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>7</v>
@@ -10937,7 +10946,7 @@
         <v>8</v>
       </c>
       <c r="K108" t="s">
-        <v>597</v>
+        <v>744</v>
       </c>
       <c r="L108" s="10" t="s">
         <v>498</v>
@@ -10985,7 +10994,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="109" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
         <v>244</v>
       </c>
@@ -11006,7 +11015,7 @@
         <v>4</v>
       </c>
       <c r="H109" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="I109" s="1" t="s">
         <v>7</v>
@@ -11015,7 +11024,7 @@
         <v>8</v>
       </c>
       <c r="K109" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L109" s="10" t="s">
         <v>498</v>
@@ -11063,7 +11072,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="110" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
         <v>245</v>
       </c>
@@ -11084,7 +11093,7 @@
         <v>4</v>
       </c>
       <c r="H110" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="I110" s="1" t="s">
         <v>7</v>
@@ -11093,7 +11102,7 @@
         <v>8</v>
       </c>
       <c r="K110" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L110" s="10" t="s">
         <v>498</v>
@@ -11141,7 +11150,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="111" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
         <v>249</v>
       </c>
@@ -11162,7 +11171,7 @@
         <v>4</v>
       </c>
       <c r="H111" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="I111" s="1" t="s">
         <v>7</v>
@@ -11171,7 +11180,7 @@
         <v>8</v>
       </c>
       <c r="K111" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="L111" s="10" t="s">
         <v>498</v>
@@ -11219,7 +11228,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="112" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
         <v>252</v>
       </c>
@@ -11240,7 +11249,7 @@
         <v>4</v>
       </c>
       <c r="H112" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>7</v>
@@ -11249,7 +11258,7 @@
         <v>8</v>
       </c>
       <c r="K112" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L112" s="10" t="s">
         <v>498</v>
@@ -11297,7 +11306,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="113" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>258</v>
       </c>
@@ -11318,7 +11327,7 @@
         <v>4</v>
       </c>
       <c r="H113" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="I113" s="1" t="s">
         <v>7</v>
@@ -11327,7 +11336,7 @@
         <v>8</v>
       </c>
       <c r="K113" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L113" s="10" t="s">
         <v>498</v>
@@ -11375,7 +11384,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="114" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
         <v>261</v>
       </c>
@@ -11396,7 +11405,7 @@
         <v>4</v>
       </c>
       <c r="H114" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="I114" s="1" t="s">
         <v>7</v>
@@ -11405,7 +11414,7 @@
         <v>8</v>
       </c>
       <c r="K114" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L114" s="10" t="s">
         <v>498</v>
@@ -11453,7 +11462,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
         <v>265</v>
       </c>
@@ -11474,7 +11483,7 @@
         <v>4</v>
       </c>
       <c r="H115" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="I115" s="1" t="s">
         <v>7</v>
@@ -11483,7 +11492,7 @@
         <v>8</v>
       </c>
       <c r="K115" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L115" s="10" t="s">
         <v>498</v>
@@ -11531,7 +11540,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
         <v>268</v>
       </c>
@@ -11552,7 +11561,7 @@
         <v>4</v>
       </c>
       <c r="H116" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="I116" s="1" t="s">
         <v>7</v>
@@ -11561,7 +11570,7 @@
         <v>8</v>
       </c>
       <c r="K116" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L116" s="10" t="s">
         <v>498</v>
@@ -11609,7 +11618,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
         <v>273</v>
       </c>
@@ -11630,7 +11639,7 @@
         <v>4</v>
       </c>
       <c r="H117" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="I117" s="1" t="s">
         <v>7</v>
@@ -11639,7 +11648,7 @@
         <v>8</v>
       </c>
       <c r="K117" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L117" s="10" t="s">
         <v>498</v>
@@ -11684,7 +11693,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="118" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
         <v>275</v>
       </c>
@@ -11705,7 +11714,7 @@
         <v>4</v>
       </c>
       <c r="H118" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="I118" s="1" t="s">
         <v>7</v>
@@ -11714,7 +11723,7 @@
         <v>8</v>
       </c>
       <c r="K118" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L118" s="10" t="s">
         <v>498</v>
@@ -11759,7 +11768,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
         <v>276</v>
       </c>
@@ -11780,7 +11789,7 @@
         <v>4</v>
       </c>
       <c r="H119" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="I119" s="1" t="s">
         <v>7</v>
@@ -11789,7 +11798,7 @@
         <v>8</v>
       </c>
       <c r="K119" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L119" s="10" t="s">
         <v>498</v>
@@ -11834,7 +11843,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
         <v>280</v>
       </c>
@@ -11855,7 +11864,7 @@
         <v>4</v>
       </c>
       <c r="H120" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="I120" s="1" t="s">
         <v>7</v>
@@ -11864,7 +11873,7 @@
         <v>8</v>
       </c>
       <c r="K120" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L120" s="10" t="s">
         <v>498</v>
@@ -11912,10 +11921,10 @@
         <v>281</v>
       </c>
       <c r="AC120" t="s">
-        <v>593</v>
-      </c>
-    </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.2">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
         <v>286</v>
       </c>
@@ -11936,7 +11945,7 @@
         <v>4</v>
       </c>
       <c r="H121" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I121" s="1" t="s">
         <v>7</v>
@@ -11945,7 +11954,7 @@
         <v>8</v>
       </c>
       <c r="K121" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L121" s="10" t="s">
         <v>498</v>
@@ -11993,7 +12002,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="122" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
         <v>290</v>
       </c>
@@ -12014,7 +12023,7 @@
         <v>4</v>
       </c>
       <c r="H122" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="I122" s="1" t="s">
         <v>7</v>
@@ -12023,7 +12032,7 @@
         <v>8</v>
       </c>
       <c r="K122" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="L122" s="10" t="s">
         <v>498</v>
@@ -12074,7 +12083,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="123" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
         <v>292</v>
       </c>
@@ -12095,7 +12104,7 @@
         <v>4</v>
       </c>
       <c r="H123" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="I123" s="1" t="s">
         <v>7</v>
@@ -12104,7 +12113,7 @@
         <v>8</v>
       </c>
       <c r="K123" s="1" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="L123" s="10" t="s">
         <v>498</v>
@@ -12155,7 +12164,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="124" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
         <v>295</v>
       </c>
@@ -12176,7 +12185,7 @@
         <v>4</v>
       </c>
       <c r="H124" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="I124" s="1" t="s">
         <v>7</v>
@@ -12185,7 +12194,7 @@
         <v>8</v>
       </c>
       <c r="K124" s="1" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="L124" s="10" t="s">
         <v>498</v>
@@ -12236,7 +12245,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
         <v>298</v>
       </c>
@@ -12257,7 +12266,7 @@
         <v>4</v>
       </c>
       <c r="H125" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I125" s="1" t="s">
         <v>302</v>
@@ -12266,7 +12275,7 @@
         <v>8</v>
       </c>
       <c r="K125" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L125" s="10" t="s">
         <v>498</v>
@@ -12317,7 +12326,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
         <v>303</v>
       </c>
@@ -12338,7 +12347,7 @@
         <v>4</v>
       </c>
       <c r="H126" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="I126" s="1" t="s">
         <v>302</v>
@@ -12347,7 +12356,7 @@
         <v>8</v>
       </c>
       <c r="K126" s="1" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="L126" s="10" t="s">
         <v>498</v>
@@ -12398,7 +12407,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="127" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
         <v>309</v>
       </c>
@@ -12419,7 +12428,7 @@
         <v>4</v>
       </c>
       <c r="H127" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="I127" s="1" t="s">
         <v>302</v>
@@ -12428,7 +12437,7 @@
         <v>8</v>
       </c>
       <c r="K127" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L127" s="10" t="s">
         <v>498</v>
@@ -12476,7 +12485,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="128" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
         <v>311</v>
       </c>
@@ -12497,7 +12506,7 @@
         <v>4</v>
       </c>
       <c r="H128" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="I128" s="1" t="s">
         <v>302</v>
@@ -12506,7 +12515,7 @@
         <v>8</v>
       </c>
       <c r="K128" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L128" s="10" t="s">
         <v>498</v>
@@ -12554,7 +12563,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="129" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
         <v>314</v>
       </c>
@@ -12575,7 +12584,7 @@
         <v>4</v>
       </c>
       <c r="H129" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="I129" s="1" t="s">
         <v>302</v>
@@ -12584,7 +12593,7 @@
         <v>8</v>
       </c>
       <c r="K129" s="1" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="L129" s="10" t="s">
         <v>498</v>
@@ -12632,7 +12641,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="130" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
         <v>317</v>
       </c>
@@ -12653,7 +12662,7 @@
         <v>4</v>
       </c>
       <c r="H130" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="I130" s="1" t="s">
         <v>302</v>
@@ -12662,7 +12671,7 @@
         <v>8</v>
       </c>
       <c r="K130" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L130" s="10" t="s">
         <v>498</v>
@@ -12710,7 +12719,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="131" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
         <v>321</v>
       </c>
@@ -12731,7 +12740,7 @@
         <v>4</v>
       </c>
       <c r="H131" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="I131" s="1" t="s">
         <v>302</v>
@@ -12740,7 +12749,7 @@
         <v>8</v>
       </c>
       <c r="K131" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L131" s="10" t="s">
         <v>498</v>
@@ -12791,7 +12800,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="132" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
         <v>327</v>
       </c>
@@ -12812,7 +12821,7 @@
         <v>4</v>
       </c>
       <c r="H132" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="I132" s="1" t="s">
         <v>302</v>
@@ -12821,7 +12830,7 @@
         <v>8</v>
       </c>
       <c r="K132" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L132" s="10" t="s">
         <v>498</v>
@@ -12872,7 +12881,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
         <v>329</v>
       </c>
@@ -12893,7 +12902,7 @@
         <v>4</v>
       </c>
       <c r="H133" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="I133" s="1" t="s">
         <v>302</v>
@@ -12902,7 +12911,7 @@
         <v>8</v>
       </c>
       <c r="K133" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L133" s="10" t="s">
         <v>503</v>
@@ -12953,7 +12962,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
         <v>335</v>
       </c>
@@ -12974,7 +12983,7 @@
         <v>4</v>
       </c>
       <c r="H134" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>302</v>
@@ -12983,7 +12992,7 @@
         <v>8</v>
       </c>
       <c r="K134" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L134" s="10" t="s">
         <v>498</v>
@@ -13031,7 +13040,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
         <v>338</v>
       </c>
@@ -13052,7 +13061,7 @@
         <v>4</v>
       </c>
       <c r="H135" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="I135" s="1" t="s">
         <v>302</v>
@@ -13061,7 +13070,7 @@
         <v>8</v>
       </c>
       <c r="K135" s="1" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="L135" s="10" t="s">
         <v>498</v>
@@ -13109,7 +13118,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
         <v>341</v>
       </c>
@@ -13130,7 +13139,7 @@
         <v>4</v>
       </c>
       <c r="H136" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I136" s="1" t="s">
         <v>302</v>
@@ -13190,7 +13199,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="137" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
         <v>345</v>
       </c>
@@ -13211,7 +13220,7 @@
         <v>4</v>
       </c>
       <c r="H137" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="I137" s="1" t="s">
         <v>302</v>
@@ -13220,7 +13229,7 @@
         <v>8</v>
       </c>
       <c r="K137" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L137" s="10" t="s">
         <v>498</v>
@@ -13268,7 +13277,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="138" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
         <v>351</v>
       </c>
@@ -13289,7 +13298,7 @@
         <v>4</v>
       </c>
       <c r="H138" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="I138" s="1" t="s">
         <v>302</v>
@@ -13298,7 +13307,7 @@
         <v>8</v>
       </c>
       <c r="K138" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L138" s="10" t="s">
         <v>498</v>
@@ -13349,7 +13358,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="139" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
         <v>355</v>
       </c>
@@ -13370,7 +13379,7 @@
         <v>4</v>
       </c>
       <c r="H139" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I139" s="1" t="s">
         <v>302</v>
@@ -13379,7 +13388,7 @@
         <v>8</v>
       </c>
       <c r="K139" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L139" s="10" t="s">
         <v>498</v>
@@ -13427,7 +13436,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="140" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
         <v>356</v>
       </c>
@@ -13448,7 +13457,7 @@
         <v>4</v>
       </c>
       <c r="H140" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="I140" s="1" t="s">
         <v>302</v>
@@ -13457,7 +13466,7 @@
         <v>8</v>
       </c>
       <c r="K140" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L140" s="10" t="s">
         <v>498</v>
@@ -13505,7 +13514,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="141" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
         <v>357</v>
       </c>
@@ -13526,7 +13535,7 @@
         <v>4</v>
       </c>
       <c r="H141" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="I141" s="1" t="s">
         <v>302</v>
@@ -13535,7 +13544,7 @@
         <v>8</v>
       </c>
       <c r="K141" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L141" s="10" t="s">
         <v>498</v>
@@ -13583,7 +13592,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="142" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
         <v>358</v>
       </c>
@@ -13604,7 +13613,7 @@
         <v>4</v>
       </c>
       <c r="H142" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="I142" s="1" t="s">
         <v>302</v>
@@ -13613,7 +13622,7 @@
         <v>8</v>
       </c>
       <c r="K142" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L142" s="10" t="s">
         <v>498</v>
@@ -13661,7 +13670,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="143" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
         <v>360</v>
       </c>
@@ -13682,7 +13691,7 @@
         <v>4</v>
       </c>
       <c r="H143" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="I143" s="1" t="s">
         <v>302</v>
@@ -13691,7 +13700,7 @@
         <v>8</v>
       </c>
       <c r="K143" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L143" s="10" t="s">
         <v>498</v>
@@ -13739,7 +13748,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="144" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
         <v>362</v>
       </c>
@@ -13760,7 +13769,7 @@
         <v>4</v>
       </c>
       <c r="H144" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="I144" s="1" t="s">
         <v>302</v>
@@ -13769,7 +13778,7 @@
         <v>8</v>
       </c>
       <c r="K144" s="1" t="s">
-        <v>583</v>
+        <v>741</v>
       </c>
       <c r="L144" s="10" t="s">
         <v>498</v>
@@ -13817,7 +13826,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="145" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
         <v>364</v>
       </c>
@@ -13838,7 +13847,7 @@
         <v>4</v>
       </c>
       <c r="H145" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="I145" s="1" t="s">
         <v>302</v>
@@ -13847,7 +13856,7 @@
         <v>8</v>
       </c>
       <c r="K145" s="1" t="s">
-        <v>583</v>
+        <v>742</v>
       </c>
       <c r="L145" s="10" t="s">
         <v>498</v>
@@ -13895,7 +13904,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="146" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
         <v>366</v>
       </c>
@@ -13916,7 +13925,7 @@
         <v>4</v>
       </c>
       <c r="H146" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="I146" s="1" t="s">
         <v>302</v>
@@ -13925,7 +13934,7 @@
         <v>8</v>
       </c>
       <c r="K146" s="1" t="s">
-        <v>583</v>
+        <v>742</v>
       </c>
       <c r="L146" s="10" t="s">
         <v>498</v>
@@ -13973,7 +13982,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="147" spans="1:29" ht="15" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
         <v>369</v>
       </c>
@@ -13994,7 +14003,7 @@
         <v>4</v>
       </c>
       <c r="H147" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="I147" s="1" t="s">
         <v>302</v>
@@ -14003,7 +14012,7 @@
         <v>8</v>
       </c>
       <c r="K147" s="1" t="s">
-        <v>583</v>
+        <v>742</v>
       </c>
       <c r="L147" s="10" t="s">
         <v>498</v>
@@ -14054,7 +14063,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="148" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
         <v>371</v>
       </c>
@@ -14075,7 +14084,7 @@
         <v>4</v>
       </c>
       <c r="H148" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="I148" s="1" t="s">
         <v>302</v>
@@ -14084,7 +14093,7 @@
         <v>8</v>
       </c>
       <c r="K148" s="1" t="s">
-        <v>583</v>
+        <v>742</v>
       </c>
       <c r="L148" s="10" t="s">
         <v>498</v>
@@ -14132,7 +14141,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="149" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
         <v>372</v>
       </c>
@@ -14153,7 +14162,7 @@
         <v>4</v>
       </c>
       <c r="H149" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>302</v>
@@ -14162,7 +14171,7 @@
         <v>8</v>
       </c>
       <c r="K149" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L149" s="10" t="s">
         <v>498</v>
@@ -14210,7 +14219,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="150" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>374</v>
       </c>
@@ -14231,7 +14240,7 @@
         <v>4</v>
       </c>
       <c r="H150" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I150" s="1" t="s">
         <v>302</v>
@@ -14240,7 +14249,7 @@
         <v>8</v>
       </c>
       <c r="K150" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L150" s="10" t="s">
         <v>498</v>
@@ -14288,7 +14297,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="151" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
         <v>376</v>
       </c>
@@ -14309,7 +14318,7 @@
         <v>4</v>
       </c>
       <c r="H151" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>302</v>
@@ -14318,7 +14327,7 @@
         <v>8</v>
       </c>
       <c r="K151" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L151" s="10" t="s">
         <v>498</v>
@@ -14369,7 +14378,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="152" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
         <v>379</v>
       </c>
@@ -14390,7 +14399,7 @@
         <v>4</v>
       </c>
       <c r="H152" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I152" s="1" t="s">
         <v>302</v>
@@ -14399,7 +14408,7 @@
         <v>8</v>
       </c>
       <c r="K152" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L152" s="10" t="s">
         <v>498</v>
@@ -14447,7 +14456,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="153" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
         <v>381</v>
       </c>
@@ -14468,7 +14477,7 @@
         <v>4</v>
       </c>
       <c r="H153" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="I153" s="1" t="s">
         <v>302</v>
@@ -14477,7 +14486,7 @@
         <v>8</v>
       </c>
       <c r="K153" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L153" s="10" t="s">
         <v>498</v>
@@ -14525,7 +14534,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="154" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
         <v>382</v>
       </c>
@@ -14546,7 +14555,7 @@
         <v>4</v>
       </c>
       <c r="H154" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I154" s="1" t="s">
         <v>302</v>
@@ -14555,7 +14564,7 @@
         <v>8</v>
       </c>
       <c r="K154" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L154" s="10" t="s">
         <v>498</v>
@@ -14606,7 +14615,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="155" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
         <v>385</v>
       </c>
@@ -14627,7 +14636,7 @@
         <v>4</v>
       </c>
       <c r="H155" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="I155" s="1" t="s">
         <v>302</v>
@@ -14636,7 +14645,7 @@
         <v>8</v>
       </c>
       <c r="K155" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L155" s="10" t="s">
         <v>498</v>
@@ -14684,7 +14693,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="156" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
         <v>386</v>
       </c>
@@ -14705,7 +14714,7 @@
         <v>4</v>
       </c>
       <c r="H156" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I156" s="1" t="s">
         <v>302</v>
@@ -14714,7 +14723,7 @@
         <v>8</v>
       </c>
       <c r="K156" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L156" s="10" t="s">
         <v>498</v>
@@ -14762,7 +14771,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="157" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
         <v>388</v>
       </c>
@@ -14783,7 +14792,7 @@
         <v>4</v>
       </c>
       <c r="H157" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I157" s="1" t="s">
         <v>302</v>
@@ -14792,7 +14801,7 @@
         <v>8</v>
       </c>
       <c r="K157" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L157" s="10" t="s">
         <v>498</v>
@@ -14840,7 +14849,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="158" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
         <v>390</v>
       </c>
@@ -14861,7 +14870,7 @@
         <v>4</v>
       </c>
       <c r="H158" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="I158" s="1" t="s">
         <v>302</v>
@@ -14870,7 +14879,7 @@
         <v>8</v>
       </c>
       <c r="K158" s="1" t="s">
-        <v>583</v>
+        <v>743</v>
       </c>
       <c r="L158" s="10" t="s">
         <v>498</v>
@@ -14921,7 +14930,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="159" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
         <v>167</v>
       </c>
@@ -14942,7 +14951,7 @@
         <v>4</v>
       </c>
       <c r="H159" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I159" s="1" t="s">
         <v>7</v>
@@ -14951,7 +14960,7 @@
         <v>8</v>
       </c>
       <c r="K159" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L159" s="10" t="s">
         <v>498</v>
@@ -14999,7 +15008,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="160" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
         <v>173</v>
       </c>
@@ -15020,7 +15029,7 @@
         <v>4</v>
       </c>
       <c r="H160" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I160" s="1" t="s">
         <v>7</v>
@@ -15029,7 +15038,7 @@
         <v>8</v>
       </c>
       <c r="K160" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L160" s="10" t="s">
         <v>498</v>
@@ -15080,7 +15089,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
         <v>174</v>
       </c>
@@ -15101,7 +15110,7 @@
         <v>4</v>
       </c>
       <c r="H161" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I161" s="1" t="s">
         <v>7</v>
@@ -15110,7 +15119,7 @@
         <v>8</v>
       </c>
       <c r="K161" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L161" s="10" t="s">
         <v>498</v>
@@ -15161,7 +15170,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="162" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
         <v>177</v>
       </c>
@@ -15182,7 +15191,7 @@
         <v>4</v>
       </c>
       <c r="H162" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I162" s="1" t="s">
         <v>7</v>
@@ -15191,7 +15200,7 @@
         <v>8</v>
       </c>
       <c r="K162" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L162" s="10" t="s">
         <v>498</v>
@@ -15242,7 +15251,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="163" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
         <v>179</v>
       </c>
@@ -15263,7 +15272,7 @@
         <v>4</v>
       </c>
       <c r="H163" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I163" s="1" t="s">
         <v>7</v>
@@ -15272,7 +15281,7 @@
         <v>8</v>
       </c>
       <c r="K163" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L163" s="10" t="s">
         <v>498</v>
@@ -15323,7 +15332,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="164" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
         <v>182</v>
       </c>
@@ -15344,7 +15353,7 @@
         <v>4</v>
       </c>
       <c r="H164" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I164" s="1" t="s">
         <v>7</v>
@@ -15353,7 +15362,7 @@
         <v>8</v>
       </c>
       <c r="K164" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L164" s="10" t="s">
         <v>498</v>
@@ -15404,7 +15413,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="165" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
         <v>48</v>
       </c>
@@ -15424,7 +15433,7 @@
         <v>4</v>
       </c>
       <c r="H165" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I165" t="s">
         <v>7</v>
@@ -15433,7 +15442,7 @@
         <v>8</v>
       </c>
       <c r="K165" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L165" s="10" t="s">
         <v>498</v>
@@ -15454,7 +15463,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="166" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
         <v>49</v>
       </c>
@@ -15474,7 +15483,7 @@
         <v>4</v>
       </c>
       <c r="H166" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I166" s="7" t="s">
         <v>86</v>
@@ -15483,7 +15492,7 @@
         <v>86</v>
       </c>
       <c r="K166" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L166" s="10" t="s">
         <v>498</v>
@@ -15501,7 +15510,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="167" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
         <v>50</v>
       </c>
@@ -15521,7 +15530,7 @@
         <v>4</v>
       </c>
       <c r="H167" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I167" s="7" t="s">
         <v>86</v>
@@ -15530,7 +15539,7 @@
         <v>86</v>
       </c>
       <c r="K167" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L167" s="10" t="s">
         <v>498</v>
@@ -15548,7 +15557,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="168" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
         <v>51</v>
       </c>
@@ -15568,7 +15577,7 @@
         <v>4</v>
       </c>
       <c r="H168" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I168" s="7" t="s">
         <v>86</v>
@@ -15577,7 +15586,7 @@
         <v>86</v>
       </c>
       <c r="K168" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L168" s="10" t="s">
         <v>498</v>
@@ -15595,7 +15604,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="169" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
         <v>52</v>
       </c>
@@ -15615,7 +15624,7 @@
         <v>4</v>
       </c>
       <c r="H169" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I169" s="7" t="s">
         <v>86</v>
@@ -15624,7 +15633,7 @@
         <v>86</v>
       </c>
       <c r="K169" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L169" s="10" t="s">
         <v>498</v>
@@ -15642,7 +15651,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="170" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
         <v>53</v>
       </c>
@@ -15662,7 +15671,7 @@
         <v>4</v>
       </c>
       <c r="H170" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I170" s="7" t="s">
         <v>86</v>
@@ -15671,7 +15680,7 @@
         <v>86</v>
       </c>
       <c r="K170" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L170" s="10" t="s">
         <v>498</v>
@@ -15689,7 +15698,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="171" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
         <v>54</v>
       </c>
@@ -15709,7 +15718,7 @@
         <v>4</v>
       </c>
       <c r="H171" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I171" s="7" t="s">
         <v>86</v>
@@ -15718,7 +15727,7 @@
         <v>86</v>
       </c>
       <c r="K171" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L171" s="10" t="s">
         <v>498</v>
@@ -15736,7 +15745,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="172" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
         <v>55</v>
       </c>
@@ -15756,7 +15765,7 @@
         <v>4</v>
       </c>
       <c r="H172" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I172" s="7" t="s">
         <v>86</v>
@@ -15765,7 +15774,7 @@
         <v>86</v>
       </c>
       <c r="K172" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L172" s="10" t="s">
         <v>498</v>
@@ -15783,7 +15792,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="173" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
         <v>56</v>
       </c>
@@ -15803,7 +15812,7 @@
         <v>4</v>
       </c>
       <c r="H173" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I173" s="7" t="s">
         <v>86</v>
@@ -15812,7 +15821,7 @@
         <v>86</v>
       </c>
       <c r="K173" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L173" s="10" t="s">
         <v>498</v>
@@ -15830,7 +15839,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="174" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
         <v>12</v>
       </c>
@@ -15850,7 +15859,7 @@
         <v>4</v>
       </c>
       <c r="H174" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I174" s="7" t="s">
         <v>86</v>
@@ -15859,7 +15868,7 @@
         <v>86</v>
       </c>
       <c r="K174" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="L174" s="10" t="s">
         <v>498</v>

</xml_diff>

<commit_message>
initial commit for decoding sequences code
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2372" uniqueCount="745">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="791">
   <si>
     <t>date</t>
   </si>
@@ -2265,6 +2265,144 @@
   </si>
   <si>
     <t>{'TBD','TBD','TBD','CA3'}</t>
+  </si>
+  <si>
+    <t>b0184_d191127</t>
+  </si>
+  <si>
+    <t>b0184_d191128</t>
+  </si>
+  <si>
+    <t>b0184_d191129</t>
+  </si>
+  <si>
+    <t>b0184_d191130</t>
+  </si>
+  <si>
+    <t>b0184_d191201</t>
+  </si>
+  <si>
+    <t>b0184_d191202</t>
+  </si>
+  <si>
+    <t>b0184_d191203</t>
+  </si>
+  <si>
+    <t>b0184_d191204</t>
+  </si>
+  <si>
+    <t>b0184_d191205</t>
+  </si>
+  <si>
+    <t>b0184_d191208</t>
+  </si>
+  <si>
+    <t>b0184_d191209</t>
+  </si>
+  <si>
+    <t>Shir</t>
+  </si>
+  <si>
+    <t>[6 1]</t>
+  </si>
+  <si>
+    <t>b0184_d191124</t>
+  </si>
+  <si>
+    <t>[1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1]</t>
+  </si>
+  <si>
+    <t>[1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16]</t>
+  </si>
+  <si>
+    <t>[59434546000 63082975000]</t>
+  </si>
+  <si>
+    <t>6m</t>
+  </si>
+  <si>
+    <t>b0184_d191125</t>
+  </si>
+  <si>
+    <t>[48776123000 51679735000]</t>
+  </si>
+  <si>
+    <t>b0184_d191126</t>
+  </si>
+  <si>
+    <t>[43714183000 46954719000]</t>
+  </si>
+  <si>
+    <t>[60145523000 66587858000]</t>
+  </si>
+  <si>
+    <t>120m</t>
+  </si>
+  <si>
+    <t>[42995335000 47390925000]</t>
+  </si>
+  <si>
+    <t>[48986037000 52928086000]</t>
+  </si>
+  <si>
+    <t>[33418817000 37379645000]</t>
+  </si>
+  <si>
+    <t>[47649050000 51464821000]</t>
+  </si>
+  <si>
+    <t>[43296150000 47443548000]</t>
+  </si>
+  <si>
+    <t>[42007182000 46353290000]</t>
+  </si>
+  <si>
+    <t>[53071661000 56916329000]</t>
+  </si>
+  <si>
+    <t>[45450019000 49507242000]</t>
+  </si>
+  <si>
+    <t>[58748740000 62174712000]</t>
+  </si>
+  <si>
+    <t>[42249148000 45446637000]</t>
+  </si>
+  <si>
+    <t>[nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;]</t>
+  </si>
+  <si>
+    <t>SpikeLog-64</t>
+  </si>
+  <si>
+    <t>one very short dark session - 1 flight only.</t>
+  </si>
+  <si>
+    <t>way to far end doing medium height, way back very low (0.5 m above the ground), mostly direct flights, landed only one time on the floor.</t>
+  </si>
+  <si>
+    <t>most flights are low, both way to and back at 0.5m above the ground or less.</t>
+  </si>
+  <si>
+    <t>the bat bumped its head in the ball and the floor in the first flight - maybe lost cells. most flights are low, both way to and back at 0.5m above the ground or less.</t>
+  </si>
+  <si>
+    <t>typical for this bat: flight upwards ehrn near Polygals</t>
+  </si>
+  <si>
+    <t>heavy raining during most of the session. The bat was a bit instress, but behavior was overall good</t>
+  </si>
+  <si>
+    <t>used sponged neurologger protector</t>
+  </si>
+  <si>
+    <t>used improvised protector with the upper bridge which is keeping the two sides of the protector from bending during hits in flight</t>
+  </si>
+  <si>
+    <t>used rgular protector with the "shelf" right to Omnetics connector when looking from the front is shaved out(because of the "flight artifacts)</t>
+  </si>
+  <si>
+    <t>the same as yesterday only that today with BeSpoon tag on the left side(near right hemisphere), instead of the battery(which is usually on the right).</t>
   </si>
 </sst>
 </file>
@@ -3016,13 +3154,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC174"/>
+  <dimension ref="A1:AC188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B146" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K108" sqref="K108"/>
+      <selection pane="bottomRight" activeCell="C177" sqref="C177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3032,7 +3170,7 @@
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="5.140625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="2" customWidth="1"/>
+    <col min="7" max="7" width="3" customWidth="1"/>
     <col min="8" max="8" width="26.42578125" customWidth="1"/>
     <col min="9" max="9" width="27.42578125" customWidth="1"/>
     <col min="10" max="10" width="8.5703125" customWidth="1"/>
@@ -3048,11 +3186,11 @@
     <col min="20" max="20" width="5.42578125" customWidth="1"/>
     <col min="21" max="21" width="19.42578125" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
-    <col min="23" max="23" width="3.7109375" customWidth="1"/>
+    <col min="23" max="23" width="5.85546875" customWidth="1"/>
     <col min="24" max="24" width="2.42578125" customWidth="1"/>
     <col min="25" max="25" width="3.7109375" customWidth="1"/>
     <col min="26" max="26" width="4.85546875" customWidth="1"/>
-    <col min="27" max="27" width="20" customWidth="1"/>
+    <col min="27" max="27" width="154.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="107.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -15883,6 +16021,1008 @@
         <v>9</v>
       </c>
       <c r="Z174" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="175" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A175" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B175" s="7">
+        <v>184</v>
+      </c>
+      <c r="C175" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D175" s="5">
+        <v>43793</v>
+      </c>
+      <c r="E175" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G175">
+        <v>16</v>
+      </c>
+      <c r="H175" t="s">
+        <v>779</v>
+      </c>
+      <c r="I175" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J175" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K175" s="7"/>
+      <c r="L175" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M175" s="9" t="s">
+        <v>761</v>
+      </c>
+      <c r="N175">
+        <v>1</v>
+      </c>
+      <c r="O175">
+        <v>1</v>
+      </c>
+      <c r="P175">
+        <v>0</v>
+      </c>
+      <c r="Q175">
+        <v>0</v>
+      </c>
+      <c r="R175">
+        <v>0</v>
+      </c>
+      <c r="S175">
+        <v>0</v>
+      </c>
+      <c r="T175" t="s">
+        <v>762</v>
+      </c>
+      <c r="U175" t="s">
+        <v>780</v>
+      </c>
+      <c r="V175">
+        <v>16</v>
+      </c>
+      <c r="W175">
+        <v>1624</v>
+      </c>
+      <c r="Z175" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="176" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="B176" s="7">
+        <v>184</v>
+      </c>
+      <c r="C176" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D176" s="5">
+        <v>43794</v>
+      </c>
+      <c r="E176" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G176">
+        <v>16</v>
+      </c>
+      <c r="H176" t="s">
+        <v>779</v>
+      </c>
+      <c r="I176" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J176" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K176" s="7"/>
+      <c r="L176" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M176" s="9" t="s">
+        <v>764</v>
+      </c>
+      <c r="N176">
+        <v>1</v>
+      </c>
+      <c r="O176">
+        <v>1</v>
+      </c>
+      <c r="P176">
+        <v>0</v>
+      </c>
+      <c r="Q176">
+        <v>0</v>
+      </c>
+      <c r="R176">
+        <v>0</v>
+      </c>
+      <c r="S176">
+        <v>0</v>
+      </c>
+      <c r="T176" t="s">
+        <v>762</v>
+      </c>
+      <c r="U176" t="s">
+        <v>780</v>
+      </c>
+      <c r="V176">
+        <v>16</v>
+      </c>
+      <c r="W176">
+        <v>1624</v>
+      </c>
+      <c r="Z176" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="177" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A177" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B177" s="7">
+        <v>184</v>
+      </c>
+      <c r="C177" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D177" s="5">
+        <v>43795</v>
+      </c>
+      <c r="E177" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G177">
+        <v>16</v>
+      </c>
+      <c r="H177" t="s">
+        <v>779</v>
+      </c>
+      <c r="I177" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J177" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K177" s="7"/>
+      <c r="L177" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M177" s="9" t="s">
+        <v>766</v>
+      </c>
+      <c r="N177">
+        <v>1</v>
+      </c>
+      <c r="O177">
+        <v>1</v>
+      </c>
+      <c r="P177">
+        <v>0</v>
+      </c>
+      <c r="Q177">
+        <v>0</v>
+      </c>
+      <c r="R177">
+        <v>0</v>
+      </c>
+      <c r="S177">
+        <v>0</v>
+      </c>
+      <c r="T177" t="s">
+        <v>762</v>
+      </c>
+      <c r="U177" t="s">
+        <v>780</v>
+      </c>
+      <c r="V177">
+        <v>16</v>
+      </c>
+      <c r="W177">
+        <v>1624</v>
+      </c>
+      <c r="Z177" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA177" t="s">
+        <v>781</v>
+      </c>
+    </row>
+    <row r="178" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B178" s="7">
+        <v>184</v>
+      </c>
+      <c r="C178" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D178" s="5">
+        <v>43796</v>
+      </c>
+      <c r="E178" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G178">
+        <v>16</v>
+      </c>
+      <c r="H178" t="s">
+        <v>779</v>
+      </c>
+      <c r="I178" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J178" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K178" s="7"/>
+      <c r="L178" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M178" s="9" t="s">
+        <v>767</v>
+      </c>
+      <c r="N178">
+        <v>1</v>
+      </c>
+      <c r="O178">
+        <v>1</v>
+      </c>
+      <c r="P178">
+        <v>0</v>
+      </c>
+      <c r="Q178">
+        <v>0</v>
+      </c>
+      <c r="R178">
+        <v>0</v>
+      </c>
+      <c r="S178">
+        <v>0</v>
+      </c>
+      <c r="T178" t="s">
+        <v>768</v>
+      </c>
+      <c r="U178" t="s">
+        <v>780</v>
+      </c>
+      <c r="V178">
+        <v>16</v>
+      </c>
+      <c r="W178">
+        <v>1624</v>
+      </c>
+      <c r="Z178" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA178" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="179" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A179" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="B179" s="7">
+        <v>184</v>
+      </c>
+      <c r="C179" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D179" s="5">
+        <v>43797</v>
+      </c>
+      <c r="E179" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G179">
+        <v>16</v>
+      </c>
+      <c r="H179" t="s">
+        <v>779</v>
+      </c>
+      <c r="I179" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J179" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K179" s="7"/>
+      <c r="L179" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M179" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="N179">
+        <v>1</v>
+      </c>
+      <c r="O179">
+        <v>1</v>
+      </c>
+      <c r="P179">
+        <v>0</v>
+      </c>
+      <c r="Q179">
+        <v>0</v>
+      </c>
+      <c r="R179">
+        <v>0</v>
+      </c>
+      <c r="S179">
+        <v>0</v>
+      </c>
+      <c r="T179" t="s">
+        <v>768</v>
+      </c>
+      <c r="U179" t="s">
+        <v>780</v>
+      </c>
+      <c r="V179">
+        <v>16</v>
+      </c>
+      <c r="W179">
+        <v>1624</v>
+      </c>
+      <c r="Z179" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA179" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="180" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>747</v>
+      </c>
+      <c r="B180" s="7">
+        <v>184</v>
+      </c>
+      <c r="C180" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D180" s="5">
+        <v>43798</v>
+      </c>
+      <c r="E180" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G180">
+        <v>16</v>
+      </c>
+      <c r="H180" t="s">
+        <v>779</v>
+      </c>
+      <c r="I180" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J180" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K180" s="7"/>
+      <c r="L180" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M180" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="N180">
+        <v>1</v>
+      </c>
+      <c r="O180">
+        <v>1</v>
+      </c>
+      <c r="P180">
+        <v>0</v>
+      </c>
+      <c r="Q180">
+        <v>0</v>
+      </c>
+      <c r="R180">
+        <v>0</v>
+      </c>
+      <c r="S180">
+        <v>0</v>
+      </c>
+      <c r="T180" t="s">
+        <v>768</v>
+      </c>
+      <c r="U180" t="s">
+        <v>780</v>
+      </c>
+      <c r="V180">
+        <v>16</v>
+      </c>
+      <c r="W180">
+        <v>1624</v>
+      </c>
+      <c r="Z180" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA180" t="s">
+        <v>783</v>
+      </c>
+      <c r="AB180" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="181" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B181" s="7">
+        <v>184</v>
+      </c>
+      <c r="C181" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D181" s="5">
+        <v>43799</v>
+      </c>
+      <c r="E181" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G181">
+        <v>16</v>
+      </c>
+      <c r="H181" t="s">
+        <v>779</v>
+      </c>
+      <c r="I181" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J181" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K181" s="7"/>
+      <c r="L181" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M181" s="9" t="s">
+        <v>771</v>
+      </c>
+      <c r="N181">
+        <v>1</v>
+      </c>
+      <c r="O181">
+        <v>1</v>
+      </c>
+      <c r="P181">
+        <v>0</v>
+      </c>
+      <c r="Q181">
+        <v>0</v>
+      </c>
+      <c r="R181">
+        <v>0</v>
+      </c>
+      <c r="S181">
+        <v>0</v>
+      </c>
+      <c r="T181" t="s">
+        <v>768</v>
+      </c>
+      <c r="U181" t="s">
+        <v>780</v>
+      </c>
+      <c r="V181">
+        <v>16</v>
+      </c>
+      <c r="W181">
+        <v>1624</v>
+      </c>
+      <c r="Z181" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA181" t="s">
+        <v>784</v>
+      </c>
+      <c r="AB181" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="182" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="B182" s="7">
+        <v>184</v>
+      </c>
+      <c r="C182" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D182" s="5">
+        <v>43800</v>
+      </c>
+      <c r="E182" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G182">
+        <v>16</v>
+      </c>
+      <c r="H182" t="s">
+        <v>779</v>
+      </c>
+      <c r="I182" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J182" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K182" s="7"/>
+      <c r="L182" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M182" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="N182">
+        <v>1</v>
+      </c>
+      <c r="O182">
+        <v>1</v>
+      </c>
+      <c r="P182">
+        <v>0</v>
+      </c>
+      <c r="Q182">
+        <v>0</v>
+      </c>
+      <c r="R182">
+        <v>0</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+      <c r="T182" t="s">
+        <v>768</v>
+      </c>
+      <c r="U182" t="s">
+        <v>780</v>
+      </c>
+      <c r="V182">
+        <v>16</v>
+      </c>
+      <c r="W182">
+        <v>1624</v>
+      </c>
+      <c r="Z182" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB182" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="183" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A183" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="B183" s="7">
+        <v>184</v>
+      </c>
+      <c r="C183" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D183" s="5">
+        <v>43801</v>
+      </c>
+      <c r="E183" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G183">
+        <v>16</v>
+      </c>
+      <c r="H183" t="s">
+        <v>779</v>
+      </c>
+      <c r="I183" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J183" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K183" s="7"/>
+      <c r="L183" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M183" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="O183">
+        <v>1</v>
+      </c>
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="Q183">
+        <v>0</v>
+      </c>
+      <c r="R183">
+        <v>0</v>
+      </c>
+      <c r="S183">
+        <v>0</v>
+      </c>
+      <c r="T183" t="s">
+        <v>768</v>
+      </c>
+      <c r="U183" t="s">
+        <v>780</v>
+      </c>
+      <c r="V183">
+        <v>16</v>
+      </c>
+      <c r="W183">
+        <v>1624</v>
+      </c>
+      <c r="Z183" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB183" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="184" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="B184" s="7">
+        <v>184</v>
+      </c>
+      <c r="C184" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D184" s="5">
+        <v>43802</v>
+      </c>
+      <c r="E184" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G184">
+        <v>16</v>
+      </c>
+      <c r="H184" t="s">
+        <v>779</v>
+      </c>
+      <c r="I184" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J184" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K184" s="7"/>
+      <c r="L184" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M184" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="N184">
+        <v>1</v>
+      </c>
+      <c r="O184">
+        <v>1</v>
+      </c>
+      <c r="P184">
+        <v>0</v>
+      </c>
+      <c r="Q184">
+        <v>0</v>
+      </c>
+      <c r="R184">
+        <v>0</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+      <c r="T184" t="s">
+        <v>768</v>
+      </c>
+      <c r="U184" t="s">
+        <v>780</v>
+      </c>
+      <c r="V184">
+        <v>16</v>
+      </c>
+      <c r="W184">
+        <v>1624</v>
+      </c>
+      <c r="Z184" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA184" t="s">
+        <v>785</v>
+      </c>
+      <c r="AB184" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="185" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A185" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B185" s="7">
+        <v>184</v>
+      </c>
+      <c r="C185" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D185" s="5">
+        <v>43803</v>
+      </c>
+      <c r="E185" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G185">
+        <v>16</v>
+      </c>
+      <c r="H185" t="s">
+        <v>779</v>
+      </c>
+      <c r="I185" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J185" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K185" s="7"/>
+      <c r="L185" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M185" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="N185">
+        <v>1</v>
+      </c>
+      <c r="O185">
+        <v>1</v>
+      </c>
+      <c r="P185">
+        <v>0</v>
+      </c>
+      <c r="Q185">
+        <v>0</v>
+      </c>
+      <c r="R185">
+        <v>0</v>
+      </c>
+      <c r="S185">
+        <v>0</v>
+      </c>
+      <c r="T185" t="s">
+        <v>768</v>
+      </c>
+      <c r="U185" t="s">
+        <v>780</v>
+      </c>
+      <c r="V185">
+        <v>16</v>
+      </c>
+      <c r="W185">
+        <v>1624</v>
+      </c>
+      <c r="Z185" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="186" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="B186" s="7">
+        <v>184</v>
+      </c>
+      <c r="C186" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D186" s="5">
+        <v>43804</v>
+      </c>
+      <c r="E186" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G186">
+        <v>16</v>
+      </c>
+      <c r="H186" t="s">
+        <v>779</v>
+      </c>
+      <c r="I186" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J186" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K186" s="7"/>
+      <c r="L186" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M186" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+      <c r="O186">
+        <v>1</v>
+      </c>
+      <c r="P186">
+        <v>0</v>
+      </c>
+      <c r="Q186">
+        <v>0</v>
+      </c>
+      <c r="R186">
+        <v>0</v>
+      </c>
+      <c r="S186">
+        <v>0</v>
+      </c>
+      <c r="T186" t="s">
+        <v>768</v>
+      </c>
+      <c r="U186" t="s">
+        <v>780</v>
+      </c>
+      <c r="V186">
+        <v>16</v>
+      </c>
+      <c r="W186">
+        <v>1624</v>
+      </c>
+      <c r="Z186" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="187" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A187" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="B187" s="7">
+        <v>184</v>
+      </c>
+      <c r="C187" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D187" s="5">
+        <v>43807</v>
+      </c>
+      <c r="E187" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G187">
+        <v>16</v>
+      </c>
+      <c r="H187" t="s">
+        <v>779</v>
+      </c>
+      <c r="I187" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J187" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K187" s="7"/>
+      <c r="L187" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M187" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="N187">
+        <v>1</v>
+      </c>
+      <c r="O187">
+        <v>1</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="Q187">
+        <v>0</v>
+      </c>
+      <c r="R187">
+        <v>0</v>
+      </c>
+      <c r="S187">
+        <v>0</v>
+      </c>
+      <c r="T187" t="s">
+        <v>768</v>
+      </c>
+      <c r="U187" t="s">
+        <v>780</v>
+      </c>
+      <c r="V187">
+        <v>16</v>
+      </c>
+      <c r="W187">
+        <v>1624</v>
+      </c>
+      <c r="Z187" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA187" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="188" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="B188" s="7">
+        <v>184</v>
+      </c>
+      <c r="C188" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="D188" s="5">
+        <v>43808</v>
+      </c>
+      <c r="E188" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="G188">
+        <v>16</v>
+      </c>
+      <c r="H188" t="s">
+        <v>779</v>
+      </c>
+      <c r="I188" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="J188" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="K188" s="7"/>
+      <c r="L188" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M188" s="9" t="s">
+        <v>778</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+      <c r="O188">
+        <v>1</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188">
+        <v>0</v>
+      </c>
+      <c r="R188">
+        <v>0</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+      <c r="T188" t="s">
+        <v>768</v>
+      </c>
+      <c r="U188" t="s">
+        <v>780</v>
+      </c>
+      <c r="V188">
+        <v>16</v>
+      </c>
+      <c r="W188">
+        <v>1624</v>
+      </c>
+      <c r="Z188" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>

<commit_message>
analyze Shir's data (bat 0184)
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2538" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="783">
   <si>
     <t>date</t>
   </si>
@@ -2315,60 +2315,18 @@
     <t>[1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16]</t>
   </si>
   <si>
-    <t>[59434546000 63082975000]</t>
-  </si>
-  <si>
     <t>6m</t>
   </si>
   <si>
     <t>b0184_d191125</t>
   </si>
   <si>
-    <t>[48776123000 51679735000]</t>
-  </si>
-  <si>
     <t>b0184_d191126</t>
   </si>
   <si>
-    <t>[43714183000 46954719000]</t>
-  </si>
-  <si>
-    <t>[60145523000 66587858000]</t>
-  </si>
-  <si>
     <t>120m</t>
   </si>
   <si>
-    <t>[42995335000 47390925000]</t>
-  </si>
-  <si>
-    <t>[48986037000 52928086000]</t>
-  </si>
-  <si>
-    <t>[33418817000 37379645000]</t>
-  </si>
-  <si>
-    <t>[47649050000 51464821000]</t>
-  </si>
-  <si>
-    <t>[43296150000 47443548000]</t>
-  </si>
-  <si>
-    <t>[42007182000 46353290000]</t>
-  </si>
-  <si>
-    <t>[53071661000 56916329000]</t>
-  </si>
-  <si>
-    <t>[45450019000 49507242000]</t>
-  </si>
-  <si>
-    <t>[58748740000 62174712000]</t>
-  </si>
-  <si>
-    <t>[42249148000 45446637000]</t>
-  </si>
-  <si>
     <t>[nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;nan;]</t>
   </si>
   <si>
@@ -2403,6 +2361,24 @@
   </si>
   <si>
     <t>the same as yesterday only that today with BeSpoon tag on the left side(near right hemisphere), instead of the battery(which is usually on the right).</t>
+  </si>
+  <si>
+    <t>{'TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD'}</t>
+  </si>
+  <si>
+    <t>[33421026000 33743453000; 33814579705 36571517679; 36638738000 37377320000]</t>
+  </si>
+  <si>
+    <t>[47651774000 48084419000; 48145514378 50853468195; 50916426000 51462587000]</t>
+  </si>
+  <si>
+    <t>[43297999000 43676890000; 43715406000 46215024000; 46248112000 47441443000]</t>
+  </si>
+  <si>
+    <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','TBD','CA1','CA1','CA1','TBD','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','CA1','CA1','CA1','CA1','TBD','CA1'}</t>
   </si>
 </sst>
 </file>
@@ -3157,10 +3133,10 @@
   <dimension ref="A1:AC188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B146" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C177" sqref="C177"/>
+      <selection pane="bottomRight" activeCell="K183" sqref="K183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16044,7 +16020,7 @@
         <v>16</v>
       </c>
       <c r="H175" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I175" s="1" t="s">
         <v>759</v>
@@ -16052,36 +16028,35 @@
       <c r="J175" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K175" s="7"/>
+      <c r="K175" t="s">
+        <v>777</v>
+      </c>
       <c r="L175" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M175" s="9" t="s">
+      <c r="N175">
+        <v>1</v>
+      </c>
+      <c r="O175">
+        <v>1</v>
+      </c>
+      <c r="P175">
+        <v>0</v>
+      </c>
+      <c r="Q175">
+        <v>0</v>
+      </c>
+      <c r="R175">
+        <v>0</v>
+      </c>
+      <c r="S175">
+        <v>0</v>
+      </c>
+      <c r="T175" t="s">
         <v>761</v>
       </c>
-      <c r="N175">
-        <v>1</v>
-      </c>
-      <c r="O175">
-        <v>1</v>
-      </c>
-      <c r="P175">
-        <v>0</v>
-      </c>
-      <c r="Q175">
-        <v>0</v>
-      </c>
-      <c r="R175">
-        <v>0</v>
-      </c>
-      <c r="S175">
-        <v>0</v>
-      </c>
-      <c r="T175" t="s">
-        <v>762</v>
-      </c>
       <c r="U175" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V175">
         <v>16</v>
@@ -16095,7 +16070,7 @@
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B176" s="7">
         <v>184</v>
@@ -16113,7 +16088,7 @@
         <v>16</v>
       </c>
       <c r="H176" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I176" s="1" t="s">
         <v>759</v>
@@ -16121,13 +16096,12 @@
       <c r="J176" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K176" s="7"/>
+      <c r="K176" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L176" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M176" s="9" t="s">
-        <v>764</v>
-      </c>
       <c r="N176">
         <v>1</v>
       </c>
@@ -16147,10 +16121,10 @@
         <v>0</v>
       </c>
       <c r="T176" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="U176" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V176">
         <v>16</v>
@@ -16164,7 +16138,7 @@
     </row>
     <row r="177" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="B177" s="7">
         <v>184</v>
@@ -16182,7 +16156,7 @@
         <v>16</v>
       </c>
       <c r="H177" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I177" s="1" t="s">
         <v>759</v>
@@ -16190,36 +16164,35 @@
       <c r="J177" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K177" s="7"/>
+      <c r="K177" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L177" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M177" s="9" t="s">
+      <c r="N177">
+        <v>1</v>
+      </c>
+      <c r="O177">
+        <v>1</v>
+      </c>
+      <c r="P177">
+        <v>0</v>
+      </c>
+      <c r="Q177">
+        <v>0</v>
+      </c>
+      <c r="R177">
+        <v>0</v>
+      </c>
+      <c r="S177">
+        <v>0</v>
+      </c>
+      <c r="T177" t="s">
+        <v>761</v>
+      </c>
+      <c r="U177" t="s">
         <v>766</v>
-      </c>
-      <c r="N177">
-        <v>1</v>
-      </c>
-      <c r="O177">
-        <v>1</v>
-      </c>
-      <c r="P177">
-        <v>0</v>
-      </c>
-      <c r="Q177">
-        <v>0</v>
-      </c>
-      <c r="R177">
-        <v>0</v>
-      </c>
-      <c r="S177">
-        <v>0</v>
-      </c>
-      <c r="T177" t="s">
-        <v>762</v>
-      </c>
-      <c r="U177" t="s">
-        <v>780</v>
       </c>
       <c r="V177">
         <v>16</v>
@@ -16231,7 +16204,7 @@
         <v>86</v>
       </c>
       <c r="AA177" t="s">
-        <v>781</v>
+        <v>767</v>
       </c>
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.25">
@@ -16254,7 +16227,7 @@
         <v>16</v>
       </c>
       <c r="H178" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I178" s="1" t="s">
         <v>759</v>
@@ -16262,13 +16235,12 @@
       <c r="J178" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K178" s="7"/>
+      <c r="K178" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L178" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M178" s="9" t="s">
-        <v>767</v>
-      </c>
       <c r="N178">
         <v>1</v>
       </c>
@@ -16288,10 +16260,10 @@
         <v>0</v>
       </c>
       <c r="T178" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U178" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V178">
         <v>16</v>
@@ -16303,7 +16275,7 @@
         <v>86</v>
       </c>
       <c r="AA178" t="s">
-        <v>782</v>
+        <v>768</v>
       </c>
     </row>
     <row r="179" spans="1:28" x14ac:dyDescent="0.25">
@@ -16326,7 +16298,7 @@
         <v>16</v>
       </c>
       <c r="H179" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I179" s="1" t="s">
         <v>759</v>
@@ -16334,13 +16306,12 @@
       <c r="J179" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K179" s="7"/>
+      <c r="K179" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L179" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M179" s="9" t="s">
-        <v>769</v>
-      </c>
       <c r="N179">
         <v>1</v>
       </c>
@@ -16360,10 +16331,10 @@
         <v>0</v>
       </c>
       <c r="T179" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U179" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V179">
         <v>16</v>
@@ -16375,7 +16346,7 @@
         <v>86</v>
       </c>
       <c r="AA179" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
     </row>
     <row r="180" spans="1:28" x14ac:dyDescent="0.25">
@@ -16398,7 +16369,7 @@
         <v>16</v>
       </c>
       <c r="H180" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I180" s="1" t="s">
         <v>759</v>
@@ -16406,13 +16377,12 @@
       <c r="J180" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K180" s="7"/>
+      <c r="K180" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L180" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M180" s="9" t="s">
-        <v>770</v>
-      </c>
       <c r="N180">
         <v>1</v>
       </c>
@@ -16432,10 +16402,10 @@
         <v>0</v>
       </c>
       <c r="T180" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U180" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V180">
         <v>16</v>
@@ -16447,10 +16417,10 @@
         <v>86</v>
       </c>
       <c r="AA180" t="s">
-        <v>783</v>
+        <v>769</v>
       </c>
       <c r="AB180" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
     </row>
     <row r="181" spans="1:28" x14ac:dyDescent="0.25">
@@ -16473,7 +16443,7 @@
         <v>16</v>
       </c>
       <c r="H181" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I181" s="1" t="s">
         <v>759</v>
@@ -16481,12 +16451,14 @@
       <c r="J181" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K181" s="7"/>
+      <c r="K181" s="7" t="s">
+        <v>781</v>
+      </c>
       <c r="L181" s="10" t="s">
         <v>498</v>
       </c>
       <c r="M181" s="9" t="s">
-        <v>771</v>
+        <v>778</v>
       </c>
       <c r="N181">
         <v>1</v>
@@ -16507,10 +16479,10 @@
         <v>0</v>
       </c>
       <c r="T181" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U181" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V181">
         <v>16</v>
@@ -16522,10 +16494,10 @@
         <v>86</v>
       </c>
       <c r="AA181" t="s">
-        <v>784</v>
+        <v>770</v>
       </c>
       <c r="AB181" t="s">
-        <v>788</v>
+        <v>774</v>
       </c>
     </row>
     <row r="182" spans="1:28" x14ac:dyDescent="0.25">
@@ -16548,7 +16520,7 @@
         <v>16</v>
       </c>
       <c r="H182" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I182" s="1" t="s">
         <v>759</v>
@@ -16556,12 +16528,14 @@
       <c r="J182" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K182" s="7"/>
+      <c r="K182" s="7" t="s">
+        <v>782</v>
+      </c>
       <c r="L182" s="10" t="s">
         <v>498</v>
       </c>
       <c r="M182" s="9" t="s">
-        <v>772</v>
+        <v>779</v>
       </c>
       <c r="N182">
         <v>1</v>
@@ -16582,10 +16556,10 @@
         <v>0</v>
       </c>
       <c r="T182" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U182" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V182">
         <v>16</v>
@@ -16597,7 +16571,7 @@
         <v>86</v>
       </c>
       <c r="AB182" t="s">
-        <v>787</v>
+        <v>773</v>
       </c>
     </row>
     <row r="183" spans="1:28" x14ac:dyDescent="0.25">
@@ -16620,7 +16594,7 @@
         <v>16</v>
       </c>
       <c r="H183" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I183" s="1" t="s">
         <v>759</v>
@@ -16628,12 +16602,14 @@
       <c r="J183" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K183" s="7"/>
+      <c r="K183" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L183" s="10" t="s">
         <v>498</v>
       </c>
       <c r="M183" s="9" t="s">
-        <v>773</v>
+        <v>780</v>
       </c>
       <c r="N183">
         <v>1</v>
@@ -16654,10 +16630,10 @@
         <v>0</v>
       </c>
       <c r="T183" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U183" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V183">
         <v>16</v>
@@ -16669,7 +16645,7 @@
         <v>86</v>
       </c>
       <c r="AB183" t="s">
-        <v>789</v>
+        <v>775</v>
       </c>
     </row>
     <row r="184" spans="1:28" x14ac:dyDescent="0.25">
@@ -16692,7 +16668,7 @@
         <v>16</v>
       </c>
       <c r="H184" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I184" s="1" t="s">
         <v>759</v>
@@ -16700,13 +16676,12 @@
       <c r="J184" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K184" s="7"/>
+      <c r="K184" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L184" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M184" s="9" t="s">
-        <v>774</v>
-      </c>
       <c r="N184">
         <v>1</v>
       </c>
@@ -16726,10 +16701,10 @@
         <v>0</v>
       </c>
       <c r="T184" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U184" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V184">
         <v>16</v>
@@ -16741,10 +16716,10 @@
         <v>86</v>
       </c>
       <c r="AA184" t="s">
-        <v>785</v>
+        <v>771</v>
       </c>
       <c r="AB184" t="s">
-        <v>790</v>
+        <v>776</v>
       </c>
     </row>
     <row r="185" spans="1:28" x14ac:dyDescent="0.25">
@@ -16767,7 +16742,7 @@
         <v>16</v>
       </c>
       <c r="H185" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I185" s="1" t="s">
         <v>759</v>
@@ -16775,13 +16750,12 @@
       <c r="J185" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K185" s="7"/>
+      <c r="K185" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L185" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M185" s="9" t="s">
-        <v>775</v>
-      </c>
       <c r="N185">
         <v>1</v>
       </c>
@@ -16801,10 +16775,10 @@
         <v>0</v>
       </c>
       <c r="T185" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U185" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V185">
         <v>16</v>
@@ -16836,7 +16810,7 @@
         <v>16</v>
       </c>
       <c r="H186" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I186" s="1" t="s">
         <v>759</v>
@@ -16844,13 +16818,12 @@
       <c r="J186" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K186" s="7"/>
+      <c r="K186" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L186" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M186" s="9" t="s">
-        <v>776</v>
-      </c>
       <c r="N186">
         <v>1</v>
       </c>
@@ -16870,10 +16843,10 @@
         <v>0</v>
       </c>
       <c r="T186" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U186" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V186">
         <v>16</v>
@@ -16905,7 +16878,7 @@
         <v>16</v>
       </c>
       <c r="H187" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I187" s="1" t="s">
         <v>759</v>
@@ -16913,13 +16886,12 @@
       <c r="J187" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K187" s="7"/>
+      <c r="K187" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L187" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M187" s="9" t="s">
-        <v>777</v>
-      </c>
       <c r="N187">
         <v>1</v>
       </c>
@@ -16939,10 +16911,10 @@
         <v>0</v>
       </c>
       <c r="T187" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U187" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V187">
         <v>16</v>
@@ -16954,7 +16926,7 @@
         <v>86</v>
       </c>
       <c r="AA187" t="s">
-        <v>786</v>
+        <v>772</v>
       </c>
     </row>
     <row r="188" spans="1:28" x14ac:dyDescent="0.25">
@@ -16977,7 +16949,7 @@
         <v>16</v>
       </c>
       <c r="H188" t="s">
-        <v>779</v>
+        <v>765</v>
       </c>
       <c r="I188" s="1" t="s">
         <v>759</v>
@@ -16985,13 +16957,12 @@
       <c r="J188" s="1" t="s">
         <v>760</v>
       </c>
-      <c r="K188" s="7"/>
+      <c r="K188" s="7" t="s">
+        <v>777</v>
+      </c>
       <c r="L188" s="10" t="s">
         <v>498</v>
       </c>
-      <c r="M188" s="9" t="s">
-        <v>778</v>
-      </c>
       <c r="N188">
         <v>1</v>
       </c>
@@ -17011,10 +16982,10 @@
         <v>0</v>
       </c>
       <c r="T188" t="s">
-        <v>768</v>
+        <v>764</v>
       </c>
       <c r="U188" t="s">
-        <v>780</v>
+        <v>766</v>
       </c>
       <c r="V188">
         <v>16</v>

</xml_diff>

<commit_message>
major update for decoding analysis
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="783">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="784">
   <si>
     <t>date</t>
   </si>
@@ -2379,6 +2379,9 @@
   </si>
   <si>
     <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','CA1','CA1','CA1','CA1','TBD','CA1'}</t>
+  </si>
+  <si>
+    <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','CA1','TBD','CA1','CA1','TBD','CA1'}</t>
   </si>
 </sst>
 </file>
@@ -3133,10 +3136,10 @@
   <dimension ref="A1:AC188"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B161" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K183" sqref="K183"/>
+      <selection pane="bottomRight" activeCell="A184" sqref="A184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3166,7 +3169,7 @@
     <col min="24" max="24" width="2.42578125" customWidth="1"/>
     <col min="25" max="25" width="3.7109375" customWidth="1"/>
     <col min="26" max="26" width="4.85546875" customWidth="1"/>
-    <col min="27" max="27" width="154.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="88.7109375" customWidth="1"/>
     <col min="28" max="28" width="107.5703125" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="78.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -16603,7 +16606,7 @@
         <v>760</v>
       </c>
       <c r="K183" s="7" t="s">
-        <v>777</v>
+        <v>783</v>
       </c>
       <c r="L183" s="10" t="s">
         <v>498</v>

</xml_diff>

<commit_message>
updates to analyze shir bat 184 for sequences
</commit_message>
<xml_diff>
--- a/inclusion_lists/exp_summary.xlsx
+++ b/inclusion_lists/exp_summary.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2541" uniqueCount="784">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2660" uniqueCount="808">
   <si>
     <t>date</t>
   </si>
@@ -2267,9 +2267,6 @@
     <t>{'TBD','TBD','TBD','CA3'}</t>
   </si>
   <si>
-    <t>b0184_d191127</t>
-  </si>
-  <si>
     <t>b0184_d191128</t>
   </si>
   <si>
@@ -2303,27 +2300,12 @@
     <t>Shir</t>
   </si>
   <si>
-    <t>[6 1]</t>
-  </si>
-  <si>
-    <t>b0184_d191124</t>
-  </si>
-  <si>
     <t>[1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1;1 1 1 1]</t>
   </si>
   <si>
     <t>[1 2 3 4 5 6 7 8 9 10 11 12 13 14 15 16]</t>
   </si>
   <si>
-    <t>6m</t>
-  </si>
-  <si>
-    <t>b0184_d191125</t>
-  </si>
-  <si>
-    <t>b0184_d191126</t>
-  </si>
-  <si>
     <t>120m</t>
   </si>
   <si>
@@ -2333,12 +2315,6 @@
     <t>SpikeLog-64</t>
   </si>
   <si>
-    <t>one very short dark session - 1 flight only.</t>
-  </si>
-  <si>
-    <t>way to far end doing medium height, way back very low (0.5 m above the ground), mostly direct flights, landed only one time on the floor.</t>
-  </si>
-  <si>
     <t>most flights are low, both way to and back at 0.5m above the ground or less.</t>
   </si>
   <si>
@@ -2363,25 +2339,121 @@
     <t>the same as yesterday only that today with BeSpoon tag on the left side(near right hemisphere), instead of the battery(which is usually on the right).</t>
   </si>
   <si>
-    <t>{'TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD','TBD'}</t>
-  </si>
-  <si>
     <t>[33421026000 33743453000; 33814579705 36571517679; 36638738000 37377320000]</t>
   </si>
   <si>
     <t>[47651774000 48084419000; 48145514378 50853468195; 50916426000 51462587000]</t>
   </si>
   <si>
-    <t>[43297999000 43676890000; 43715406000 46215024000; 46248112000 47441443000]</t>
-  </si>
-  <si>
-    <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','TBD','CA1','CA1','CA1','TBD','CA1'}</t>
-  </si>
-  <si>
     <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','CA1','CA1','CA1','CA1','TBD','CA1'}</t>
   </si>
   <si>
-    <t>{'CA1','TBD','TBD','TBD','TBD','TBD','CA1','TBD','TBD','TBD','CA1','TBD','CA1','CA1','TBD','CA1'}</t>
+    <t>[42996716000 43398344000;  43448478283 46758852405;  46833804000 47374483000]</t>
+  </si>
+  <si>
+    <t>[48990278000 49360176767; 49385702555 52410745642; 52453715000 52924663000]</t>
+  </si>
+  <si>
+    <t>[43297999000 43676890000; 43703190036 46198524689; 46248112000 47441443000]</t>
+  </si>
+  <si>
+    <t>[42008508000 42509030916; 42549382153 45847232000; 45891038000 46349301000]</t>
+  </si>
+  <si>
+    <t>[53072884000 53525554248; 53561649000 56039684731; 56073933000 56700724000]</t>
+  </si>
+  <si>
+    <t>[45451593000 45959709000; 46014682197 48249405865; 48306648000 49505503000]</t>
+  </si>
+  <si>
+    <t>b0184_d191210</t>
+  </si>
+  <si>
+    <t>b0184_d191211</t>
+  </si>
+  <si>
+    <t>b0184_d191212</t>
+  </si>
+  <si>
+    <t>b0184_d191215</t>
+  </si>
+  <si>
+    <t>b0184_d191216</t>
+  </si>
+  <si>
+    <t>b0184_d191217</t>
+  </si>
+  <si>
+    <t>b0184_d191220</t>
+  </si>
+  <si>
+    <t>b0184_d191222</t>
+  </si>
+  <si>
+    <t>b0184_d191224</t>
+  </si>
+  <si>
+    <t>b0184_d191225</t>
+  </si>
+  <si>
+    <t>b0184_d191226</t>
+  </si>
+  <si>
+    <t>b0184_d200101</t>
+  </si>
+  <si>
+    <t>b0184_d200102</t>
+  </si>
+  <si>
+    <t>the logger was restarted a few times during the run - the protector was hiting the SD card</t>
+  </si>
+  <si>
+    <t>winds in the beginning of the run. The MAHSOM fell in the the first 10 minutes of the behavior and Efrat had to hold it. The bat was a bit scared but still flew well.</t>
+  </si>
+  <si>
+    <t>[42250304000 42603202524; 42679783380 44921609000; 44987515000 45444983000]</t>
+  </si>
+  <si>
+    <t>[53267796000 53844871000; 53899448613 56206936743; 56261380000 57003580000]</t>
+  </si>
+  <si>
+    <t>[54472068000 55636937000; 55663181459 57765648372; 57812019000 58221774000]</t>
+  </si>
+  <si>
+    <t>[48806414000 49409970000; 49445590711 51784103472; 51846449000 52225157000]</t>
+  </si>
+  <si>
+    <t>[44592759000 45045998000; 45075851632 46992051329; 47063238000 47623872000]</t>
+  </si>
+  <si>
+    <t>[49925120000 50551000000; 50620905164 52988270184; 53054221000 54394434000]</t>
+  </si>
+  <si>
+    <t>[58751273000 59087557000; 59125261260 61614240000; 61553064299 62173276000]</t>
+  </si>
+  <si>
+    <t>[35936083000 36452649000; 36518390854 38668695143; 38731961000 39212575000]</t>
+  </si>
+  <si>
+    <t>[41969900000 42287386000; 42322454185 44507265110; 44582143000 45129013000]</t>
+  </si>
+  <si>
+    <t>[57783002000 58687385000; 58728865921 60602453000; 60627515000 60978019000]</t>
+  </si>
+  <si>
+    <t>[40889960000 41276030000; 41308462435 43418558820; 43474109000 43928114000]</t>
+  </si>
+  <si>
+    <t>[47714400000 48126668590; 48189894153 49640148066; 49682755000 50216473000]</t>
+  </si>
+  <si>
+    <t>[39927708000 40275994244; 40367561459 41924687825; 41976757000 42307975000]</t>
+  </si>
+  <si>
+    <t>[40328462000 40669666471; 40740890384 42966271431; 43055435000 43631985000]</t>
+  </si>
+  <si>
+    <t>[39954098000 40362586512; 40486117434 42625785856; 42710397336 43214325000]</t>
   </si>
 </sst>
 </file>
@@ -3133,13 +3205,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC188"/>
+  <dimension ref="A1:AC197"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B158" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B166" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A184" sqref="A184"/>
+      <selection pane="bottomRight" activeCell="E189" sqref="E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3148,14 +3220,15 @@
     <col min="2" max="2" width="4.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="7" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.140625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="7" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
-    <col min="8" max="8" width="26.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.42578125" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" customWidth="1"/>
-    <col min="11" max="11" width="25.5703125" customWidth="1"/>
-    <col min="12" max="12" width="2.7109375" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" style="9" customWidth="1"/>
+    <col min="8" max="8" width="19.140625" customWidth="1"/>
+    <col min="9" max="9" width="103.28515625" customWidth="1"/>
+    <col min="10" max="10" width="39.28515625" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.42578125" style="9" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" customWidth="1"/>
     <col min="15" max="15" width="2.42578125" customWidth="1"/>
     <col min="16" max="16" width="3" customWidth="1"/>
@@ -3163,7 +3236,7 @@
     <col min="18" max="18" width="6.42578125" customWidth="1"/>
     <col min="19" max="19" width="3.140625" customWidth="1"/>
     <col min="20" max="20" width="5.42578125" customWidth="1"/>
-    <col min="21" max="21" width="19.42578125" customWidth="1"/>
+    <col min="21" max="21" width="12.7109375" customWidth="1"/>
     <col min="22" max="22" width="3" customWidth="1"/>
     <col min="23" max="23" width="5.85546875" customWidth="1"/>
     <col min="24" max="24" width="2.42578125" customWidth="1"/>
@@ -16005,61 +16078,64 @@
     </row>
     <row r="175" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>758</v>
+        <v>745</v>
       </c>
       <c r="B175" s="7">
         <v>184</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D175" s="5">
-        <v>43793</v>
-      </c>
-      <c r="E175" s="1" t="s">
-        <v>757</v>
+        <v>43797</v>
+      </c>
+      <c r="E175" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G175">
         <v>16</v>
       </c>
       <c r="H175" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I175" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J175" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K175" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L175" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M175" s="9" t="s">
+        <v>772</v>
+      </c>
+      <c r="N175">
+        <v>1</v>
+      </c>
+      <c r="O175">
+        <v>1</v>
+      </c>
+      <c r="P175">
+        <v>0</v>
+      </c>
+      <c r="Q175">
+        <v>0</v>
+      </c>
+      <c r="R175">
+        <v>0</v>
+      </c>
+      <c r="S175">
+        <v>0</v>
+      </c>
+      <c r="T175" t="s">
+        <v>758</v>
+      </c>
+      <c r="U175" t="s">
         <v>760</v>
-      </c>
-      <c r="K175" t="s">
-        <v>777</v>
-      </c>
-      <c r="L175" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N175">
-        <v>1</v>
-      </c>
-      <c r="O175">
-        <v>1</v>
-      </c>
-      <c r="P175">
-        <v>0</v>
-      </c>
-      <c r="Q175">
-        <v>0</v>
-      </c>
-      <c r="R175">
-        <v>0</v>
-      </c>
-      <c r="S175">
-        <v>0</v>
-      </c>
-      <c r="T175" t="s">
-        <v>761</v>
-      </c>
-      <c r="U175" t="s">
-        <v>766</v>
       </c>
       <c r="V175">
         <v>16</v>
@@ -16070,64 +16146,70 @@
       <c r="Z175" t="s">
         <v>86</v>
       </c>
+      <c r="AA175" t="s">
+        <v>761</v>
+      </c>
     </row>
     <row r="176" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>762</v>
+        <v>746</v>
       </c>
       <c r="B176" s="7">
         <v>184</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D176" s="5">
-        <v>43794</v>
-      </c>
-      <c r="E176" s="1" t="s">
-        <v>757</v>
+        <v>43798</v>
+      </c>
+      <c r="E176" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G176">
         <v>16</v>
       </c>
       <c r="H176" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I176" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J176" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K176" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L176" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M176" s="9" t="s">
+        <v>773</v>
+      </c>
+      <c r="N176">
+        <v>1</v>
+      </c>
+      <c r="O176">
+        <v>1</v>
+      </c>
+      <c r="P176">
+        <v>0</v>
+      </c>
+      <c r="Q176">
+        <v>0</v>
+      </c>
+      <c r="R176">
+        <v>0</v>
+      </c>
+      <c r="S176">
+        <v>0</v>
+      </c>
+      <c r="T176" t="s">
+        <v>758</v>
+      </c>
+      <c r="U176" t="s">
         <v>760</v>
-      </c>
-      <c r="K176" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L176" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N176">
-        <v>1</v>
-      </c>
-      <c r="O176">
-        <v>1</v>
-      </c>
-      <c r="P176">
-        <v>0</v>
-      </c>
-      <c r="Q176">
-        <v>0</v>
-      </c>
-      <c r="R176">
-        <v>0</v>
-      </c>
-      <c r="S176">
-        <v>0</v>
-      </c>
-      <c r="T176" t="s">
-        <v>761</v>
-      </c>
-      <c r="U176" t="s">
-        <v>766</v>
       </c>
       <c r="V176">
         <v>16</v>
@@ -16138,64 +16220,73 @@
       <c r="Z176" t="s">
         <v>86</v>
       </c>
+      <c r="AA176" t="s">
+        <v>761</v>
+      </c>
+      <c r="AB176" t="s">
+        <v>765</v>
+      </c>
     </row>
     <row r="177" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>763</v>
+        <v>747</v>
       </c>
       <c r="B177" s="7">
         <v>184</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D177" s="5">
-        <v>43795</v>
-      </c>
-      <c r="E177" s="1" t="s">
-        <v>757</v>
+        <v>43799</v>
+      </c>
+      <c r="E177" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G177">
         <v>16</v>
       </c>
       <c r="H177" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I177" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J177" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K177" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L177" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M177" s="9" t="s">
+        <v>769</v>
+      </c>
+      <c r="N177">
+        <v>1</v>
+      </c>
+      <c r="O177">
+        <v>1</v>
+      </c>
+      <c r="P177">
+        <v>0</v>
+      </c>
+      <c r="Q177">
+        <v>0</v>
+      </c>
+      <c r="R177">
+        <v>0</v>
+      </c>
+      <c r="S177">
+        <v>0</v>
+      </c>
+      <c r="T177" t="s">
+        <v>758</v>
+      </c>
+      <c r="U177" t="s">
         <v>760</v>
-      </c>
-      <c r="K177" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L177" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N177">
-        <v>1</v>
-      </c>
-      <c r="O177">
-        <v>1</v>
-      </c>
-      <c r="P177">
-        <v>0</v>
-      </c>
-      <c r="Q177">
-        <v>0</v>
-      </c>
-      <c r="R177">
-        <v>0</v>
-      </c>
-      <c r="S177">
-        <v>0</v>
-      </c>
-      <c r="T177" t="s">
-        <v>761</v>
-      </c>
-      <c r="U177" t="s">
-        <v>766</v>
       </c>
       <c r="V177">
         <v>16</v>
@@ -16207,66 +16298,72 @@
         <v>86</v>
       </c>
       <c r="AA177" t="s">
-        <v>767</v>
+        <v>762</v>
+      </c>
+      <c r="AB177" t="s">
+        <v>766</v>
       </c>
     </row>
     <row r="178" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
       <c r="B178" s="7">
         <v>184</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D178" s="5">
-        <v>43796</v>
-      </c>
-      <c r="E178" s="1" t="s">
-        <v>757</v>
+        <v>43800</v>
+      </c>
+      <c r="E178" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G178">
         <v>16</v>
       </c>
       <c r="H178" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I178" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J178" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K178" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L178" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M178" s="9" t="s">
+        <v>770</v>
+      </c>
+      <c r="N178">
+        <v>1</v>
+      </c>
+      <c r="O178">
+        <v>1</v>
+      </c>
+      <c r="P178">
+        <v>0</v>
+      </c>
+      <c r="Q178">
+        <v>0</v>
+      </c>
+      <c r="R178">
+        <v>0</v>
+      </c>
+      <c r="S178">
+        <v>0</v>
+      </c>
+      <c r="T178" t="s">
+        <v>758</v>
+      </c>
+      <c r="U178" t="s">
         <v>760</v>
-      </c>
-      <c r="K178" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L178" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N178">
-        <v>1</v>
-      </c>
-      <c r="O178">
-        <v>1</v>
-      </c>
-      <c r="P178">
-        <v>0</v>
-      </c>
-      <c r="Q178">
-        <v>0</v>
-      </c>
-      <c r="R178">
-        <v>0</v>
-      </c>
-      <c r="S178">
-        <v>0</v>
-      </c>
-      <c r="T178" t="s">
-        <v>764</v>
-      </c>
-      <c r="U178" t="s">
-        <v>766</v>
       </c>
       <c r="V178">
         <v>16</v>
@@ -16277,67 +16374,70 @@
       <c r="Z178" t="s">
         <v>86</v>
       </c>
-      <c r="AA178" t="s">
-        <v>768</v>
+      <c r="AB178" t="s">
+        <v>765</v>
       </c>
     </row>
     <row r="179" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="B179" s="7">
         <v>184</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D179" s="5">
-        <v>43797</v>
-      </c>
-      <c r="E179" s="1" t="s">
-        <v>757</v>
+        <v>43801</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G179">
         <v>16</v>
       </c>
       <c r="H179" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I179" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J179" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K179" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L179" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M179" s="9" t="s">
+        <v>774</v>
+      </c>
+      <c r="N179">
+        <v>1</v>
+      </c>
+      <c r="O179">
+        <v>1</v>
+      </c>
+      <c r="P179">
+        <v>0</v>
+      </c>
+      <c r="Q179">
+        <v>0</v>
+      </c>
+      <c r="R179">
+        <v>0</v>
+      </c>
+      <c r="S179">
+        <v>0</v>
+      </c>
+      <c r="T179" t="s">
+        <v>758</v>
+      </c>
+      <c r="U179" t="s">
         <v>760</v>
-      </c>
-      <c r="K179" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L179" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N179">
-        <v>1</v>
-      </c>
-      <c r="O179">
-        <v>1</v>
-      </c>
-      <c r="P179">
-        <v>0</v>
-      </c>
-      <c r="Q179">
-        <v>0</v>
-      </c>
-      <c r="R179">
-        <v>0</v>
-      </c>
-      <c r="S179">
-        <v>0</v>
-      </c>
-      <c r="T179" t="s">
-        <v>764</v>
-      </c>
-      <c r="U179" t="s">
-        <v>766</v>
       </c>
       <c r="V179">
         <v>16</v>
@@ -16348,67 +16448,70 @@
       <c r="Z179" t="s">
         <v>86</v>
       </c>
-      <c r="AA179" t="s">
-        <v>769</v>
+      <c r="AB179" t="s">
+        <v>767</v>
       </c>
     </row>
     <row r="180" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
       <c r="B180" s="7">
         <v>184</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D180" s="5">
-        <v>43798</v>
-      </c>
-      <c r="E180" s="1" t="s">
-        <v>757</v>
+        <v>43802</v>
+      </c>
+      <c r="E180" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G180">
         <v>16</v>
       </c>
       <c r="H180" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I180" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J180" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K180" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L180" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M180" s="9" t="s">
+        <v>775</v>
+      </c>
+      <c r="N180">
+        <v>1</v>
+      </c>
+      <c r="O180">
+        <v>1</v>
+      </c>
+      <c r="P180">
+        <v>0</v>
+      </c>
+      <c r="Q180">
+        <v>0</v>
+      </c>
+      <c r="R180">
+        <v>0</v>
+      </c>
+      <c r="S180">
+        <v>0</v>
+      </c>
+      <c r="T180" t="s">
+        <v>758</v>
+      </c>
+      <c r="U180" t="s">
         <v>760</v>
-      </c>
-      <c r="K180" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L180" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N180">
-        <v>1</v>
-      </c>
-      <c r="O180">
-        <v>1</v>
-      </c>
-      <c r="P180">
-        <v>0</v>
-      </c>
-      <c r="Q180">
-        <v>0</v>
-      </c>
-      <c r="R180">
-        <v>0</v>
-      </c>
-      <c r="S180">
-        <v>0</v>
-      </c>
-      <c r="T180" t="s">
-        <v>764</v>
-      </c>
-      <c r="U180" t="s">
-        <v>766</v>
       </c>
       <c r="V180">
         <v>16</v>
@@ -16420,72 +16523,72 @@
         <v>86</v>
       </c>
       <c r="AA180" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
       <c r="AB180" t="s">
-        <v>773</v>
+        <v>768</v>
       </c>
     </row>
     <row r="181" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
       <c r="B181" s="7">
         <v>184</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D181" s="5">
-        <v>43799</v>
-      </c>
-      <c r="E181" s="1" t="s">
-        <v>757</v>
+        <v>43803</v>
+      </c>
+      <c r="E181" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G181">
         <v>16</v>
       </c>
       <c r="H181" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I181" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J181" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K181" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L181" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M181" s="9" t="s">
+        <v>776</v>
+      </c>
+      <c r="N181">
+        <v>1</v>
+      </c>
+      <c r="O181">
+        <v>1</v>
+      </c>
+      <c r="P181">
+        <v>0</v>
+      </c>
+      <c r="Q181">
+        <v>0</v>
+      </c>
+      <c r="R181">
+        <v>0</v>
+      </c>
+      <c r="S181">
+        <v>0</v>
+      </c>
+      <c r="T181" t="s">
+        <v>758</v>
+      </c>
+      <c r="U181" t="s">
         <v>760</v>
-      </c>
-      <c r="K181" s="7" t="s">
-        <v>781</v>
-      </c>
-      <c r="L181" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="M181" s="9" t="s">
-        <v>778</v>
-      </c>
-      <c r="N181">
-        <v>1</v>
-      </c>
-      <c r="O181">
-        <v>1</v>
-      </c>
-      <c r="P181">
-        <v>0</v>
-      </c>
-      <c r="Q181">
-        <v>0</v>
-      </c>
-      <c r="R181">
-        <v>0</v>
-      </c>
-      <c r="S181">
-        <v>0</v>
-      </c>
-      <c r="T181" t="s">
-        <v>764</v>
-      </c>
-      <c r="U181" t="s">
-        <v>766</v>
       </c>
       <c r="V181">
         <v>16</v>
@@ -16496,73 +16599,67 @@
       <c r="Z181" t="s">
         <v>86</v>
       </c>
-      <c r="AA181" t="s">
-        <v>770</v>
-      </c>
-      <c r="AB181" t="s">
-        <v>774</v>
-      </c>
     </row>
     <row r="182" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
       <c r="B182" s="7">
         <v>184</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D182" s="5">
-        <v>43800</v>
-      </c>
-      <c r="E182" s="1" t="s">
-        <v>757</v>
+        <v>43804</v>
+      </c>
+      <c r="E182" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G182">
         <v>16</v>
       </c>
       <c r="H182" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I182" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J182" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K182" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L182" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M182" s="9" t="s">
+        <v>777</v>
+      </c>
+      <c r="N182">
+        <v>1</v>
+      </c>
+      <c r="O182">
+        <v>1</v>
+      </c>
+      <c r="P182">
+        <v>0</v>
+      </c>
+      <c r="Q182">
+        <v>0</v>
+      </c>
+      <c r="R182">
+        <v>0</v>
+      </c>
+      <c r="S182">
+        <v>0</v>
+      </c>
+      <c r="T182" t="s">
+        <v>758</v>
+      </c>
+      <c r="U182" t="s">
         <v>760</v>
-      </c>
-      <c r="K182" s="7" t="s">
-        <v>782</v>
-      </c>
-      <c r="L182" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="M182" s="9" t="s">
-        <v>779</v>
-      </c>
-      <c r="N182">
-        <v>1</v>
-      </c>
-      <c r="O182">
-        <v>1</v>
-      </c>
-      <c r="P182">
-        <v>0</v>
-      </c>
-      <c r="Q182">
-        <v>0</v>
-      </c>
-      <c r="R182">
-        <v>0</v>
-      </c>
-      <c r="S182">
-        <v>0</v>
-      </c>
-      <c r="T182" t="s">
-        <v>764</v>
-      </c>
-      <c r="U182" t="s">
-        <v>766</v>
       </c>
       <c r="V182">
         <v>16</v>
@@ -16573,70 +16670,67 @@
       <c r="Z182" t="s">
         <v>86</v>
       </c>
-      <c r="AB182" t="s">
-        <v>773</v>
-      </c>
     </row>
     <row r="183" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
       <c r="B183" s="7">
         <v>184</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D183" s="5">
-        <v>43801</v>
-      </c>
-      <c r="E183" s="1" t="s">
-        <v>757</v>
+        <v>43807</v>
+      </c>
+      <c r="E183" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G183">
         <v>16</v>
       </c>
       <c r="H183" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I183" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J183" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K183" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L183" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M183" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="N183">
+        <v>1</v>
+      </c>
+      <c r="O183">
+        <v>1</v>
+      </c>
+      <c r="P183">
+        <v>0</v>
+      </c>
+      <c r="Q183">
+        <v>0</v>
+      </c>
+      <c r="R183">
+        <v>0</v>
+      </c>
+      <c r="S183">
+        <v>0</v>
+      </c>
+      <c r="T183" t="s">
+        <v>758</v>
+      </c>
+      <c r="U183" t="s">
         <v>760</v>
-      </c>
-      <c r="K183" s="7" t="s">
-        <v>783</v>
-      </c>
-      <c r="L183" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="M183" s="9" t="s">
-        <v>780</v>
-      </c>
-      <c r="N183">
-        <v>1</v>
-      </c>
-      <c r="O183">
-        <v>1</v>
-      </c>
-      <c r="P183">
-        <v>0</v>
-      </c>
-      <c r="Q183">
-        <v>0</v>
-      </c>
-      <c r="R183">
-        <v>0</v>
-      </c>
-      <c r="S183">
-        <v>0</v>
-      </c>
-      <c r="T183" t="s">
-        <v>764</v>
-      </c>
-      <c r="U183" t="s">
-        <v>766</v>
       </c>
       <c r="V183">
         <v>16</v>
@@ -16647,67 +16741,70 @@
       <c r="Z183" t="s">
         <v>86</v>
       </c>
-      <c r="AB183" t="s">
-        <v>775</v>
+      <c r="AA183" t="s">
+        <v>764</v>
       </c>
     </row>
     <row r="184" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
       <c r="B184" s="7">
         <v>184</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D184" s="5">
-        <v>43802</v>
-      </c>
-      <c r="E184" s="1" t="s">
-        <v>757</v>
+        <v>43808</v>
+      </c>
+      <c r="E184" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G184">
         <v>16</v>
       </c>
       <c r="H184" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I184" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J184" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K184" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L184" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M184" s="9" t="s">
+        <v>793</v>
+      </c>
+      <c r="N184">
+        <v>1</v>
+      </c>
+      <c r="O184">
+        <v>1</v>
+      </c>
+      <c r="P184">
+        <v>0</v>
+      </c>
+      <c r="Q184">
+        <v>0</v>
+      </c>
+      <c r="R184">
+        <v>0</v>
+      </c>
+      <c r="S184">
+        <v>0</v>
+      </c>
+      <c r="T184" t="s">
+        <v>758</v>
+      </c>
+      <c r="U184" t="s">
         <v>760</v>
-      </c>
-      <c r="K184" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L184" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N184">
-        <v>1</v>
-      </c>
-      <c r="O184">
-        <v>1</v>
-      </c>
-      <c r="P184">
-        <v>0</v>
-      </c>
-      <c r="Q184">
-        <v>0</v>
-      </c>
-      <c r="R184">
-        <v>0</v>
-      </c>
-      <c r="S184">
-        <v>0</v>
-      </c>
-      <c r="T184" t="s">
-        <v>764</v>
-      </c>
-      <c r="U184" t="s">
-        <v>766</v>
       </c>
       <c r="V184">
         <v>16</v>
@@ -16718,70 +16815,67 @@
       <c r="Z184" t="s">
         <v>86</v>
       </c>
-      <c r="AA184" t="s">
-        <v>771</v>
-      </c>
-      <c r="AB184" t="s">
-        <v>776</v>
-      </c>
     </row>
     <row r="185" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>752</v>
+        <v>778</v>
       </c>
       <c r="B185" s="7">
         <v>184</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D185" s="5">
-        <v>43803</v>
-      </c>
-      <c r="E185" s="1" t="s">
-        <v>757</v>
+        <v>43809</v>
+      </c>
+      <c r="E185" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G185">
         <v>16</v>
       </c>
       <c r="H185" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I185" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J185" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K185" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L185" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M185" s="9" t="s">
+        <v>794</v>
+      </c>
+      <c r="N185">
+        <v>1</v>
+      </c>
+      <c r="O185">
+        <v>1</v>
+      </c>
+      <c r="P185">
+        <v>0</v>
+      </c>
+      <c r="Q185">
+        <v>0</v>
+      </c>
+      <c r="R185">
+        <v>0</v>
+      </c>
+      <c r="S185">
+        <v>0</v>
+      </c>
+      <c r="T185" t="s">
+        <v>758</v>
+      </c>
+      <c r="U185" t="s">
         <v>760</v>
-      </c>
-      <c r="K185" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L185" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N185">
-        <v>1</v>
-      </c>
-      <c r="O185">
-        <v>1</v>
-      </c>
-      <c r="P185">
-        <v>0</v>
-      </c>
-      <c r="Q185">
-        <v>0</v>
-      </c>
-      <c r="R185">
-        <v>0</v>
-      </c>
-      <c r="S185">
-        <v>0</v>
-      </c>
-      <c r="T185" t="s">
-        <v>764</v>
-      </c>
-      <c r="U185" t="s">
-        <v>766</v>
       </c>
       <c r="V185">
         <v>16</v>
@@ -16795,61 +16889,64 @@
     </row>
     <row r="186" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>753</v>
+        <v>779</v>
       </c>
       <c r="B186" s="7">
         <v>184</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D186" s="5">
-        <v>43804</v>
-      </c>
-      <c r="E186" s="1" t="s">
-        <v>757</v>
+        <v>43810</v>
+      </c>
+      <c r="E186" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G186">
         <v>16</v>
       </c>
       <c r="H186" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I186" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J186" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K186" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L186" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M186" s="9" t="s">
+        <v>795</v>
+      </c>
+      <c r="N186">
+        <v>1</v>
+      </c>
+      <c r="O186">
+        <v>1</v>
+      </c>
+      <c r="P186">
+        <v>0</v>
+      </c>
+      <c r="Q186">
+        <v>0</v>
+      </c>
+      <c r="R186">
+        <v>0</v>
+      </c>
+      <c r="S186">
+        <v>0</v>
+      </c>
+      <c r="T186" t="s">
+        <v>758</v>
+      </c>
+      <c r="U186" t="s">
         <v>760</v>
-      </c>
-      <c r="K186" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L186" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N186">
-        <v>1</v>
-      </c>
-      <c r="O186">
-        <v>1</v>
-      </c>
-      <c r="P186">
-        <v>0</v>
-      </c>
-      <c r="Q186">
-        <v>0</v>
-      </c>
-      <c r="R186">
-        <v>0</v>
-      </c>
-      <c r="S186">
-        <v>0</v>
-      </c>
-      <c r="T186" t="s">
-        <v>764</v>
-      </c>
-      <c r="U186" t="s">
-        <v>766</v>
       </c>
       <c r="V186">
         <v>16</v>
@@ -16863,61 +16960,64 @@
     </row>
     <row r="187" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>754</v>
+        <v>780</v>
       </c>
       <c r="B187" s="7">
         <v>184</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D187" s="5">
-        <v>43807</v>
-      </c>
-      <c r="E187" s="1" t="s">
-        <v>757</v>
+        <v>43811</v>
+      </c>
+      <c r="E187" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G187">
         <v>16</v>
       </c>
       <c r="H187" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I187" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J187" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K187" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L187" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M187" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="N187">
+        <v>1</v>
+      </c>
+      <c r="O187">
+        <v>1</v>
+      </c>
+      <c r="P187">
+        <v>0</v>
+      </c>
+      <c r="Q187">
+        <v>0</v>
+      </c>
+      <c r="R187">
+        <v>0</v>
+      </c>
+      <c r="S187">
+        <v>0</v>
+      </c>
+      <c r="T187" t="s">
+        <v>758</v>
+      </c>
+      <c r="U187" t="s">
         <v>760</v>
-      </c>
-      <c r="K187" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L187" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N187">
-        <v>1</v>
-      </c>
-      <c r="O187">
-        <v>1</v>
-      </c>
-      <c r="P187">
-        <v>0</v>
-      </c>
-      <c r="Q187">
-        <v>0</v>
-      </c>
-      <c r="R187">
-        <v>0</v>
-      </c>
-      <c r="S187">
-        <v>0</v>
-      </c>
-      <c r="T187" t="s">
-        <v>764</v>
-      </c>
-      <c r="U187" t="s">
-        <v>766</v>
       </c>
       <c r="V187">
         <v>16</v>
@@ -16928,67 +17028,67 @@
       <c r="Z187" t="s">
         <v>86</v>
       </c>
-      <c r="AA187" t="s">
-        <v>772</v>
-      </c>
     </row>
     <row r="188" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>755</v>
+        <v>781</v>
       </c>
       <c r="B188" s="7">
         <v>184</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="D188" s="5">
-        <v>43808</v>
-      </c>
-      <c r="E188" s="1" t="s">
-        <v>757</v>
+        <v>43814</v>
+      </c>
+      <c r="E188" s="7" t="s">
+        <v>86</v>
       </c>
       <c r="G188">
         <v>16</v>
       </c>
       <c r="H188" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
       <c r="I188" s="1" t="s">
-        <v>759</v>
+        <v>756</v>
       </c>
       <c r="J188" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K188" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L188" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M188" s="9" t="s">
+        <v>797</v>
+      </c>
+      <c r="N188">
+        <v>1</v>
+      </c>
+      <c r="O188">
+        <v>1</v>
+      </c>
+      <c r="P188">
+        <v>0</v>
+      </c>
+      <c r="Q188">
+        <v>0</v>
+      </c>
+      <c r="R188">
+        <v>0</v>
+      </c>
+      <c r="S188">
+        <v>0</v>
+      </c>
+      <c r="T188" t="s">
+        <v>758</v>
+      </c>
+      <c r="U188" t="s">
         <v>760</v>
-      </c>
-      <c r="K188" s="7" t="s">
-        <v>777</v>
-      </c>
-      <c r="L188" s="10" t="s">
-        <v>498</v>
-      </c>
-      <c r="N188">
-        <v>1</v>
-      </c>
-      <c r="O188">
-        <v>1</v>
-      </c>
-      <c r="P188">
-        <v>0</v>
-      </c>
-      <c r="Q188">
-        <v>0</v>
-      </c>
-      <c r="R188">
-        <v>0</v>
-      </c>
-      <c r="S188">
-        <v>0</v>
-      </c>
-      <c r="T188" t="s">
-        <v>764</v>
-      </c>
-      <c r="U188" t="s">
-        <v>766</v>
       </c>
       <c r="V188">
         <v>16</v>
@@ -16997,6 +17097,651 @@
         <v>1624</v>
       </c>
       <c r="Z188" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="189" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A189" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B189" s="7">
+        <v>184</v>
+      </c>
+      <c r="C189" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D189" s="5">
+        <v>43815</v>
+      </c>
+      <c r="E189" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G189">
+        <v>16</v>
+      </c>
+      <c r="H189" t="s">
+        <v>759</v>
+      </c>
+      <c r="I189" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J189" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K189" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L189" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M189" s="9" t="s">
+        <v>798</v>
+      </c>
+      <c r="N189">
+        <v>1</v>
+      </c>
+      <c r="O189">
+        <v>1</v>
+      </c>
+      <c r="P189">
+        <v>0</v>
+      </c>
+      <c r="Q189">
+        <v>0</v>
+      </c>
+      <c r="R189">
+        <v>0</v>
+      </c>
+      <c r="S189">
+        <v>0</v>
+      </c>
+      <c r="T189" t="s">
+        <v>758</v>
+      </c>
+      <c r="U189" t="s">
+        <v>760</v>
+      </c>
+      <c r="V189">
+        <v>16</v>
+      </c>
+      <c r="W189">
+        <v>1624</v>
+      </c>
+      <c r="Z189" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="190" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B190" s="7">
+        <v>184</v>
+      </c>
+      <c r="C190" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D190" s="5">
+        <v>43816</v>
+      </c>
+      <c r="E190" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G190">
+        <v>16</v>
+      </c>
+      <c r="H190" t="s">
+        <v>759</v>
+      </c>
+      <c r="I190" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J190" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K190" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L190" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M190" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="N190">
+        <v>1</v>
+      </c>
+      <c r="O190">
+        <v>1</v>
+      </c>
+      <c r="P190">
+        <v>0</v>
+      </c>
+      <c r="Q190">
+        <v>0</v>
+      </c>
+      <c r="R190">
+        <v>0</v>
+      </c>
+      <c r="S190">
+        <v>0</v>
+      </c>
+      <c r="T190" t="s">
+        <v>758</v>
+      </c>
+      <c r="U190" t="s">
+        <v>760</v>
+      </c>
+      <c r="V190">
+        <v>16</v>
+      </c>
+      <c r="W190">
+        <v>1624</v>
+      </c>
+      <c r="Z190" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="191" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A191" s="1" t="s">
+        <v>784</v>
+      </c>
+      <c r="B191" s="7">
+        <v>184</v>
+      </c>
+      <c r="C191" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D191" s="5">
+        <v>43819</v>
+      </c>
+      <c r="E191" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G191">
+        <v>16</v>
+      </c>
+      <c r="H191" t="s">
+        <v>759</v>
+      </c>
+      <c r="I191" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J191" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K191" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L191" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M191" s="9" t="s">
+        <v>801</v>
+      </c>
+      <c r="N191">
+        <v>1</v>
+      </c>
+      <c r="O191">
+        <v>1</v>
+      </c>
+      <c r="P191">
+        <v>0</v>
+      </c>
+      <c r="Q191">
+        <v>0</v>
+      </c>
+      <c r="R191">
+        <v>0</v>
+      </c>
+      <c r="S191">
+        <v>0</v>
+      </c>
+      <c r="T191" t="s">
+        <v>758</v>
+      </c>
+      <c r="U191" t="s">
+        <v>760</v>
+      </c>
+      <c r="V191">
+        <v>16</v>
+      </c>
+      <c r="W191">
+        <v>1624</v>
+      </c>
+      <c r="Z191" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="192" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B192" s="7">
+        <v>184</v>
+      </c>
+      <c r="C192" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D192" s="5">
+        <v>43821</v>
+      </c>
+      <c r="E192" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G192">
+        <v>16</v>
+      </c>
+      <c r="H192" t="s">
+        <v>759</v>
+      </c>
+      <c r="I192" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J192" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K192" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L192" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M192" s="9" t="s">
+        <v>802</v>
+      </c>
+      <c r="N192">
+        <v>1</v>
+      </c>
+      <c r="O192">
+        <v>1</v>
+      </c>
+      <c r="P192">
+        <v>0</v>
+      </c>
+      <c r="Q192">
+        <v>0</v>
+      </c>
+      <c r="R192">
+        <v>0</v>
+      </c>
+      <c r="S192">
+        <v>0</v>
+      </c>
+      <c r="T192" t="s">
+        <v>758</v>
+      </c>
+      <c r="U192" t="s">
+        <v>760</v>
+      </c>
+      <c r="V192">
+        <v>16</v>
+      </c>
+      <c r="W192">
+        <v>1624</v>
+      </c>
+      <c r="Z192" t="s">
+        <v>86</v>
+      </c>
+      <c r="AB192" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="193" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A193" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="B193" s="7">
+        <v>184</v>
+      </c>
+      <c r="C193" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D193" s="5">
+        <v>43823</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G193">
+        <v>16</v>
+      </c>
+      <c r="H193" t="s">
+        <v>759</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J193" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K193" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L193" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M193" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="N193">
+        <v>1</v>
+      </c>
+      <c r="O193">
+        <v>1</v>
+      </c>
+      <c r="P193">
+        <v>0</v>
+      </c>
+      <c r="Q193">
+        <v>0</v>
+      </c>
+      <c r="R193">
+        <v>0</v>
+      </c>
+      <c r="S193">
+        <v>0</v>
+      </c>
+      <c r="T193" t="s">
+        <v>758</v>
+      </c>
+      <c r="U193" t="s">
+        <v>760</v>
+      </c>
+      <c r="V193">
+        <v>16</v>
+      </c>
+      <c r="W193">
+        <v>1624</v>
+      </c>
+      <c r="Z193" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA193" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="194" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>787</v>
+      </c>
+      <c r="B194" s="7">
+        <v>184</v>
+      </c>
+      <c r="C194" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D194" s="5">
+        <v>43824</v>
+      </c>
+      <c r="E194" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G194">
+        <v>16</v>
+      </c>
+      <c r="H194" t="s">
+        <v>759</v>
+      </c>
+      <c r="I194" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J194" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K194" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L194" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M194" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="N194">
+        <v>1</v>
+      </c>
+      <c r="O194">
+        <v>1</v>
+      </c>
+      <c r="P194">
+        <v>0</v>
+      </c>
+      <c r="Q194">
+        <v>0</v>
+      </c>
+      <c r="R194">
+        <v>0</v>
+      </c>
+      <c r="S194">
+        <v>0</v>
+      </c>
+      <c r="T194" t="s">
+        <v>758</v>
+      </c>
+      <c r="U194" t="s">
+        <v>760</v>
+      </c>
+      <c r="V194">
+        <v>16</v>
+      </c>
+      <c r="W194">
+        <v>1624</v>
+      </c>
+      <c r="Z194" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="195" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A195" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B195" s="7">
+        <v>184</v>
+      </c>
+      <c r="C195" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D195" s="5">
+        <v>43825</v>
+      </c>
+      <c r="E195" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G195">
+        <v>16</v>
+      </c>
+      <c r="H195" t="s">
+        <v>759</v>
+      </c>
+      <c r="I195" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J195" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K195" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L195" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M195" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="N195">
+        <v>1</v>
+      </c>
+      <c r="O195">
+        <v>1</v>
+      </c>
+      <c r="P195">
+        <v>0</v>
+      </c>
+      <c r="Q195">
+        <v>0</v>
+      </c>
+      <c r="R195">
+        <v>0</v>
+      </c>
+      <c r="S195">
+        <v>0</v>
+      </c>
+      <c r="T195" t="s">
+        <v>758</v>
+      </c>
+      <c r="U195" t="s">
+        <v>760</v>
+      </c>
+      <c r="V195">
+        <v>16</v>
+      </c>
+      <c r="W195">
+        <v>1624</v>
+      </c>
+      <c r="Z195" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="196" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>789</v>
+      </c>
+      <c r="B196" s="7">
+        <v>184</v>
+      </c>
+      <c r="C196" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D196" s="5">
+        <v>43831</v>
+      </c>
+      <c r="E196" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G196">
+        <v>16</v>
+      </c>
+      <c r="H196" t="s">
+        <v>759</v>
+      </c>
+      <c r="I196" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J196" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K196" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L196" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M196" s="9" t="s">
+        <v>806</v>
+      </c>
+      <c r="N196">
+        <v>1</v>
+      </c>
+      <c r="O196">
+        <v>1</v>
+      </c>
+      <c r="P196">
+        <v>0</v>
+      </c>
+      <c r="Q196">
+        <v>0</v>
+      </c>
+      <c r="R196">
+        <v>0</v>
+      </c>
+      <c r="S196">
+        <v>0</v>
+      </c>
+      <c r="T196" t="s">
+        <v>758</v>
+      </c>
+      <c r="U196" t="s">
+        <v>760</v>
+      </c>
+      <c r="V196">
+        <v>16</v>
+      </c>
+      <c r="W196">
+        <v>1624</v>
+      </c>
+      <c r="Z196" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="197" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A197" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B197" s="7">
+        <v>184</v>
+      </c>
+      <c r="C197" s="1" t="s">
+        <v>755</v>
+      </c>
+      <c r="D197" s="5">
+        <v>43832</v>
+      </c>
+      <c r="E197" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G197">
+        <v>16</v>
+      </c>
+      <c r="H197" t="s">
+        <v>759</v>
+      </c>
+      <c r="I197" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="J197" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="K197" s="7" t="s">
+        <v>771</v>
+      </c>
+      <c r="L197" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="M197" s="9" t="s">
+        <v>807</v>
+      </c>
+      <c r="N197">
+        <v>1</v>
+      </c>
+      <c r="O197">
+        <v>1</v>
+      </c>
+      <c r="P197">
+        <v>0</v>
+      </c>
+      <c r="Q197">
+        <v>0</v>
+      </c>
+      <c r="R197">
+        <v>0</v>
+      </c>
+      <c r="S197">
+        <v>0</v>
+      </c>
+      <c r="T197" t="s">
+        <v>758</v>
+      </c>
+      <c r="U197" t="s">
+        <v>760</v>
+      </c>
+      <c r="V197">
+        <v>16</v>
+      </c>
+      <c r="W197">
+        <v>1624</v>
+      </c>
+      <c r="Z197" t="s">
         <v>86</v>
       </c>
     </row>

</xml_diff>